<commit_message>
Updates to cardiovascular validation and documentation,
</commit_message>
<xml_diff>
--- a/test/validation/SystemValidationData.xlsx
+++ b/test/validation/SystemValidationData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21126"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\physiology\engine\test\validation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\PulseHemorrhage\engine\test\validation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{DC26569B-DEA8-4A67-AB33-1FA0F3DF31DA}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85F90A60-35B2-406E-8762-17CCD7A2E67F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="1320" windowWidth="11850" windowHeight="6645" tabRatio="724" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="720" yWindow="1320" windowWidth="11856" windowHeight="6648" tabRatio="724" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blood Chemistry" sheetId="4" r:id="rId1"/>
@@ -23,12 +23,12 @@
     <sheet name="Respiratory" sheetId="2" r:id="rId8"/>
     <sheet name="Tissue" sheetId="34" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3602" uniqueCount="1008">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3626" uniqueCount="1016">
   <si>
     <t>Output</t>
   </si>
@@ -3175,6 +3175,30 @@
   </si>
   <si>
     <t>ChymeAbsorptionRate</t>
+  </si>
+  <si>
+    <t>LeftArmVasculature-InFlow</t>
+  </si>
+  <si>
+    <t>common femoral artery estimate</t>
+  </si>
+  <si>
+    <t>holland1998lower</t>
+  </si>
+  <si>
+    <t>LeftLegVasculature-InFlow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RightLegVasculature-InFlow </t>
+  </si>
+  <si>
+    <t>gault1966patterns</t>
+  </si>
+  <si>
+    <t>brachial artery average</t>
+  </si>
+  <si>
+    <t>RightArmVasculature-InFlow</t>
   </si>
 </sst>
 </file>
@@ -4865,20 +4889,20 @@
       <selection pane="topRight" activeCell="L54" sqref="L54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="12"/>
   <cols>
-    <col min="1" max="1" width="40.140625" style="73" customWidth="1"/>
-    <col min="2" max="2" width="7.140625" style="74" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" style="74" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" style="74" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="33.85546875" style="74" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.5703125" style="74" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.109375" style="73" customWidth="1"/>
+    <col min="2" max="2" width="7.109375" style="74" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.88671875" style="74" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.88671875" style="74" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.88671875" style="74" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.5546875" style="74" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="48" style="74" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="49.28515625" style="73" customWidth="1"/>
+    <col min="8" max="8" width="49.33203125" style="73" customWidth="1"/>
     <col min="9" max="9" width="36" style="73" customWidth="1"/>
-    <col min="10" max="11" width="28.85546875" style="74" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="30.42578125" style="74" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="73"/>
+    <col min="10" max="11" width="28.88671875" style="74" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="30.44140625" style="74" customWidth="1"/>
+    <col min="13" max="16384" width="9.109375" style="73"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="26.25" customHeight="1">
@@ -5503,7 +5527,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="56.25">
+    <row r="22" spans="1:12" ht="40.799999999999997">
       <c r="A22" s="142" t="s">
         <v>921</v>
       </c>
@@ -5533,7 +5557,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="22.5">
+    <row r="23" spans="1:12" ht="20.399999999999999">
       <c r="A23" s="21" t="s">
         <v>922</v>
       </c>
@@ -6381,7 +6405,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="50" spans="1:12" ht="15">
+    <row r="50" spans="1:12" ht="14.4">
       <c r="A50" s="104" t="s">
         <v>452</v>
       </c>
@@ -6475,7 +6499,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="53" spans="1:12" ht="12.75">
+    <row r="53" spans="1:12" ht="13.2">
       <c r="A53" s="104" t="s">
         <v>455</v>
       </c>
@@ -7789,28 +7813,28 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:L105"/>
+  <dimension ref="A1:L109"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" topLeftCell="G1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="L27" sqref="L27"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="4" topLeftCell="F1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="K80" sqref="K80"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="12"/>
   <cols>
-    <col min="1" max="1" width="38.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="36" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" style="36" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.5703125" style="36" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.109375" style="36" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.88671875" style="36" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.5546875" style="36" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="29" style="37" customWidth="1"/>
-    <col min="6" max="6" width="21.7109375" style="37" customWidth="1"/>
-    <col min="7" max="7" width="32.7109375" style="36" customWidth="1"/>
-    <col min="8" max="8" width="36.28515625" style="140" customWidth="1"/>
-    <col min="9" max="9" width="29.5703125" style="9" customWidth="1"/>
-    <col min="10" max="10" width="27.5703125" style="36" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="28.85546875" style="74" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="30.42578125" style="74" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="9"/>
+    <col min="6" max="6" width="21.6640625" style="37" customWidth="1"/>
+    <col min="7" max="7" width="32.6640625" style="36" customWidth="1"/>
+    <col min="8" max="8" width="36.33203125" style="140" customWidth="1"/>
+    <col min="9" max="9" width="29.5546875" style="9" customWidth="1"/>
+    <col min="10" max="10" width="27.5546875" style="36" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="28.88671875" style="74" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="30.44140625" style="74" customWidth="1"/>
+    <col min="13" max="16384" width="9.109375" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -7963,7 +7987,7 @@
         <v>1006</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="60">
+    <row r="6" spans="1:12" ht="48">
       <c r="A6" s="23" t="s">
         <v>176</v>
       </c>
@@ -8296,7 +8320,7 @@
       <c r="K17" s="80"/>
       <c r="L17" s="80"/>
     </row>
-    <row r="18" spans="1:12" s="73" customFormat="1" ht="60">
+    <row r="18" spans="1:12" s="73" customFormat="1" ht="48">
       <c r="A18" s="89" t="s">
         <v>175</v>
       </c>
@@ -8328,16 +8352,16 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="19" spans="1:12" s="73" customFormat="1" ht="24">
+    <row r="19" spans="1:12" s="73" customFormat="1">
       <c r="A19" s="89" t="s">
         <v>208</v>
       </c>
       <c r="B19" s="82" t="str">
-        <f>B93</f>
+        <f>B97</f>
         <v>mL/s</v>
       </c>
       <c r="C19" s="82" t="str">
-        <f t="shared" ref="C19:E19" si="0">C93</f>
+        <f t="shared" ref="C19:E19" si="0">C97</f>
         <v>Mean</v>
       </c>
       <c r="D19" s="82">
@@ -8545,7 +8569,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="27" spans="1:12" s="73" customFormat="1" ht="24">
+    <row r="27" spans="1:12" s="73" customFormat="1">
       <c r="A27" s="153" t="s">
         <v>938</v>
       </c>
@@ -9117,7 +9141,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="46" spans="1:12" ht="36">
+    <row r="46" spans="1:12" ht="24">
       <c r="A46" s="89" t="s">
         <v>646</v>
       </c>
@@ -9148,32 +9172,32 @@
       </c>
     </row>
     <row r="47" spans="1:12">
-      <c r="A47" s="89" t="s">
-        <v>697</v>
-      </c>
-      <c r="B47" s="83" t="s">
-        <v>7</v>
-      </c>
-      <c r="C47" s="85" t="s">
-        <v>172</v>
-      </c>
-      <c r="D47" s="48" t="s">
-        <v>169</v>
-      </c>
-      <c r="E47" s="83" t="s">
-        <v>156</v>
-      </c>
-      <c r="F47" s="83"/>
-      <c r="G47" s="7"/>
-      <c r="H47" s="135"/>
+      <c r="A47" s="153" t="s">
+        <v>1008</v>
+      </c>
+      <c r="B47" s="175" t="s">
+        <v>553</v>
+      </c>
+      <c r="C47" s="186" t="s">
+        <v>171</v>
+      </c>
+      <c r="D47" s="48">
+        <v>1.23</v>
+      </c>
+      <c r="E47" s="175" t="s">
+        <v>1013</v>
+      </c>
+      <c r="F47" s="175"/>
+      <c r="G47" s="176"/>
+      <c r="H47" s="179" t="s">
+        <v>1014</v>
+      </c>
       <c r="I47" s="109"/>
-      <c r="J47" s="80" t="s">
+      <c r="J47" s="191" t="s">
         <v>418</v>
       </c>
-      <c r="K47" s="80"/>
-      <c r="L47" s="191" t="s">
-        <v>1005</v>
-      </c>
+      <c r="K47" s="191"/>
+      <c r="L47" s="191"/>
     </row>
     <row r="48" spans="1:12">
       <c r="A48" s="89" t="s">
@@ -9183,10 +9207,10 @@
         <v>7</v>
       </c>
       <c r="C48" s="85" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D48" s="48" t="s">
-        <v>546</v>
+        <v>169</v>
       </c>
       <c r="E48" s="83" t="s">
         <v>156</v>
@@ -9205,19 +9229,19 @@
     </row>
     <row r="49" spans="1:12">
       <c r="A49" s="89" t="s">
-        <v>696</v>
+        <v>697</v>
       </c>
       <c r="B49" s="83" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C49" s="85" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D49" s="48" t="s">
-        <v>537</v>
+        <v>546</v>
       </c>
       <c r="E49" s="83" t="s">
-        <v>902</v>
+        <v>156</v>
       </c>
       <c r="F49" s="83"/>
       <c r="G49" s="7"/>
@@ -9231,7 +9255,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="50" spans="1:12" ht="48">
+    <row r="50" spans="1:12">
       <c r="A50" s="89" t="s">
         <v>696</v>
       </c>
@@ -9239,21 +9263,17 @@
         <v>5</v>
       </c>
       <c r="C50" s="85" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D50" s="48" t="s">
-        <v>170</v>
+        <v>537</v>
       </c>
       <c r="E50" s="83" t="s">
-        <v>547</v>
-      </c>
-      <c r="F50" s="83" t="s">
-        <v>548</v>
-      </c>
+        <v>902</v>
+      </c>
+      <c r="F50" s="83"/>
       <c r="G50" s="7"/>
-      <c r="H50" s="135" t="s">
-        <v>549</v>
-      </c>
+      <c r="H50" s="135"/>
       <c r="I50" s="109"/>
       <c r="J50" s="80" t="s">
         <v>418</v>
@@ -9263,25 +9283,29 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="51" spans="1:12">
+    <row r="51" spans="1:12" ht="48">
       <c r="A51" s="89" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="B51" s="83" t="s">
-        <v>553</v>
-      </c>
-      <c r="C51" s="82" t="s">
-        <v>171</v>
-      </c>
-      <c r="D51" s="48">
-        <v>94.7</v>
+        <v>5</v>
+      </c>
+      <c r="C51" s="85" t="s">
+        <v>173</v>
+      </c>
+      <c r="D51" s="48" t="s">
+        <v>170</v>
       </c>
       <c r="E51" s="83" t="s">
-        <v>98</v>
-      </c>
-      <c r="F51" s="83"/>
+        <v>547</v>
+      </c>
+      <c r="F51" s="83" t="s">
+        <v>548</v>
+      </c>
       <c r="G51" s="7"/>
-      <c r="H51" s="135"/>
+      <c r="H51" s="135" t="s">
+        <v>549</v>
+      </c>
       <c r="I51" s="109"/>
       <c r="J51" s="80" t="s">
         <v>418</v>
@@ -9291,27 +9315,25 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="52" spans="1:12" ht="24">
+    <row r="52" spans="1:12">
       <c r="A52" s="89" t="s">
-        <v>647</v>
+        <v>698</v>
       </c>
       <c r="B52" s="83" t="s">
-        <v>7</v>
+        <v>553</v>
       </c>
       <c r="C52" s="82" t="s">
         <v>171</v>
       </c>
-      <c r="D52" s="178" t="s">
-        <v>790</v>
-      </c>
-      <c r="E52" s="177" t="s">
-        <v>791</v>
-      </c>
-      <c r="F52" s="175"/>
-      <c r="G52" s="176"/>
-      <c r="H52" s="179" t="s">
-        <v>570</v>
-      </c>
+      <c r="D52" s="48">
+        <v>94.7</v>
+      </c>
+      <c r="E52" s="83" t="s">
+        <v>98</v>
+      </c>
+      <c r="F52" s="83"/>
+      <c r="G52" s="7"/>
+      <c r="H52" s="135"/>
       <c r="I52" s="109"/>
       <c r="J52" s="80" t="s">
         <v>418</v>
@@ -9323,24 +9345,24 @@
     </row>
     <row r="53" spans="1:12" ht="24">
       <c r="A53" s="89" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="B53" s="83" t="s">
-        <v>553</v>
+        <v>7</v>
       </c>
       <c r="C53" s="82" t="s">
         <v>171</v>
       </c>
-      <c r="D53" s="34">
-        <v>9.3000000000000007</v>
-      </c>
-      <c r="E53" s="83" t="s">
-        <v>98</v>
-      </c>
-      <c r="F53" s="83"/>
-      <c r="G53" s="7"/>
-      <c r="H53" s="135" t="s">
-        <v>578</v>
+      <c r="D53" s="178" t="s">
+        <v>790</v>
+      </c>
+      <c r="E53" s="177" t="s">
+        <v>791</v>
+      </c>
+      <c r="F53" s="175"/>
+      <c r="G53" s="176"/>
+      <c r="H53" s="179" t="s">
+        <v>570</v>
       </c>
       <c r="I53" s="109"/>
       <c r="J53" s="80" t="s">
@@ -9351,26 +9373,26 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="54" spans="1:12" ht="36">
+    <row r="54" spans="1:12" ht="24">
       <c r="A54" s="89" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="B54" s="83" t="s">
-        <v>7</v>
+        <v>553</v>
       </c>
       <c r="C54" s="82" t="s">
         <v>171</v>
       </c>
-      <c r="D54" s="48">
-        <v>85.7</v>
+      <c r="D54" s="34">
+        <v>9.3000000000000007</v>
       </c>
       <c r="E54" s="83" t="s">
         <v>98</v>
       </c>
       <c r="F54" s="83"/>
       <c r="G54" s="7"/>
-      <c r="H54" s="110" t="s">
-        <v>567</v>
+      <c r="H54" s="135" t="s">
+        <v>578</v>
       </c>
       <c r="I54" s="109"/>
       <c r="J54" s="80" t="s">
@@ -9383,7 +9405,7 @@
     </row>
     <row r="55" spans="1:12" ht="24">
       <c r="A55" s="89" t="s">
-        <v>670</v>
+        <v>649</v>
       </c>
       <c r="B55" s="83" t="s">
         <v>7</v>
@@ -9392,7 +9414,7 @@
         <v>171</v>
       </c>
       <c r="D55" s="48">
-        <v>96.5</v>
+        <v>85.7</v>
       </c>
       <c r="E55" s="83" t="s">
         <v>98</v>
@@ -9400,7 +9422,7 @@
       <c r="F55" s="83"/>
       <c r="G55" s="7"/>
       <c r="H55" s="110" t="s">
-        <v>575</v>
+        <v>567</v>
       </c>
       <c r="I55" s="109"/>
       <c r="J55" s="80" t="s">
@@ -9412,36 +9434,36 @@
       </c>
     </row>
     <row r="56" spans="1:12">
-      <c r="A56" s="89" t="s">
-        <v>671</v>
-      </c>
-      <c r="B56" s="83" t="s">
+      <c r="A56" s="153" t="s">
+        <v>1011</v>
+      </c>
+      <c r="B56" s="175" t="s">
         <v>553</v>
       </c>
-      <c r="C56" s="82" t="s">
+      <c r="C56" s="186" t="s">
         <v>171</v>
       </c>
       <c r="D56" s="48">
-        <v>45</v>
-      </c>
-      <c r="E56" s="83" t="s">
-        <v>98</v>
-      </c>
-      <c r="F56" s="83"/>
-      <c r="G56" s="7"/>
-      <c r="H56" s="135"/>
+        <v>2.5299999999999998</v>
+      </c>
+      <c r="E56" s="175" t="s">
+        <v>1010</v>
+      </c>
+      <c r="F56" s="175"/>
+      <c r="G56" s="176"/>
+      <c r="H56" s="179" t="s">
+        <v>1009</v>
+      </c>
       <c r="I56" s="109"/>
-      <c r="J56" s="80" t="s">
+      <c r="J56" s="191" t="s">
         <v>418</v>
       </c>
-      <c r="K56" s="80"/>
-      <c r="L56" s="191" t="s">
-        <v>1005</v>
-      </c>
-    </row>
-    <row r="57" spans="1:12" ht="24">
+      <c r="K56" s="191"/>
+      <c r="L56" s="191"/>
+    </row>
+    <row r="57" spans="1:12">
       <c r="A57" s="89" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="B57" s="83" t="s">
         <v>7</v>
@@ -9450,7 +9472,7 @@
         <v>171</v>
       </c>
       <c r="D57" s="48">
-        <v>65.3</v>
+        <v>96.5</v>
       </c>
       <c r="E57" s="83" t="s">
         <v>98</v>
@@ -9471,7 +9493,7 @@
     </row>
     <row r="58" spans="1:12">
       <c r="A58" s="89" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="B58" s="83" t="s">
         <v>553</v>
@@ -9497,9 +9519,9 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="59" spans="1:12" ht="24">
+    <row r="59" spans="1:12">
       <c r="A59" s="89" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="B59" s="83" t="s">
         <v>7</v>
@@ -9508,7 +9530,7 @@
         <v>171</v>
       </c>
       <c r="D59" s="48">
-        <v>192.9</v>
+        <v>65.3</v>
       </c>
       <c r="E59" s="83" t="s">
         <v>98</v>
@@ -9529,7 +9551,7 @@
     </row>
     <row r="60" spans="1:12">
       <c r="A60" s="89" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="B60" s="83" t="s">
         <v>553</v>
@@ -9555,9 +9577,9 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="61" spans="1:12" ht="24">
+    <row r="61" spans="1:12">
       <c r="A61" s="89" t="s">
-        <v>650</v>
+        <v>674</v>
       </c>
       <c r="B61" s="83" t="s">
         <v>7</v>
@@ -9565,16 +9587,16 @@
       <c r="C61" s="82" t="s">
         <v>171</v>
       </c>
-      <c r="D61" s="34">
-        <v>601.5</v>
+      <c r="D61" s="48">
+        <v>192.9</v>
       </c>
       <c r="E61" s="83" t="s">
         <v>98</v>
       </c>
       <c r="F61" s="83"/>
-      <c r="G61" s="83"/>
+      <c r="G61" s="7"/>
       <c r="H61" s="110" t="s">
-        <v>572</v>
+        <v>575</v>
       </c>
       <c r="I61" s="109"/>
       <c r="J61" s="80" t="s">
@@ -9587,7 +9609,7 @@
     </row>
     <row r="62" spans="1:12">
       <c r="A62" s="89" t="s">
-        <v>651</v>
+        <v>675</v>
       </c>
       <c r="B62" s="83" t="s">
         <v>553</v>
@@ -9595,19 +9617,15 @@
       <c r="C62" s="82" t="s">
         <v>171</v>
       </c>
-      <c r="D62" s="34">
-        <v>24.2</v>
+      <c r="D62" s="48">
+        <v>45</v>
       </c>
       <c r="E62" s="83" t="s">
-        <v>96</v>
-      </c>
-      <c r="F62" s="83" t="s">
-        <v>226</v>
-      </c>
-      <c r="G62" s="83"/>
-      <c r="H62" s="135" t="s">
-        <v>577</v>
-      </c>
+        <v>98</v>
+      </c>
+      <c r="F62" s="83"/>
+      <c r="G62" s="7"/>
+      <c r="H62" s="135"/>
       <c r="I62" s="109"/>
       <c r="J62" s="80" t="s">
         <v>418</v>
@@ -9619,7 +9637,7 @@
     </row>
     <row r="63" spans="1:12">
       <c r="A63" s="89" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="B63" s="83" t="s">
         <v>7</v>
@@ -9627,8 +9645,8 @@
       <c r="C63" s="82" t="s">
         <v>171</v>
       </c>
-      <c r="D63" s="48">
-        <v>794.4</v>
+      <c r="D63" s="34">
+        <v>601.5</v>
       </c>
       <c r="E63" s="83" t="s">
         <v>98</v>
@@ -9636,7 +9654,7 @@
       <c r="F63" s="83"/>
       <c r="G63" s="83"/>
       <c r="H63" s="110" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="I63" s="109"/>
       <c r="J63" s="80" t="s">
@@ -9649,7 +9667,7 @@
     </row>
     <row r="64" spans="1:12">
       <c r="A64" s="89" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="B64" s="83" t="s">
         <v>553</v>
@@ -9657,15 +9675,19 @@
       <c r="C64" s="82" t="s">
         <v>171</v>
       </c>
-      <c r="D64" s="48">
-        <v>16.100000000000001</v>
+      <c r="D64" s="34">
+        <v>24.2</v>
       </c>
       <c r="E64" s="83" t="s">
-        <v>98</v>
-      </c>
-      <c r="F64" s="83"/>
+        <v>96</v>
+      </c>
+      <c r="F64" s="83" t="s">
+        <v>226</v>
+      </c>
       <c r="G64" s="83"/>
-      <c r="H64" s="135"/>
+      <c r="H64" s="135" t="s">
+        <v>577</v>
+      </c>
       <c r="I64" s="109"/>
       <c r="J64" s="80" t="s">
         <v>418</v>
@@ -9677,7 +9699,7 @@
     </row>
     <row r="65" spans="1:12">
       <c r="A65" s="89" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="B65" s="83" t="s">
         <v>7</v>
@@ -9686,15 +9708,15 @@
         <v>171</v>
       </c>
       <c r="D65" s="48">
-        <v>39.700000000000003</v>
+        <v>794.4</v>
       </c>
       <c r="E65" s="83" t="s">
         <v>98</v>
       </c>
       <c r="F65" s="83"/>
-      <c r="G65" s="45"/>
+      <c r="G65" s="83"/>
       <c r="H65" s="110" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="I65" s="109"/>
       <c r="J65" s="80" t="s">
@@ -9707,7 +9729,7 @@
     </row>
     <row r="66" spans="1:12">
       <c r="A66" s="89" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="B66" s="83" t="s">
         <v>553</v>
@@ -9716,13 +9738,13 @@
         <v>171</v>
       </c>
       <c r="D66" s="48">
-        <v>3.8</v>
+        <v>16.100000000000001</v>
       </c>
       <c r="E66" s="83" t="s">
         <v>98</v>
       </c>
       <c r="F66" s="83"/>
-      <c r="G66" s="45"/>
+      <c r="G66" s="83"/>
       <c r="H66" s="135"/>
       <c r="I66" s="109"/>
       <c r="J66" s="80" t="s">
@@ -9733,9 +9755,9 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="67" spans="1:12" ht="24">
+    <row r="67" spans="1:12">
       <c r="A67" s="89" t="s">
-        <v>676</v>
+        <v>654</v>
       </c>
       <c r="B67" s="83" t="s">
         <v>7</v>
@@ -9744,15 +9766,15 @@
         <v>171</v>
       </c>
       <c r="D67" s="48">
-        <v>192.9</v>
+        <v>39.700000000000003</v>
       </c>
       <c r="E67" s="83" t="s">
         <v>98</v>
       </c>
       <c r="F67" s="83"/>
-      <c r="G67" s="7"/>
+      <c r="G67" s="45"/>
       <c r="H67" s="110" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="I67" s="109"/>
       <c r="J67" s="80" t="s">
@@ -9765,7 +9787,7 @@
     </row>
     <row r="68" spans="1:12">
       <c r="A68" s="89" t="s">
-        <v>677</v>
+        <v>655</v>
       </c>
       <c r="B68" s="83" t="s">
         <v>553</v>
@@ -9774,13 +9796,13 @@
         <v>171</v>
       </c>
       <c r="D68" s="48">
-        <v>94.7</v>
+        <v>3.8</v>
       </c>
       <c r="E68" s="83" t="s">
         <v>98</v>
       </c>
       <c r="F68" s="83"/>
-      <c r="G68" s="7"/>
+      <c r="G68" s="45"/>
       <c r="H68" s="135"/>
       <c r="I68" s="109"/>
       <c r="J68" s="80" t="s">
@@ -9793,27 +9815,27 @@
     </row>
     <row r="69" spans="1:12">
       <c r="A69" s="89" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="B69" s="83" t="s">
-        <v>5</v>
-      </c>
-      <c r="C69" s="85" t="s">
-        <v>172</v>
-      </c>
-      <c r="D69" s="48" t="s">
-        <v>537</v>
-      </c>
-      <c r="E69" s="84" t="s">
-        <v>821</v>
-      </c>
-      <c r="F69" s="83" t="s">
-        <v>539</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="C69" s="82" t="s">
+        <v>171</v>
+      </c>
+      <c r="D69" s="48">
+        <v>192.9</v>
+      </c>
+      <c r="E69" s="83" t="s">
+        <v>98</v>
+      </c>
+      <c r="F69" s="83"/>
       <c r="G69" s="7"/>
-      <c r="H69" s="135"/>
+      <c r="H69" s="110" t="s">
+        <v>575</v>
+      </c>
       <c r="I69" s="109"/>
-      <c r="J69" s="191" t="s">
+      <c r="J69" s="80" t="s">
         <v>418</v>
       </c>
       <c r="K69" s="80"/>
@@ -9823,27 +9845,25 @@
     </row>
     <row r="70" spans="1:12">
       <c r="A70" s="89" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="B70" s="83" t="s">
-        <v>5</v>
-      </c>
-      <c r="C70" s="85" t="s">
-        <v>173</v>
-      </c>
-      <c r="D70" s="48" t="s">
-        <v>174</v>
-      </c>
-      <c r="E70" s="84" t="s">
-        <v>821</v>
-      </c>
-      <c r="F70" s="83" t="s">
-        <v>539</v>
-      </c>
+        <v>553</v>
+      </c>
+      <c r="C70" s="82" t="s">
+        <v>171</v>
+      </c>
+      <c r="D70" s="48">
+        <v>94.7</v>
+      </c>
+      <c r="E70" s="83" t="s">
+        <v>98</v>
+      </c>
+      <c r="F70" s="83"/>
       <c r="G70" s="7"/>
       <c r="H70" s="135"/>
       <c r="I70" s="109"/>
-      <c r="J70" s="191" t="s">
+      <c r="J70" s="80" t="s">
         <v>418</v>
       </c>
       <c r="K70" s="80"/>
@@ -9851,29 +9871,29 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="71" spans="1:12" ht="24">
+    <row r="71" spans="1:12">
       <c r="A71" s="89" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="B71" s="83" t="s">
-        <v>7</v>
-      </c>
-      <c r="C71" s="82" t="s">
-        <v>171</v>
-      </c>
-      <c r="D71" s="48">
-        <v>130.5</v>
-      </c>
-      <c r="E71" s="83" t="s">
-        <v>98</v>
-      </c>
-      <c r="F71" s="83"/>
+        <v>5</v>
+      </c>
+      <c r="C71" s="85" t="s">
+        <v>172</v>
+      </c>
+      <c r="D71" s="48" t="s">
+        <v>537</v>
+      </c>
+      <c r="E71" s="84" t="s">
+        <v>821</v>
+      </c>
+      <c r="F71" s="83" t="s">
+        <v>539</v>
+      </c>
       <c r="G71" s="7"/>
-      <c r="H71" s="110" t="s">
-        <v>575</v>
-      </c>
+      <c r="H71" s="135"/>
       <c r="I71" s="109"/>
-      <c r="J71" s="80" t="s">
+      <c r="J71" s="191" t="s">
         <v>418</v>
       </c>
       <c r="K71" s="80"/>
@@ -9883,25 +9903,27 @@
     </row>
     <row r="72" spans="1:12">
       <c r="A72" s="89" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="B72" s="83" t="s">
-        <v>553</v>
-      </c>
-      <c r="C72" s="82" t="s">
-        <v>171</v>
-      </c>
-      <c r="D72" s="48">
-        <v>94.7</v>
-      </c>
-      <c r="E72" s="83" t="s">
-        <v>98</v>
-      </c>
-      <c r="F72" s="83"/>
+        <v>5</v>
+      </c>
+      <c r="C72" s="85" t="s">
+        <v>173</v>
+      </c>
+      <c r="D72" s="48" t="s">
+        <v>174</v>
+      </c>
+      <c r="E72" s="84" t="s">
+        <v>821</v>
+      </c>
+      <c r="F72" s="83" t="s">
+        <v>539</v>
+      </c>
       <c r="G72" s="7"/>
       <c r="H72" s="135"/>
       <c r="I72" s="109"/>
-      <c r="J72" s="80" t="s">
+      <c r="J72" s="191" t="s">
         <v>418</v>
       </c>
       <c r="K72" s="80"/>
@@ -9911,29 +9933,27 @@
     </row>
     <row r="73" spans="1:12">
       <c r="A73" s="89" t="s">
-        <v>681</v>
-      </c>
-      <c r="B73" s="154" t="s">
-        <v>5</v>
-      </c>
-      <c r="C73" s="156" t="s">
+        <v>679</v>
+      </c>
+      <c r="B73" s="83" t="s">
+        <v>7</v>
+      </c>
+      <c r="C73" s="82" t="s">
         <v>171</v>
       </c>
-      <c r="D73" s="48" t="s">
-        <v>537</v>
-      </c>
-      <c r="E73" s="154" t="s">
-        <v>821</v>
-      </c>
-      <c r="F73" s="154" t="s">
-        <v>539</v>
-      </c>
+      <c r="D73" s="48">
+        <v>130.5</v>
+      </c>
+      <c r="E73" s="83" t="s">
+        <v>98</v>
+      </c>
+      <c r="F73" s="83"/>
       <c r="G73" s="7"/>
-      <c r="H73" s="135" t="s">
-        <v>788</v>
+      <c r="H73" s="110" t="s">
+        <v>575</v>
       </c>
       <c r="I73" s="109"/>
-      <c r="J73" s="191" t="s">
+      <c r="J73" s="80" t="s">
         <v>418</v>
       </c>
       <c r="K73" s="80"/>
@@ -9941,27 +9961,25 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="74" spans="1:12" ht="24">
+    <row r="74" spans="1:12">
       <c r="A74" s="89" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="B74" s="83" t="s">
-        <v>7</v>
+        <v>553</v>
       </c>
       <c r="C74" s="82" t="s">
         <v>171</v>
       </c>
       <c r="D74" s="48">
-        <v>385.8</v>
+        <v>94.7</v>
       </c>
       <c r="E74" s="83" t="s">
         <v>98</v>
       </c>
       <c r="F74" s="83"/>
       <c r="G74" s="7"/>
-      <c r="H74" s="110" t="s">
-        <v>575</v>
-      </c>
+      <c r="H74" s="135"/>
       <c r="I74" s="109"/>
       <c r="J74" s="80" t="s">
         <v>418</v>
@@ -9973,25 +9991,29 @@
     </row>
     <row r="75" spans="1:12">
       <c r="A75" s="89" t="s">
-        <v>683</v>
-      </c>
-      <c r="B75" s="83" t="s">
-        <v>553</v>
-      </c>
-      <c r="C75" s="82" t="s">
+        <v>681</v>
+      </c>
+      <c r="B75" s="154" t="s">
+        <v>5</v>
+      </c>
+      <c r="C75" s="156" t="s">
         <v>171</v>
       </c>
-      <c r="D75" s="48">
-        <v>94.7</v>
-      </c>
-      <c r="E75" s="83" t="s">
-        <v>98</v>
-      </c>
-      <c r="F75" s="83"/>
+      <c r="D75" s="48" t="s">
+        <v>537</v>
+      </c>
+      <c r="E75" s="154" t="s">
+        <v>821</v>
+      </c>
+      <c r="F75" s="154" t="s">
+        <v>539</v>
+      </c>
       <c r="G75" s="7"/>
-      <c r="H75" s="135"/>
+      <c r="H75" s="135" t="s">
+        <v>788</v>
+      </c>
       <c r="I75" s="109"/>
-      <c r="J75" s="80" t="s">
+      <c r="J75" s="191" t="s">
         <v>418</v>
       </c>
       <c r="K75" s="80"/>
@@ -9999,31 +10021,29 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="76" spans="1:12" ht="36">
+    <row r="76" spans="1:12">
       <c r="A76" s="89" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="B76" s="83" t="s">
-        <v>5</v>
-      </c>
-      <c r="C76" s="85" t="s">
+        <v>7</v>
+      </c>
+      <c r="C76" s="82" t="s">
         <v>171</v>
       </c>
-      <c r="D76" s="48" t="s">
-        <v>537</v>
+      <c r="D76" s="48">
+        <v>385.8</v>
       </c>
       <c r="E76" s="83" t="s">
-        <v>821</v>
-      </c>
-      <c r="F76" s="83" t="s">
-        <v>539</v>
-      </c>
+        <v>98</v>
+      </c>
+      <c r="F76" s="83"/>
       <c r="G76" s="7"/>
-      <c r="H76" s="135" t="s">
-        <v>789</v>
+      <c r="H76" s="110" t="s">
+        <v>575</v>
       </c>
       <c r="I76" s="109"/>
-      <c r="J76" s="191" t="s">
+      <c r="J76" s="80" t="s">
         <v>418</v>
       </c>
       <c r="K76" s="80"/>
@@ -10031,27 +10051,25 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="77" spans="1:12" ht="36">
+    <row r="77" spans="1:12">
       <c r="A77" s="89" t="s">
-        <v>656</v>
+        <v>683</v>
       </c>
       <c r="B77" s="83" t="s">
-        <v>7</v>
+        <v>553</v>
       </c>
       <c r="C77" s="82" t="s">
         <v>171</v>
       </c>
       <c r="D77" s="48">
-        <v>56.7</v>
+        <v>94.7</v>
       </c>
       <c r="E77" s="83" t="s">
         <v>98</v>
       </c>
       <c r="F77" s="83"/>
       <c r="G77" s="7"/>
-      <c r="H77" s="110" t="s">
-        <v>567</v>
-      </c>
+      <c r="H77" s="135"/>
       <c r="I77" s="109"/>
       <c r="J77" s="80" t="s">
         <v>418</v>
@@ -10061,29 +10079,31 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="78" spans="1:12" ht="60">
+    <row r="78" spans="1:12" ht="36">
       <c r="A78" s="89" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="B78" s="83" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C78" s="85" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D78" s="48" t="s">
-        <v>550</v>
+        <v>537</v>
       </c>
       <c r="E78" s="83" t="s">
-        <v>903</v>
-      </c>
-      <c r="F78" s="83"/>
+        <v>821</v>
+      </c>
+      <c r="F78" s="83" t="s">
+        <v>539</v>
+      </c>
       <c r="G78" s="7"/>
-      <c r="H78" s="110" t="s">
-        <v>569</v>
+      <c r="H78" s="135" t="s">
+        <v>789</v>
       </c>
       <c r="I78" s="109"/>
-      <c r="J78" s="80" t="s">
+      <c r="J78" s="191" t="s">
         <v>418</v>
       </c>
       <c r="K78" s="80"/>
@@ -10093,23 +10113,25 @@
     </row>
     <row r="79" spans="1:12" ht="24">
       <c r="A79" s="89" t="s">
-        <v>685</v>
+        <v>656</v>
       </c>
       <c r="B79" s="83" t="s">
         <v>7</v>
       </c>
-      <c r="C79" s="85" t="s">
-        <v>173</v>
-      </c>
-      <c r="D79" s="48" t="s">
-        <v>551</v>
+      <c r="C79" s="82" t="s">
+        <v>171</v>
+      </c>
+      <c r="D79" s="48">
+        <v>56.7</v>
       </c>
       <c r="E79" s="83" t="s">
-        <v>903</v>
+        <v>98</v>
       </c>
       <c r="F79" s="83"/>
       <c r="G79" s="7"/>
-      <c r="H79" s="135"/>
+      <c r="H79" s="110" t="s">
+        <v>567</v>
+      </c>
       <c r="I79" s="109"/>
       <c r="J79" s="80" t="s">
         <v>418</v>
@@ -10119,55 +10141,55 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="80" spans="1:12" ht="36">
-      <c r="A80" s="89" t="s">
-        <v>686</v>
-      </c>
-      <c r="B80" s="83" t="s">
-        <v>5</v>
-      </c>
-      <c r="C80" s="85" t="s">
+    <row r="80" spans="1:12">
+      <c r="A80" s="153" t="s">
+        <v>1015</v>
+      </c>
+      <c r="B80" s="175" t="s">
+        <v>553</v>
+      </c>
+      <c r="C80" s="186" t="s">
+        <v>171</v>
+      </c>
+      <c r="D80" s="48">
+        <v>1.23</v>
+      </c>
+      <c r="E80" s="175" t="s">
+        <v>1013</v>
+      </c>
+      <c r="F80" s="175"/>
+      <c r="G80" s="176"/>
+      <c r="H80" s="179" t="s">
+        <v>1014</v>
+      </c>
+      <c r="I80" s="109"/>
+      <c r="J80" s="191" t="s">
+        <v>418</v>
+      </c>
+      <c r="K80" s="191"/>
+      <c r="L80" s="191"/>
+    </row>
+    <row r="81" spans="1:12" ht="48">
+      <c r="A81" s="89" t="s">
+        <v>685</v>
+      </c>
+      <c r="B81" s="83" t="s">
+        <v>7</v>
+      </c>
+      <c r="C81" s="85" t="s">
         <v>172</v>
       </c>
-      <c r="D80" s="48" t="s">
-        <v>542</v>
-      </c>
-      <c r="E80" s="83" t="s">
-        <v>902</v>
-      </c>
-      <c r="F80" s="83"/>
-      <c r="G80" s="7"/>
-      <c r="H80" s="135" t="s">
-        <v>543</v>
-      </c>
-      <c r="I80" s="109"/>
-      <c r="J80" s="80" t="s">
-        <v>418</v>
-      </c>
-      <c r="K80" s="80"/>
-      <c r="L80" s="191" t="s">
-        <v>1005</v>
-      </c>
-    </row>
-    <row r="81" spans="1:12">
-      <c r="A81" s="89" t="s">
-        <v>686</v>
-      </c>
-      <c r="B81" s="83" t="s">
-        <v>5</v>
-      </c>
-      <c r="C81" s="85" t="s">
-        <v>173</v>
-      </c>
       <c r="D81" s="48" t="s">
-        <v>174</v>
+        <v>550</v>
       </c>
       <c r="E81" s="83" t="s">
-        <v>902</v>
+        <v>903</v>
       </c>
       <c r="F81" s="83"/>
       <c r="G81" s="7"/>
-      <c r="H81" s="135"/>
+      <c r="H81" s="110" t="s">
+        <v>569</v>
+      </c>
       <c r="I81" s="109"/>
       <c r="J81" s="80" t="s">
         <v>418</v>
@@ -10177,21 +10199,21 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="82" spans="1:12">
+    <row r="82" spans="1:12" ht="24">
       <c r="A82" s="89" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
       <c r="B82" s="83" t="s">
-        <v>553</v>
-      </c>
-      <c r="C82" s="82" t="s">
-        <v>171</v>
-      </c>
-      <c r="D82" s="48">
-        <v>94.7</v>
+        <v>7</v>
+      </c>
+      <c r="C82" s="85" t="s">
+        <v>173</v>
+      </c>
+      <c r="D82" s="48" t="s">
+        <v>551</v>
       </c>
       <c r="E82" s="83" t="s">
-        <v>98</v>
+        <v>903</v>
       </c>
       <c r="F82" s="83"/>
       <c r="G82" s="7"/>
@@ -10205,26 +10227,26 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="83" spans="1:12" ht="24">
+    <row r="83" spans="1:12" ht="36">
       <c r="A83" s="89" t="s">
-        <v>657</v>
+        <v>686</v>
       </c>
       <c r="B83" s="83" t="s">
-        <v>7</v>
-      </c>
-      <c r="C83" s="82" t="s">
-        <v>171</v>
-      </c>
-      <c r="D83" s="183" t="s">
-        <v>790</v>
-      </c>
-      <c r="E83" s="182" t="s">
-        <v>791</v>
+        <v>5</v>
+      </c>
+      <c r="C83" s="85" t="s">
+        <v>172</v>
+      </c>
+      <c r="D83" s="48" t="s">
+        <v>542</v>
+      </c>
+      <c r="E83" s="83" t="s">
+        <v>902</v>
       </c>
       <c r="F83" s="83"/>
       <c r="G83" s="7"/>
-      <c r="H83" s="110" t="s">
-        <v>570</v>
+      <c r="H83" s="135" t="s">
+        <v>543</v>
       </c>
       <c r="I83" s="109"/>
       <c r="J83" s="80" t="s">
@@ -10235,27 +10257,25 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="84" spans="1:12" ht="24">
+    <row r="84" spans="1:12">
       <c r="A84" s="89" t="s">
-        <v>658</v>
+        <v>686</v>
       </c>
       <c r="B84" s="83" t="s">
-        <v>553</v>
-      </c>
-      <c r="C84" s="82" t="s">
-        <v>171</v>
-      </c>
-      <c r="D84" s="34">
-        <v>9.3000000000000007</v>
+        <v>5</v>
+      </c>
+      <c r="C84" s="85" t="s">
+        <v>173</v>
+      </c>
+      <c r="D84" s="48" t="s">
+        <v>174</v>
       </c>
       <c r="E84" s="83" t="s">
-        <v>98</v>
+        <v>902</v>
       </c>
       <c r="F84" s="83"/>
       <c r="G84" s="7"/>
-      <c r="H84" s="135" t="s">
-        <v>578</v>
-      </c>
+      <c r="H84" s="135"/>
       <c r="I84" s="109"/>
       <c r="J84" s="80" t="s">
         <v>418</v>
@@ -10265,27 +10285,25 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="85" spans="1:12" ht="36">
+    <row r="85" spans="1:12">
       <c r="A85" s="89" t="s">
-        <v>659</v>
+        <v>687</v>
       </c>
       <c r="B85" s="83" t="s">
-        <v>7</v>
+        <v>553</v>
       </c>
       <c r="C85" s="82" t="s">
         <v>171</v>
       </c>
       <c r="D85" s="48">
-        <v>85.7</v>
+        <v>94.7</v>
       </c>
       <c r="E85" s="83" t="s">
         <v>98</v>
       </c>
       <c r="F85" s="83"/>
       <c r="G85" s="7"/>
-      <c r="H85" s="110" t="s">
-        <v>567</v>
-      </c>
+      <c r="H85" s="135"/>
       <c r="I85" s="109"/>
       <c r="J85" s="80" t="s">
         <v>418</v>
@@ -10297,7 +10315,7 @@
     </row>
     <row r="86" spans="1:12" ht="24">
       <c r="A86" s="89" t="s">
-        <v>688</v>
+        <v>657</v>
       </c>
       <c r="B86" s="83" t="s">
         <v>7</v>
@@ -10305,16 +10323,16 @@
       <c r="C86" s="82" t="s">
         <v>171</v>
       </c>
-      <c r="D86" s="48">
-        <v>96.5</v>
-      </c>
-      <c r="E86" s="83" t="s">
-        <v>98</v>
+      <c r="D86" s="183" t="s">
+        <v>790</v>
+      </c>
+      <c r="E86" s="182" t="s">
+        <v>791</v>
       </c>
       <c r="F86" s="83"/>
       <c r="G86" s="7"/>
       <c r="H86" s="110" t="s">
-        <v>575</v>
+        <v>570</v>
       </c>
       <c r="I86" s="109"/>
       <c r="J86" s="80" t="s">
@@ -10325,9 +10343,9 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="87" spans="1:12">
+    <row r="87" spans="1:12" ht="24">
       <c r="A87" s="89" t="s">
-        <v>689</v>
+        <v>658</v>
       </c>
       <c r="B87" s="83" t="s">
         <v>553</v>
@@ -10335,15 +10353,17 @@
       <c r="C87" s="82" t="s">
         <v>171</v>
       </c>
-      <c r="D87" s="48">
-        <v>49.7</v>
+      <c r="D87" s="34">
+        <v>9.3000000000000007</v>
       </c>
       <c r="E87" s="83" t="s">
         <v>98</v>
       </c>
       <c r="F87" s="83"/>
       <c r="G87" s="7"/>
-      <c r="H87" s="135"/>
+      <c r="H87" s="135" t="s">
+        <v>578</v>
+      </c>
       <c r="I87" s="109"/>
       <c r="J87" s="80" t="s">
         <v>418</v>
@@ -10355,7 +10375,7 @@
     </row>
     <row r="88" spans="1:12" ht="24">
       <c r="A88" s="89" t="s">
-        <v>690</v>
+        <v>659</v>
       </c>
       <c r="B88" s="83" t="s">
         <v>7</v>
@@ -10364,7 +10384,7 @@
         <v>171</v>
       </c>
       <c r="D88" s="48">
-        <v>65.3</v>
+        <v>85.7</v>
       </c>
       <c r="E88" s="83" t="s">
         <v>98</v>
@@ -10372,7 +10392,7 @@
       <c r="F88" s="83"/>
       <c r="G88" s="7"/>
       <c r="H88" s="110" t="s">
-        <v>575</v>
+        <v>567</v>
       </c>
       <c r="I88" s="109"/>
       <c r="J88" s="80" t="s">
@@ -10384,36 +10404,36 @@
       </c>
     </row>
     <row r="89" spans="1:12">
-      <c r="A89" s="89" t="s">
-        <v>691</v>
-      </c>
-      <c r="B89" s="83" t="s">
+      <c r="A89" s="153" t="s">
+        <v>1012</v>
+      </c>
+      <c r="B89" s="175" t="s">
         <v>553</v>
       </c>
-      <c r="C89" s="82" t="s">
+      <c r="C89" s="186" t="s">
         <v>171</v>
       </c>
       <c r="D89" s="48">
-        <v>49.7</v>
-      </c>
-      <c r="E89" s="83" t="s">
-        <v>98</v>
-      </c>
-      <c r="F89" s="83"/>
-      <c r="G89" s="7"/>
-      <c r="H89" s="135"/>
+        <v>2.5299999999999998</v>
+      </c>
+      <c r="E89" s="175" t="s">
+        <v>1010</v>
+      </c>
+      <c r="F89" s="175"/>
+      <c r="G89" s="176"/>
+      <c r="H89" s="179" t="s">
+        <v>1009</v>
+      </c>
       <c r="I89" s="109"/>
-      <c r="J89" s="80" t="s">
+      <c r="J89" s="191" t="s">
         <v>418</v>
       </c>
-      <c r="K89" s="80"/>
-      <c r="L89" s="191" t="s">
-        <v>1005</v>
-      </c>
-    </row>
-    <row r="90" spans="1:12" ht="24">
+      <c r="K89" s="191"/>
+      <c r="L89" s="191"/>
+    </row>
+    <row r="90" spans="1:12">
       <c r="A90" s="89" t="s">
-        <v>692</v>
+        <v>688</v>
       </c>
       <c r="B90" s="83" t="s">
         <v>7</v>
@@ -10422,13 +10442,13 @@
         <v>171</v>
       </c>
       <c r="D90" s="48">
-        <v>192.9</v>
+        <v>96.5</v>
       </c>
       <c r="E90" s="83" t="s">
         <v>98</v>
       </c>
       <c r="F90" s="83"/>
-      <c r="G90" s="83"/>
+      <c r="G90" s="7"/>
       <c r="H90" s="110" t="s">
         <v>575</v>
       </c>
@@ -10443,7 +10463,7 @@
     </row>
     <row r="91" spans="1:12">
       <c r="A91" s="89" t="s">
-        <v>693</v>
+        <v>689</v>
       </c>
       <c r="B91" s="83" t="s">
         <v>553</v>
@@ -10458,7 +10478,7 @@
         <v>98</v>
       </c>
       <c r="F91" s="83"/>
-      <c r="G91" s="83"/>
+      <c r="G91" s="7"/>
       <c r="H91" s="135"/>
       <c r="I91" s="109"/>
       <c r="J91" s="80" t="s">
@@ -10469,9 +10489,9 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="92" spans="1:12" ht="24">
+    <row r="92" spans="1:12">
       <c r="A92" s="89" t="s">
-        <v>660</v>
+        <v>690</v>
       </c>
       <c r="B92" s="83" t="s">
         <v>7</v>
@@ -10480,15 +10500,15 @@
         <v>171</v>
       </c>
       <c r="D92" s="48">
-        <v>181.6</v>
+        <v>65.3</v>
       </c>
       <c r="E92" s="83" t="s">
         <v>98</v>
       </c>
       <c r="F92" s="83"/>
-      <c r="G92" s="83"/>
+      <c r="G92" s="7"/>
       <c r="H92" s="110" t="s">
-        <v>572</v>
+        <v>575</v>
       </c>
       <c r="I92" s="109"/>
       <c r="J92" s="80" t="s">
@@ -10501,7 +10521,7 @@
     </row>
     <row r="93" spans="1:12">
       <c r="A93" s="89" t="s">
-        <v>661</v>
+        <v>691</v>
       </c>
       <c r="B93" s="83" t="s">
         <v>553</v>
@@ -10510,13 +10530,13 @@
         <v>171</v>
       </c>
       <c r="D93" s="48">
-        <v>6.3</v>
+        <v>49.7</v>
       </c>
       <c r="E93" s="83" t="s">
         <v>98</v>
       </c>
       <c r="F93" s="83"/>
-      <c r="G93" s="83"/>
+      <c r="G93" s="7"/>
       <c r="H93" s="135"/>
       <c r="I93" s="109"/>
       <c r="J93" s="80" t="s">
@@ -10529,7 +10549,7 @@
     </row>
     <row r="94" spans="1:12">
       <c r="A94" s="89" t="s">
-        <v>662</v>
+        <v>692</v>
       </c>
       <c r="B94" s="83" t="s">
         <v>7</v>
@@ -10537,15 +10557,17 @@
       <c r="C94" s="82" t="s">
         <v>171</v>
       </c>
-      <c r="D94" s="34">
-        <v>215.6</v>
+      <c r="D94" s="48">
+        <v>192.9</v>
       </c>
       <c r="E94" s="83" t="s">
         <v>98</v>
       </c>
       <c r="F94" s="83"/>
       <c r="G94" s="83"/>
-      <c r="H94" s="135"/>
+      <c r="H94" s="110" t="s">
+        <v>575</v>
+      </c>
       <c r="I94" s="109"/>
       <c r="J94" s="80" t="s">
         <v>418</v>
@@ -10557,7 +10579,7 @@
     </row>
     <row r="95" spans="1:12">
       <c r="A95" s="89" t="s">
-        <v>663</v>
+        <v>693</v>
       </c>
       <c r="B95" s="83" t="s">
         <v>553</v>
@@ -10565,8 +10587,8 @@
       <c r="C95" s="82" t="s">
         <v>171</v>
       </c>
-      <c r="D95" s="34">
-        <v>9.5</v>
+      <c r="D95" s="48">
+        <v>49.7</v>
       </c>
       <c r="E95" s="83" t="s">
         <v>98</v>
@@ -10585,7 +10607,7 @@
     </row>
     <row r="96" spans="1:12">
       <c r="A96" s="89" t="s">
-        <v>664</v>
+        <v>660</v>
       </c>
       <c r="B96" s="83" t="s">
         <v>7</v>
@@ -10593,15 +10615,17 @@
       <c r="C96" s="82" t="s">
         <v>171</v>
       </c>
-      <c r="D96" s="34">
-        <v>65.8</v>
+      <c r="D96" s="48">
+        <v>181.6</v>
       </c>
       <c r="E96" s="83" t="s">
         <v>98</v>
       </c>
       <c r="F96" s="83"/>
       <c r="G96" s="83"/>
-      <c r="H96" s="135"/>
+      <c r="H96" s="110" t="s">
+        <v>572</v>
+      </c>
       <c r="I96" s="109"/>
       <c r="J96" s="80" t="s">
         <v>418</v>
@@ -10613,7 +10637,7 @@
     </row>
     <row r="97" spans="1:12">
       <c r="A97" s="89" t="s">
-        <v>665</v>
+        <v>661</v>
       </c>
       <c r="B97" s="83" t="s">
         <v>553</v>
@@ -10621,17 +10645,15 @@
       <c r="C97" s="82" t="s">
         <v>171</v>
       </c>
-      <c r="D97" s="34">
-        <v>2.4</v>
+      <c r="D97" s="48">
+        <v>6.3</v>
       </c>
       <c r="E97" s="83" t="s">
         <v>98</v>
       </c>
-      <c r="F97" s="82"/>
-      <c r="G97" s="82"/>
-      <c r="H97" s="110" t="s">
-        <v>576</v>
-      </c>
+      <c r="F97" s="83"/>
+      <c r="G97" s="83"/>
+      <c r="H97" s="135"/>
       <c r="I97" s="109"/>
       <c r="J97" s="80" t="s">
         <v>418</v>
@@ -10643,7 +10665,7 @@
     </row>
     <row r="98" spans="1:12">
       <c r="A98" s="89" t="s">
-        <v>666</v>
+        <v>662</v>
       </c>
       <c r="B98" s="83" t="s">
         <v>7</v>
@@ -10652,13 +10674,13 @@
         <v>171</v>
       </c>
       <c r="D98" s="34">
-        <v>79.400000000000006</v>
+        <v>215.6</v>
       </c>
       <c r="E98" s="83" t="s">
         <v>98</v>
       </c>
       <c r="F98" s="83"/>
-      <c r="G98" s="7"/>
+      <c r="G98" s="83"/>
       <c r="H98" s="135"/>
       <c r="I98" s="109"/>
       <c r="J98" s="80" t="s">
@@ -10671,7 +10693,7 @@
     </row>
     <row r="99" spans="1:12">
       <c r="A99" s="89" t="s">
-        <v>667</v>
+        <v>663</v>
       </c>
       <c r="B99" s="83" t="s">
         <v>553</v>
@@ -10680,13 +10702,13 @@
         <v>171</v>
       </c>
       <c r="D99" s="34">
-        <v>2.84</v>
+        <v>9.5</v>
       </c>
       <c r="E99" s="83" t="s">
         <v>98</v>
       </c>
       <c r="F99" s="83"/>
-      <c r="G99" s="7"/>
+      <c r="G99" s="83"/>
       <c r="H99" s="135"/>
       <c r="I99" s="109"/>
       <c r="J99" s="80" t="s">
@@ -10697,9 +10719,9 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="100" spans="1:12" ht="24">
+    <row r="100" spans="1:12">
       <c r="A100" s="89" t="s">
-        <v>668</v>
+        <v>664</v>
       </c>
       <c r="B100" s="83" t="s">
         <v>7</v>
@@ -10707,18 +10729,16 @@
       <c r="C100" s="82" t="s">
         <v>171</v>
       </c>
-      <c r="D100" s="48">
-        <v>1032.7</v>
+      <c r="D100" s="34">
+        <v>65.8</v>
       </c>
       <c r="E100" s="83" t="s">
         <v>98</v>
       </c>
-      <c r="F100" s="87"/>
-      <c r="G100" s="8"/>
-      <c r="H100" s="110" t="s">
-        <v>572</v>
-      </c>
-      <c r="I100" s="43"/>
+      <c r="F100" s="83"/>
+      <c r="G100" s="83"/>
+      <c r="H100" s="135"/>
+      <c r="I100" s="109"/>
       <c r="J100" s="80" t="s">
         <v>418</v>
       </c>
@@ -10729,7 +10749,7 @@
     </row>
     <row r="101" spans="1:12">
       <c r="A101" s="89" t="s">
-        <v>669</v>
+        <v>665</v>
       </c>
       <c r="B101" s="83" t="s">
         <v>553</v>
@@ -10737,16 +10757,18 @@
       <c r="C101" s="82" t="s">
         <v>171</v>
       </c>
-      <c r="D101" s="48">
-        <v>94.7</v>
+      <c r="D101" s="34">
+        <v>2.4</v>
       </c>
       <c r="E101" s="83" t="s">
         <v>98</v>
       </c>
-      <c r="F101" s="87"/>
-      <c r="G101" s="8"/>
-      <c r="H101" s="139"/>
-      <c r="I101" s="43"/>
+      <c r="F101" s="82"/>
+      <c r="G101" s="82"/>
+      <c r="H101" s="110" t="s">
+        <v>576</v>
+      </c>
+      <c r="I101" s="109"/>
       <c r="J101" s="80" t="s">
         <v>418</v>
       </c>
@@ -10756,16 +10778,130 @@
       </c>
     </row>
     <row r="102" spans="1:12">
-      <c r="F102" s="36"/>
+      <c r="A102" s="89" t="s">
+        <v>666</v>
+      </c>
+      <c r="B102" s="83" t="s">
+        <v>7</v>
+      </c>
+      <c r="C102" s="82" t="s">
+        <v>171</v>
+      </c>
+      <c r="D102" s="34">
+        <v>79.400000000000006</v>
+      </c>
+      <c r="E102" s="83" t="s">
+        <v>98</v>
+      </c>
+      <c r="F102" s="83"/>
+      <c r="G102" s="7"/>
+      <c r="H102" s="135"/>
+      <c r="I102" s="109"/>
+      <c r="J102" s="80" t="s">
+        <v>418</v>
+      </c>
+      <c r="K102" s="80"/>
+      <c r="L102" s="191" t="s">
+        <v>1005</v>
+      </c>
     </row>
     <row r="103" spans="1:12">
-      <c r="F103" s="36"/>
+      <c r="A103" s="89" t="s">
+        <v>667</v>
+      </c>
+      <c r="B103" s="83" t="s">
+        <v>553</v>
+      </c>
+      <c r="C103" s="82" t="s">
+        <v>171</v>
+      </c>
+      <c r="D103" s="34">
+        <v>2.84</v>
+      </c>
+      <c r="E103" s="83" t="s">
+        <v>98</v>
+      </c>
+      <c r="F103" s="83"/>
+      <c r="G103" s="7"/>
+      <c r="H103" s="135"/>
+      <c r="I103" s="109"/>
+      <c r="J103" s="80" t="s">
+        <v>418</v>
+      </c>
+      <c r="K103" s="80"/>
+      <c r="L103" s="191" t="s">
+        <v>1005</v>
+      </c>
     </row>
     <row r="104" spans="1:12">
-      <c r="E104" s="36"/>
+      <c r="A104" s="89" t="s">
+        <v>668</v>
+      </c>
+      <c r="B104" s="83" t="s">
+        <v>7</v>
+      </c>
+      <c r="C104" s="82" t="s">
+        <v>171</v>
+      </c>
+      <c r="D104" s="48">
+        <v>1032.7</v>
+      </c>
+      <c r="E104" s="83" t="s">
+        <v>98</v>
+      </c>
+      <c r="F104" s="87"/>
+      <c r="G104" s="8"/>
+      <c r="H104" s="110" t="s">
+        <v>572</v>
+      </c>
+      <c r="I104" s="43"/>
+      <c r="J104" s="80" t="s">
+        <v>418</v>
+      </c>
+      <c r="K104" s="80"/>
+      <c r="L104" s="191" t="s">
+        <v>1005</v>
+      </c>
     </row>
     <row r="105" spans="1:12">
-      <c r="E105" s="36"/>
+      <c r="A105" s="89" t="s">
+        <v>669</v>
+      </c>
+      <c r="B105" s="83" t="s">
+        <v>553</v>
+      </c>
+      <c r="C105" s="82" t="s">
+        <v>171</v>
+      </c>
+      <c r="D105" s="48">
+        <v>94.7</v>
+      </c>
+      <c r="E105" s="83" t="s">
+        <v>98</v>
+      </c>
+      <c r="F105" s="87"/>
+      <c r="G105" s="8"/>
+      <c r="H105" s="139"/>
+      <c r="I105" s="43"/>
+      <c r="J105" s="80" t="s">
+        <v>418</v>
+      </c>
+      <c r="K105" s="80"/>
+      <c r="L105" s="191" t="s">
+        <v>1005</v>
+      </c>
+    </row>
+    <row r="106" spans="1:12">
+      <c r="F106" s="36"/>
+    </row>
+    <row r="107" spans="1:12">
+      <c r="F107" s="36"/>
+    </row>
+    <row r="108" spans="1:12">
+      <c r="E108" s="36"/>
+    </row>
+    <row r="109" spans="1:12">
+      <c r="E109" s="36"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10784,20 +10920,20 @@
       <selection pane="bottomRight" activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="12"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" style="73" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.85546875" style="73" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.5703125" style="27" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="27"/>
-    <col min="5" max="6" width="17.28515625" style="73" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.28515625" style="73" customWidth="1"/>
-    <col min="8" max="8" width="29.7109375" style="73" customWidth="1"/>
-    <col min="9" max="9" width="21.42578125" style="73" customWidth="1"/>
-    <col min="10" max="10" width="18.28515625" style="73" customWidth="1"/>
-    <col min="11" max="11" width="28.85546875" style="73" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="30.42578125" style="73" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="73"/>
+    <col min="1" max="1" width="20.6640625" style="73" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.88671875" style="73" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5546875" style="27" customWidth="1"/>
+    <col min="4" max="4" width="9.109375" style="27"/>
+    <col min="5" max="6" width="17.33203125" style="73" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.33203125" style="73" customWidth="1"/>
+    <col min="8" max="8" width="29.6640625" style="73" customWidth="1"/>
+    <col min="9" max="9" width="21.44140625" style="73" customWidth="1"/>
+    <col min="10" max="10" width="18.33203125" style="73" customWidth="1"/>
+    <col min="11" max="11" width="28.88671875" style="73" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="30.44140625" style="73" customWidth="1"/>
+    <col min="13" max="16384" width="9.109375" style="73"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="24">
@@ -10838,7 +10974,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="72">
+    <row r="2" spans="1:12" ht="60">
       <c r="A2" s="50" t="s">
         <v>178</v>
       </c>
@@ -10882,19 +11018,19 @@
       <selection pane="topRight" activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="29.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" customWidth="1"/>
-    <col min="5" max="5" width="23.5703125" customWidth="1"/>
-    <col min="6" max="7" width="23.5703125" style="15" customWidth="1"/>
-    <col min="8" max="8" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="46.140625" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" style="13"/>
-    <col min="11" max="11" width="28.85546875" style="73" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="30.42578125" style="73" customWidth="1"/>
+    <col min="1" max="1" width="29.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.88671875" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" customWidth="1"/>
+    <col min="4" max="4" width="14.44140625" customWidth="1"/>
+    <col min="5" max="5" width="23.5546875" customWidth="1"/>
+    <col min="6" max="7" width="23.5546875" style="15" customWidth="1"/>
+    <col min="8" max="8" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="46.109375" customWidth="1"/>
+    <col min="10" max="10" width="9.109375" style="13"/>
+    <col min="11" max="11" width="28.88671875" style="73" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="30.44140625" style="73" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16384">
@@ -27586,28 +27722,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="12"/>
   <cols>
-    <col min="1" max="1" width="26.42578125" style="73" customWidth="1"/>
-    <col min="2" max="2" width="17.7109375" style="73" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" style="73" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" style="73" customWidth="1"/>
-    <col min="5" max="5" width="31.42578125" style="73" customWidth="1"/>
+    <col min="1" max="1" width="26.44140625" style="73" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" style="73" customWidth="1"/>
+    <col min="3" max="3" width="16.5546875" style="73" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" style="73" customWidth="1"/>
+    <col min="5" max="5" width="31.44140625" style="73" customWidth="1"/>
     <col min="6" max="6" width="12" style="73" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.140625" style="73" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="44.7109375" style="110" customWidth="1"/>
-    <col min="9" max="9" width="6.7109375" style="73" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.28515625" style="27" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="28.85546875" style="73" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="30.42578125" style="73" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="73"/>
+    <col min="7" max="7" width="5.109375" style="73" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="44.6640625" style="110" customWidth="1"/>
+    <col min="9" max="9" width="6.6640625" style="73" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.33203125" style="27" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="28.88671875" style="73" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="30.44140625" style="73" customWidth="1"/>
+    <col min="13" max="16384" width="9.109375" style="73"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -27691,18 +27827,18 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="12"/>
   <cols>
-    <col min="1" max="1" width="28.28515625" style="27" customWidth="1"/>
-    <col min="2" max="2" width="9.85546875" style="27" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.33203125" style="27" customWidth="1"/>
+    <col min="2" max="2" width="9.88671875" style="27" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20" style="27" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="27"/>
-    <col min="5" max="6" width="17.28515625" style="27" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="14.7109375" style="27" customWidth="1"/>
-    <col min="9" max="10" width="9.140625" style="27"/>
-    <col min="11" max="11" width="28.85546875" style="73" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="30.42578125" style="73" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="27"/>
+    <col min="4" max="4" width="9.109375" style="27"/>
+    <col min="5" max="6" width="17.33203125" style="27" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="14.6640625" style="27" customWidth="1"/>
+    <col min="9" max="10" width="9.109375" style="27"/>
+    <col min="11" max="11" width="28.88671875" style="73" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="30.44140625" style="73" customWidth="1"/>
+    <col min="13" max="16384" width="9.109375" style="27"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="24">
@@ -27853,21 +27989,21 @@
       <selection pane="topRight" activeCell="I118" sqref="I118"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="12"/>
   <cols>
-    <col min="1" max="1" width="38.42578125" style="9" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" style="9" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" style="9" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" style="111" customWidth="1"/>
-    <col min="5" max="5" width="24.5703125" style="111" customWidth="1"/>
-    <col min="6" max="6" width="28.5703125" style="73" customWidth="1"/>
+    <col min="1" max="1" width="38.44140625" style="9" customWidth="1"/>
+    <col min="2" max="2" width="14.88671875" style="9" customWidth="1"/>
+    <col min="3" max="3" width="17.44140625" style="9" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" style="111" customWidth="1"/>
+    <col min="5" max="5" width="24.5546875" style="111" customWidth="1"/>
+    <col min="6" max="6" width="28.5546875" style="73" customWidth="1"/>
     <col min="7" max="7" width="40" style="73" customWidth="1"/>
-    <col min="8" max="8" width="41.85546875" style="73" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="51.140625" style="73" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.42578125" style="74" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="28.85546875" style="73" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="30.42578125" style="73" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="73"/>
+    <col min="8" max="8" width="41.88671875" style="73" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="51.109375" style="73" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.44140625" style="74" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="28.88671875" style="73" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="30.44140625" style="73" customWidth="1"/>
+    <col min="13" max="16384" width="9.109375" style="73"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -28030,7 +28166,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="24">
+    <row r="6" spans="1:12">
       <c r="A6" s="89" t="s">
         <v>357</v>
       </c>
@@ -28349,7 +28485,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="24">
+    <row r="17" spans="1:12">
       <c r="A17" s="94" t="s">
         <v>459</v>
       </c>
@@ -28567,7 +28703,7 @@
         <v>1006</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="24">
+    <row r="24" spans="1:12">
       <c r="A24" s="23" t="s">
         <v>351</v>
       </c>
@@ -28807,7 +28943,7 @@
       <c r="K31" s="80"/>
       <c r="L31" s="80"/>
     </row>
-    <row r="32" spans="1:12" ht="24">
+    <row r="32" spans="1:12">
       <c r="A32" s="23" t="s">
         <v>354</v>
       </c>
@@ -28985,7 +29121,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="38" spans="1:12" ht="24">
+    <row r="38" spans="1:12">
       <c r="A38" s="94" t="s">
         <v>461</v>
       </c>
@@ -29203,7 +29339,7 @@
         <v>1006</v>
       </c>
     </row>
-    <row r="45" spans="1:12" ht="24">
+    <row r="45" spans="1:12">
       <c r="A45" s="23" t="s">
         <v>350</v>
       </c>
@@ -29441,7 +29577,7 @@
       <c r="K52" s="80"/>
       <c r="L52" s="191"/>
     </row>
-    <row r="53" spans="1:12" ht="24">
+    <row r="53" spans="1:12">
       <c r="A53" s="23" t="s">
         <v>353</v>
       </c>
@@ -29597,7 +29733,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="58" spans="1:12" ht="48">
+    <row r="58" spans="1:12" ht="36">
       <c r="A58" s="89" t="s">
         <v>743</v>
       </c>
@@ -29627,7 +29763,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="59" spans="1:12" ht="48">
+    <row r="59" spans="1:12" ht="36">
       <c r="A59" s="89" t="s">
         <v>744</v>
       </c>
@@ -29657,7 +29793,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="60" spans="1:12" ht="48">
+    <row r="60" spans="1:12" ht="36">
       <c r="A60" s="89" t="s">
         <v>745</v>
       </c>
@@ -29687,7 +29823,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="61" spans="1:12" ht="48">
+    <row r="61" spans="1:12" ht="36">
       <c r="A61" s="89" t="s">
         <v>746</v>
       </c>
@@ -29717,7 +29853,7 @@
         <v>1004</v>
       </c>
     </row>
-    <row r="62" spans="1:12" ht="48">
+    <row r="62" spans="1:12" ht="36">
       <c r="A62" s="89" t="s">
         <v>747</v>
       </c>
@@ -29747,7 +29883,7 @@
         <v>1004</v>
       </c>
     </row>
-    <row r="63" spans="1:12" ht="48">
+    <row r="63" spans="1:12" ht="36">
       <c r="A63" s="89" t="s">
         <v>748</v>
       </c>
@@ -29777,7 +29913,7 @@
         <v>1004</v>
       </c>
     </row>
-    <row r="64" spans="1:12" ht="48">
+    <row r="64" spans="1:12" ht="36">
       <c r="A64" s="89" t="s">
         <v>732</v>
       </c>
@@ -29807,7 +29943,7 @@
         <v>1004</v>
       </c>
     </row>
-    <row r="65" spans="1:12" ht="48">
+    <row r="65" spans="1:12" ht="36">
       <c r="A65" s="89" t="s">
         <v>733</v>
       </c>
@@ -29901,7 +30037,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="68" spans="1:12" ht="48">
+    <row r="68" spans="1:12" ht="36">
       <c r="A68" s="153" t="s">
         <v>750</v>
       </c>
@@ -29931,7 +30067,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="69" spans="1:12" ht="48">
+    <row r="69" spans="1:12" ht="36">
       <c r="A69" s="153" t="s">
         <v>751</v>
       </c>
@@ -29961,7 +30097,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="70" spans="1:12" ht="48">
+    <row r="70" spans="1:12" ht="36">
       <c r="A70" s="153" t="s">
         <v>752</v>
       </c>
@@ -29991,7 +30127,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="71" spans="1:12" ht="48">
+    <row r="71" spans="1:12" ht="36">
       <c r="A71" s="153" t="s">
         <v>753</v>
       </c>
@@ -30021,7 +30157,7 @@
         <v>1004</v>
       </c>
     </row>
-    <row r="72" spans="1:12" ht="48">
+    <row r="72" spans="1:12" ht="36">
       <c r="A72" s="153" t="s">
         <v>754</v>
       </c>
@@ -30051,7 +30187,7 @@
         <v>1004</v>
       </c>
     </row>
-    <row r="73" spans="1:12" ht="48">
+    <row r="73" spans="1:12" ht="36">
       <c r="A73" s="153" t="s">
         <v>755</v>
       </c>
@@ -30081,7 +30217,7 @@
         <v>1004</v>
       </c>
     </row>
-    <row r="74" spans="1:12" ht="48">
+    <row r="74" spans="1:12" ht="36">
       <c r="A74" s="153" t="s">
         <v>735</v>
       </c>
@@ -30111,7 +30247,7 @@
         <v>1004</v>
       </c>
     </row>
-    <row r="75" spans="1:12" ht="48">
+    <row r="75" spans="1:12" ht="36">
       <c r="A75" s="153" t="s">
         <v>736</v>
       </c>
@@ -31197,7 +31333,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="109" spans="1:12" ht="36">
+    <row r="109" spans="1:12" ht="24">
       <c r="A109" s="89" t="s">
         <v>956</v>
       </c>
@@ -31291,7 +31427,7 @@
         <v>1003</v>
       </c>
     </row>
-    <row r="112" spans="1:12" ht="36">
+    <row r="112" spans="1:12" ht="24">
       <c r="A112" s="89" t="s">
         <v>959</v>
       </c>
@@ -32325,7 +32461,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="145" spans="1:12" s="81" customFormat="1" ht="15">
+    <row r="145" spans="1:12" s="81" customFormat="1" ht="14.4">
       <c r="A145" s="12" t="s">
         <v>484</v>
       </c>
@@ -32363,7 +32499,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="146" spans="1:12" s="81" customFormat="1" ht="15">
+    <row r="146" spans="1:12" s="81" customFormat="1" ht="14.4">
       <c r="A146" s="104" t="s">
         <v>486</v>
       </c>
@@ -32391,7 +32527,7 @@
       </c>
       <c r="L146" s="80"/>
     </row>
-    <row r="147" spans="1:12" s="81" customFormat="1" ht="15">
+    <row r="147" spans="1:12" s="81" customFormat="1" ht="14.4">
       <c r="A147" s="104" t="s">
         <v>487</v>
       </c>
@@ -32411,7 +32547,7 @@
       </c>
       <c r="L147" s="80"/>
     </row>
-    <row r="148" spans="1:12" s="81" customFormat="1" ht="15">
+    <row r="148" spans="1:12" s="81" customFormat="1" ht="14.4">
       <c r="A148" s="104" t="s">
         <v>393</v>
       </c>
@@ -32439,7 +32575,7 @@
       </c>
       <c r="L148" s="80"/>
     </row>
-    <row r="149" spans="1:12" s="81" customFormat="1" ht="15">
+    <row r="149" spans="1:12" s="81" customFormat="1" ht="14.4">
       <c r="A149" s="104" t="s">
         <v>488</v>
       </c>
@@ -32467,7 +32603,7 @@
       </c>
       <c r="L149" s="80"/>
     </row>
-    <row r="150" spans="1:12" s="81" customFormat="1" ht="15">
+    <row r="150" spans="1:12" s="81" customFormat="1" ht="14.4">
       <c r="A150" s="104" t="s">
         <v>492</v>
       </c>
@@ -32487,7 +32623,7 @@
       </c>
       <c r="L150" s="80"/>
     </row>
-    <row r="151" spans="1:12" s="81" customFormat="1" ht="15">
+    <row r="151" spans="1:12" s="81" customFormat="1" ht="14.4">
       <c r="A151" s="104" t="s">
         <v>489</v>
       </c>
@@ -32521,7 +32657,7 @@
       </c>
       <c r="L151" s="80"/>
     </row>
-    <row r="152" spans="1:12" s="81" customFormat="1" ht="15">
+    <row r="152" spans="1:12" s="81" customFormat="1" ht="14.4">
       <c r="A152" s="104" t="s">
         <v>490</v>
       </c>
@@ -32549,7 +32685,7 @@
       </c>
       <c r="L152" s="80"/>
     </row>
-    <row r="153" spans="1:12" s="81" customFormat="1" ht="15">
+    <row r="153" spans="1:12" s="81" customFormat="1" ht="14.4">
       <c r="A153" s="104" t="s">
         <v>493</v>
       </c>
@@ -32569,7 +32705,7 @@
       </c>
       <c r="L153" s="80"/>
     </row>
-    <row r="154" spans="1:12" s="81" customFormat="1" ht="15">
+    <row r="154" spans="1:12" s="81" customFormat="1" ht="14.4">
       <c r="A154" s="104" t="s">
         <v>491</v>
       </c>
@@ -32597,7 +32733,7 @@
       </c>
       <c r="L154" s="80"/>
     </row>
-    <row r="155" spans="1:12" s="81" customFormat="1" ht="15">
+    <row r="155" spans="1:12" s="81" customFormat="1" ht="14.4">
       <c r="A155" s="104" t="s">
         <v>494</v>
       </c>
@@ -32617,7 +32753,7 @@
       </c>
       <c r="L155" s="80"/>
     </row>
-    <row r="156" spans="1:12" s="81" customFormat="1" ht="15">
+    <row r="156" spans="1:12" s="81" customFormat="1" ht="14.4">
       <c r="A156" s="104" t="s">
         <v>495</v>
       </c>
@@ -32637,7 +32773,7 @@
       </c>
       <c r="L156" s="80"/>
     </row>
-    <row r="157" spans="1:12" s="81" customFormat="1" ht="15">
+    <row r="157" spans="1:12" s="81" customFormat="1" ht="14.4">
       <c r="A157" s="104" t="s">
         <v>496</v>
       </c>
@@ -35193,21 +35329,21 @@
       <selection pane="bottomRight" activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="44.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" style="36" customWidth="1"/>
+    <col min="1" max="1" width="44.44140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" style="36" customWidth="1"/>
     <col min="3" max="3" width="30" style="36" customWidth="1"/>
-    <col min="4" max="4" width="18.5703125" style="36" customWidth="1"/>
+    <col min="4" max="4" width="18.5546875" style="36" customWidth="1"/>
     <col min="5" max="5" width="20" style="37" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.28515625" style="37" customWidth="1"/>
+    <col min="6" max="6" width="27.33203125" style="37" customWidth="1"/>
     <col min="7" max="7" width="24" style="37" customWidth="1"/>
-    <col min="8" max="8" width="37.5703125" style="36" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="37.5546875" style="36" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="52" style="9" customWidth="1"/>
-    <col min="10" max="10" width="24.7109375" style="105" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="28.85546875" style="73" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="30.42578125" style="73" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="1"/>
+    <col min="10" max="10" width="24.6640625" style="105" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="28.88671875" style="73" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="30.44140625" style="73" customWidth="1"/>
+    <col min="13" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24">
@@ -35260,7 +35396,7 @@
       <c r="W1" s="3"/>
       <c r="X1" s="3"/>
     </row>
-    <row r="2" spans="1:24" ht="48">
+    <row r="2" spans="1:24" ht="36">
       <c r="A2" s="17" t="s">
         <v>950</v>
       </c>
@@ -37104,7 +37240,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="57" spans="1:12" s="81" customFormat="1" ht="24.75">
+    <row r="57" spans="1:12" s="81" customFormat="1" ht="24.6">
       <c r="A57" s="104" t="s">
         <v>407</v>
       </c>
@@ -37386,7 +37522,7 @@
         <v>806</v>
       </c>
     </row>
-    <row r="66" spans="1:12" s="81" customFormat="1" ht="24.75">
+    <row r="66" spans="1:12" s="81" customFormat="1" ht="24.6">
       <c r="A66" s="104" t="s">
         <v>411</v>
       </c>
@@ -37450,7 +37586,7 @@
       </c>
       <c r="L67" s="80"/>
     </row>
-    <row r="68" spans="1:12" s="81" customFormat="1" ht="24.75">
+    <row r="68" spans="1:12" s="81" customFormat="1" ht="24.6">
       <c r="A68" s="104" t="s">
         <v>412</v>
       </c>
@@ -37558,20 +37694,20 @@
       <selection pane="topRight" activeCell="L39" sqref="L39:L76"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="31.140625" style="137" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9.140625" style="137"/>
-    <col min="4" max="4" width="14.85546875" style="137" customWidth="1"/>
-    <col min="5" max="5" width="26.42578125" style="138" customWidth="1"/>
-    <col min="6" max="6" width="30.7109375" style="137" customWidth="1"/>
-    <col min="7" max="7" width="26.140625" style="137" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="61.42578125" style="168" customWidth="1"/>
-    <col min="9" max="9" width="52.42578125" style="137" customWidth="1"/>
-    <col min="10" max="10" width="24.85546875" style="137" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.140625" style="137"/>
-    <col min="12" max="12" width="12.5703125" style="137" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="137"/>
+    <col min="1" max="1" width="31.109375" style="137" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.109375" style="137"/>
+    <col min="4" max="4" width="14.88671875" style="137" customWidth="1"/>
+    <col min="5" max="5" width="26.44140625" style="138" customWidth="1"/>
+    <col min="6" max="6" width="30.6640625" style="137" customWidth="1"/>
+    <col min="7" max="7" width="26.109375" style="137" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="61.44140625" style="168" customWidth="1"/>
+    <col min="9" max="9" width="52.44140625" style="137" customWidth="1"/>
+    <col min="10" max="10" width="24.88671875" style="137" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.109375" style="137"/>
+    <col min="12" max="12" width="12.5546875" style="137" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.109375" style="137"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="73" customFormat="1" ht="26.25" customHeight="1">
@@ -38854,7 +38990,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="39" spans="1:12" ht="24.75">
+    <row r="39" spans="1:12">
       <c r="A39" s="142" t="s">
         <v>853</v>
       </c>
@@ -39034,7 +39170,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="45" spans="1:12" ht="36.75">
+    <row r="45" spans="1:12" ht="36.6">
       <c r="A45" s="142" t="s">
         <v>860</v>
       </c>
@@ -39056,7 +39192,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="46" spans="1:12" ht="72.75">
+    <row r="46" spans="1:12" ht="60.6">
       <c r="A46" s="142" t="s">
         <v>861</v>
       </c>
@@ -39146,7 +39282,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="49" spans="1:12" ht="24.75">
+    <row r="49" spans="1:12" ht="24">
       <c r="A49" s="142" t="s">
         <v>864</v>
       </c>
@@ -39178,7 +39314,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="50" spans="1:12" ht="48.75">
+    <row r="50" spans="1:12" ht="36.6">
       <c r="A50" s="142" t="s">
         <v>865</v>
       </c>
@@ -39406,7 +39542,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="58" spans="1:12" ht="24.75">
+    <row r="58" spans="1:12">
       <c r="A58" s="142" t="s">
         <v>873</v>
       </c>
@@ -39580,7 +39716,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="64" spans="1:12" ht="36.75">
+    <row r="64" spans="1:12" ht="24.6">
       <c r="A64" s="142" t="s">
         <v>879</v>
       </c>
@@ -39606,7 +39742,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="65" spans="1:12" ht="72.75">
+    <row r="65" spans="1:12" ht="60.6">
       <c r="A65" s="142" t="s">
         <v>880</v>
       </c>
@@ -39696,7 +39832,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="68" spans="1:12" ht="24.75">
+    <row r="68" spans="1:12" ht="24">
       <c r="A68" s="142" t="s">
         <v>883</v>
       </c>
@@ -39728,7 +39864,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="69" spans="1:12" ht="48.75">
+    <row r="69" spans="1:12" ht="36.6">
       <c r="A69" s="142" t="s">
         <v>884</v>
       </c>

</xml_diff>

<commit_message>
Corrected the pulmonary vascular resistance and pulmonary vascular resistance index equations. Also corrected the Cardiovascular validation table to reflect an accurate value for pulmonary vascular resistance index. Previously calculated value was miscalculated.
</commit_message>
<xml_diff>
--- a/test/validation/SystemValidationData.xlsx
+++ b/test/validation/SystemValidationData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21727"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\PulseHemorrhage\engine\test\validation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85F90A60-35B2-406E-8762-17CCD7A2E67F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A910F68-5B4B-4161-BACF-D174A9053B53}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="1320" windowWidth="11856" windowHeight="6648" tabRatio="724" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="724" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blood Chemistry" sheetId="4" r:id="rId1"/>
@@ -24,11 +24,18 @@
     <sheet name="Tissue" sheetId="34" r:id="rId9"/>
   </sheets>
   <calcPr calcId="181029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3626" uniqueCount="1016">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3627" uniqueCount="1017">
   <si>
     <t>Output</t>
   </si>
@@ -2977,9 +2984,6 @@
     <t>p167 &amp; p232</t>
   </si>
   <si>
-    <t>"The normal human weighing 70kg has a body surface area of about 1.7 square meteres." Therefore, 0.14/1.7.</t>
-  </si>
-  <si>
     <t>RespirationMusclePressure*</t>
   </si>
   <si>
@@ -3199,6 +3203,12 @@
   </si>
   <si>
     <t>RightArmVasculature-InFlow</t>
+  </si>
+  <si>
+    <t>The normal human weighing 70kg has a body surface area of about 1.7 square meteres.</t>
+  </si>
+  <si>
+    <t>The normal human weighing 70kg has a body surface area of about 1.7 square meteres. Therefore, 0.14*1.7.</t>
   </si>
 </sst>
 </file>
@@ -4889,20 +4899,20 @@
       <selection pane="topRight" activeCell="L54" sqref="L54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12"/>
   <cols>
-    <col min="1" max="1" width="40.109375" style="73" customWidth="1"/>
-    <col min="2" max="2" width="7.109375" style="74" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.88671875" style="74" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.88671875" style="74" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="33.88671875" style="74" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.5546875" style="74" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.140625" style="73" customWidth="1"/>
+    <col min="2" max="2" width="7.140625" style="74" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" style="74" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" style="74" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.85546875" style="74" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.5703125" style="74" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="48" style="74" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="49.33203125" style="73" customWidth="1"/>
+    <col min="8" max="8" width="49.28515625" style="73" customWidth="1"/>
     <col min="9" max="9" width="36" style="73" customWidth="1"/>
-    <col min="10" max="11" width="28.88671875" style="74" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="30.44140625" style="74" customWidth="1"/>
-    <col min="13" max="16384" width="9.109375" style="73"/>
+    <col min="10" max="11" width="28.85546875" style="74" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="30.42578125" style="74" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="73"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="26.25" customHeight="1">
@@ -4970,7 +4980,7 @@
       </c>
       <c r="K2" s="80"/>
       <c r="L2" s="80" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="24">
@@ -4998,7 +5008,7 @@
       </c>
       <c r="K3" s="80"/>
       <c r="L3" s="80" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -5026,7 +5036,7 @@
       </c>
       <c r="K4" s="80"/>
       <c r="L4" s="80" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="24">
@@ -5058,7 +5068,7 @@
       </c>
       <c r="K5" s="80"/>
       <c r="L5" s="80" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -5084,12 +5094,12 @@
       </c>
       <c r="K6" s="80"/>
       <c r="L6" s="80" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="7" spans="1:12">
       <c r="A7" s="153" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
       <c r="B7" s="186"/>
       <c r="C7" s="186" t="s">
@@ -5101,7 +5111,7 @@
       <c r="E7" s="186"/>
       <c r="F7" s="186"/>
       <c r="G7" s="186" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="H7" s="24"/>
       <c r="I7" s="78"/>
@@ -5138,7 +5148,7 @@
       </c>
       <c r="K8" s="80"/>
       <c r="L8" s="191" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -5168,7 +5178,7 @@
       </c>
       <c r="K9" s="80"/>
       <c r="L9" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="24">
@@ -5196,7 +5206,7 @@
       </c>
       <c r="K10" s="80"/>
       <c r="L10" s="80" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="27.75" customHeight="1">
@@ -5224,7 +5234,7 @@
       </c>
       <c r="K11" s="158"/>
       <c r="L11" s="158" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="27.75" customHeight="1">
@@ -5258,12 +5268,12 @@
       </c>
       <c r="K12" s="80"/>
       <c r="L12" s="80" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="24">
       <c r="A13" s="153" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="B13" s="186"/>
       <c r="C13" s="186" t="s">
@@ -5286,7 +5296,7 @@
       </c>
       <c r="K13" s="191"/>
       <c r="L13" s="191" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="24">
@@ -5344,7 +5354,7 @@
       </c>
       <c r="K15" s="80"/>
       <c r="L15" s="80" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -5372,7 +5382,7 @@
       </c>
       <c r="K16" s="158"/>
       <c r="L16" s="158" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="17" spans="1:12">
@@ -5402,7 +5412,7 @@
       </c>
       <c r="K17" s="80"/>
       <c r="L17" s="80" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="18" spans="1:12">
@@ -5428,7 +5438,7 @@
       </c>
       <c r="K18" s="80"/>
       <c r="L18" s="80" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="19" spans="1:12">
@@ -5454,7 +5464,7 @@
       </c>
       <c r="K19" s="80"/>
       <c r="L19" s="80" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="20" spans="1:12">
@@ -5527,7 +5537,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="40.799999999999997">
+    <row r="22" spans="1:12" ht="56.25">
       <c r="A22" s="142" t="s">
         <v>921</v>
       </c>
@@ -5554,10 +5564,10 @@
       </c>
       <c r="K22" s="145"/>
       <c r="L22" s="145" t="s">
-        <v>1005</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" ht="20.399999999999999">
+        <v>1004</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="22.5">
       <c r="A23" s="21" t="s">
         <v>922</v>
       </c>
@@ -5586,7 +5596,7 @@
       </c>
       <c r="K23" s="80"/>
       <c r="L23" s="80" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="24" spans="1:12">
@@ -5618,7 +5628,7 @@
       </c>
       <c r="K24" s="80"/>
       <c r="L24" s="80" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="25" spans="1:12">
@@ -5650,7 +5660,7 @@
       </c>
       <c r="K25" s="80"/>
       <c r="L25" s="80" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="26" spans="1:12" ht="36">
@@ -5680,7 +5690,7 @@
       <c r="J26" s="148"/>
       <c r="K26" s="148"/>
       <c r="L26" s="148" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="27" spans="1:12" ht="24">
@@ -5710,12 +5720,12 @@
       </c>
       <c r="K27" s="80"/>
       <c r="L27" s="80" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="28" spans="1:12" ht="60">
       <c r="A28" s="153" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="B28" s="154" t="s">
         <v>774</v>
@@ -5724,10 +5734,10 @@
         <v>171</v>
       </c>
       <c r="D28" s="186" t="s">
+        <v>999</v>
+      </c>
+      <c r="E28" s="155" t="s">
         <v>1000</v>
-      </c>
-      <c r="E28" s="155" t="s">
-        <v>1001</v>
       </c>
       <c r="F28" s="155"/>
       <c r="G28" s="155"/>
@@ -5736,7 +5746,7 @@
       <c r="J28" s="152"/>
       <c r="K28" s="152"/>
       <c r="L28" s="152" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="29" spans="1:12">
@@ -5766,7 +5776,7 @@
       </c>
       <c r="K29" s="80"/>
       <c r="L29" s="80" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="30" spans="1:12">
@@ -5796,7 +5806,7 @@
       </c>
       <c r="K30" s="80"/>
       <c r="L30" s="80" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="31" spans="1:12" ht="36">
@@ -5830,7 +5840,7 @@
       </c>
       <c r="K31" s="80"/>
       <c r="L31" s="80" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="32" spans="1:12" ht="24">
@@ -5862,7 +5872,7 @@
       </c>
       <c r="K32" s="80"/>
       <c r="L32" s="80" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="33" spans="1:12" ht="24">
@@ -5894,7 +5904,7 @@
       </c>
       <c r="K33" s="80"/>
       <c r="L33" s="80" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="34" spans="1:12" ht="24">
@@ -5926,7 +5936,7 @@
       </c>
       <c r="K34" s="80"/>
       <c r="L34" s="80" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="35" spans="1:12" ht="24">
@@ -5958,7 +5968,7 @@
       </c>
       <c r="K35" s="80"/>
       <c r="L35" s="80" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="36" spans="1:12">
@@ -5990,7 +6000,7 @@
       </c>
       <c r="K36" s="80"/>
       <c r="L36" s="80" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="37" spans="1:12" ht="36">
@@ -6024,7 +6034,7 @@
       </c>
       <c r="K37" s="158"/>
       <c r="L37" s="80" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="38" spans="1:12">
@@ -6090,7 +6100,7 @@
       </c>
       <c r="K39" s="80"/>
       <c r="L39" s="80" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="40" spans="1:12">
@@ -6120,7 +6130,7 @@
       </c>
       <c r="K40" s="80"/>
       <c r="L40" s="80" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="41" spans="1:12">
@@ -6150,7 +6160,7 @@
       </c>
       <c r="K41" s="80"/>
       <c r="L41" s="80" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="42" spans="1:12">
@@ -6180,7 +6190,7 @@
       </c>
       <c r="K42" s="80"/>
       <c r="L42" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="43" spans="1:12">
@@ -6210,7 +6220,7 @@
       </c>
       <c r="K43" s="80"/>
       <c r="L43" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="44" spans="1:12">
@@ -6240,7 +6250,7 @@
       </c>
       <c r="K44" s="80"/>
       <c r="L44" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="45" spans="1:12">
@@ -6270,7 +6280,7 @@
       </c>
       <c r="K45" s="80"/>
       <c r="L45" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="46" spans="1:12">
@@ -6300,7 +6310,7 @@
       </c>
       <c r="K46" s="80"/>
       <c r="L46" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="47" spans="1:12">
@@ -6368,7 +6378,7 @@
         <v>431</v>
       </c>
       <c r="L48" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="49" spans="1:12">
@@ -6402,10 +6412,10 @@
         <v>431</v>
       </c>
       <c r="L49" s="191" t="s">
-        <v>1005</v>
-      </c>
-    </row>
-    <row r="50" spans="1:12" ht="14.4">
+        <v>1004</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" ht="15">
       <c r="A50" s="104" t="s">
         <v>452</v>
       </c>
@@ -6434,7 +6444,7 @@
         <v>431</v>
       </c>
       <c r="L50" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="51" spans="1:12">
@@ -6464,7 +6474,7 @@
         <v>431</v>
       </c>
       <c r="L51" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="52" spans="1:12">
@@ -6496,10 +6506,10 @@
         <v>431</v>
       </c>
       <c r="L52" s="191" t="s">
-        <v>1005</v>
-      </c>
-    </row>
-    <row r="53" spans="1:12" ht="13.2">
+        <v>1004</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" ht="12.75">
       <c r="A53" s="104" t="s">
         <v>455</v>
       </c>
@@ -6596,7 +6606,7 @@
         <v>431</v>
       </c>
       <c r="L55" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="56" spans="1:12">
@@ -6664,7 +6674,7 @@
         <v>432</v>
       </c>
       <c r="L57" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="58" spans="1:12">
@@ -6688,7 +6698,7 @@
         <v>432</v>
       </c>
       <c r="L58" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="59" spans="1:12">
@@ -6712,7 +6722,7 @@
         <v>432</v>
       </c>
       <c r="L59" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="60" spans="1:12">
@@ -6736,7 +6746,7 @@
         <v>432</v>
       </c>
       <c r="L60" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="61" spans="1:12">
@@ -6770,7 +6780,7 @@
         <v>432</v>
       </c>
       <c r="L61" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="62" spans="1:12">
@@ -6802,7 +6812,7 @@
         <v>432</v>
       </c>
       <c r="L62" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="63" spans="1:12">
@@ -6826,7 +6836,7 @@
         <v>432</v>
       </c>
       <c r="L63" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="64" spans="1:12">
@@ -6857,7 +6867,7 @@
         <v>432</v>
       </c>
       <c r="L64" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="65" spans="1:12">
@@ -6889,7 +6899,7 @@
         <v>432</v>
       </c>
       <c r="L65" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="66" spans="1:12">
@@ -6919,7 +6929,7 @@
         <v>432</v>
       </c>
       <c r="L66" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="67" spans="1:12">
@@ -6943,7 +6953,7 @@
         <v>432</v>
       </c>
       <c r="L67" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="68" spans="1:12">
@@ -6975,7 +6985,7 @@
         <v>432</v>
       </c>
       <c r="L68" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="69" spans="1:12">
@@ -6999,7 +7009,7 @@
         <v>432</v>
       </c>
       <c r="L69" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="70" spans="1:12">
@@ -7031,7 +7041,7 @@
         <v>432</v>
       </c>
       <c r="L70" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="72" spans="1:12">
@@ -7815,26 +7825,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L109"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="4" topLeftCell="F1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="K80" sqref="K80"/>
+      <selection pane="topRight" activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12"/>
   <cols>
-    <col min="1" max="1" width="38.5546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.109375" style="36" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.88671875" style="36" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.5546875" style="36" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="36" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" style="36" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.5703125" style="36" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="29" style="37" customWidth="1"/>
-    <col min="6" max="6" width="21.6640625" style="37" customWidth="1"/>
-    <col min="7" max="7" width="32.6640625" style="36" customWidth="1"/>
-    <col min="8" max="8" width="36.33203125" style="140" customWidth="1"/>
-    <col min="9" max="9" width="29.5546875" style="9" customWidth="1"/>
-    <col min="10" max="10" width="27.5546875" style="36" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="28.88671875" style="74" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="30.44140625" style="74" customWidth="1"/>
-    <col min="13" max="16384" width="9.109375" style="9"/>
+    <col min="6" max="6" width="21.7109375" style="37" customWidth="1"/>
+    <col min="7" max="7" width="32.7109375" style="36" customWidth="1"/>
+    <col min="8" max="8" width="36.28515625" style="140" customWidth="1"/>
+    <col min="9" max="9" width="29.5703125" style="9" customWidth="1"/>
+    <col min="10" max="10" width="27.5703125" style="36" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="28.85546875" style="74" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="30.42578125" style="74" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -7924,7 +7934,7 @@
       </c>
       <c r="K3" s="80"/>
       <c r="L3" s="80" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="36.75" customHeight="1">
@@ -7946,7 +7956,9 @@
       <c r="F4" s="186" t="s">
         <v>153</v>
       </c>
-      <c r="G4" s="8"/>
+      <c r="G4" s="190" t="s">
+        <v>1015</v>
+      </c>
       <c r="H4" s="186"/>
       <c r="I4" s="109"/>
       <c r="J4" s="191" t="s">
@@ -7954,7 +7966,7 @@
       </c>
       <c r="K4" s="191"/>
       <c r="L4" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="45.75" customHeight="1">
@@ -7984,10 +7996,10 @@
       </c>
       <c r="K5" s="80"/>
       <c r="L5" s="80" t="s">
-        <v>1006</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="48">
+        <v>1005</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="60">
       <c r="A6" s="23" t="s">
         <v>176</v>
       </c>
@@ -8048,7 +8060,7 @@
       </c>
       <c r="K7" s="191"/>
       <c r="L7" s="191" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -8076,7 +8088,7 @@
       </c>
       <c r="K8" s="191"/>
       <c r="L8" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="45.75" customHeight="1">
@@ -8108,7 +8120,7 @@
       </c>
       <c r="K9" s="80"/>
       <c r="L9" s="80" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="27.75" customHeight="1">
@@ -8136,7 +8148,7 @@
       </c>
       <c r="K10" s="80"/>
       <c r="L10" s="80" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="74.25" customHeight="1">
@@ -8165,7 +8177,7 @@
       </c>
       <c r="K11" s="80"/>
       <c r="L11" s="80" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="12" spans="1:12" s="73" customFormat="1">
@@ -8215,7 +8227,7 @@
       </c>
       <c r="K13" s="80"/>
       <c r="L13" s="80" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -8245,7 +8257,7 @@
       </c>
       <c r="K14" s="191"/>
       <c r="L14" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="40.5" customHeight="1">
@@ -8277,7 +8289,7 @@
       </c>
       <c r="K15" s="80"/>
       <c r="L15" s="80" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="16" spans="1:12" s="73" customFormat="1">
@@ -8320,7 +8332,7 @@
       <c r="K17" s="80"/>
       <c r="L17" s="80"/>
     </row>
-    <row r="18" spans="1:12" s="73" customFormat="1" ht="48">
+    <row r="18" spans="1:12" s="73" customFormat="1" ht="60">
       <c r="A18" s="89" t="s">
         <v>175</v>
       </c>
@@ -8349,10 +8361,10 @@
       </c>
       <c r="K18" s="80"/>
       <c r="L18" s="80" t="s">
-        <v>1005</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" s="73" customFormat="1">
+        <v>1004</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" s="73" customFormat="1" ht="24">
       <c r="A19" s="89" t="s">
         <v>208</v>
       </c>
@@ -8382,7 +8394,7 @@
       </c>
       <c r="K19" s="80"/>
       <c r="L19" s="80" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="20" spans="1:12" s="73" customFormat="1" ht="24">
@@ -8434,7 +8446,7 @@
       </c>
       <c r="K21" s="80"/>
       <c r="L21" s="80" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="22" spans="1:12" s="73" customFormat="1" ht="24">
@@ -8466,7 +8478,7 @@
       </c>
       <c r="K22" s="80"/>
       <c r="L22" s="80" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="23" spans="1:12" s="73" customFormat="1">
@@ -8494,7 +8506,7 @@
       </c>
       <c r="K23" s="80"/>
       <c r="L23" s="80" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="24" spans="1:12" s="73" customFormat="1">
@@ -8566,10 +8578,10 @@
       </c>
       <c r="K26" s="80"/>
       <c r="L26" s="80" t="s">
-        <v>1005</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" s="73" customFormat="1">
+        <v>1004</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" s="73" customFormat="1" ht="24">
       <c r="A27" s="153" t="s">
         <v>938</v>
       </c>
@@ -8596,7 +8608,7 @@
       </c>
       <c r="K27" s="191"/>
       <c r="L27" s="191" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="28" spans="1:12" s="73" customFormat="1" ht="36">
@@ -8610,7 +8622,7 @@
         <v>171</v>
       </c>
       <c r="D28" s="186">
-        <v>8.2000000000000003E-2</v>
+        <v>0.24</v>
       </c>
       <c r="E28" s="186" t="s">
         <v>96</v>
@@ -8618,9 +8630,8 @@
       <c r="F28" s="186" t="s">
         <v>943</v>
       </c>
-      <c r="G28" s="186"/>
-      <c r="H28" s="186" t="s">
-        <v>944</v>
+      <c r="G28" s="186" t="s">
+        <v>1016</v>
       </c>
       <c r="I28" s="108"/>
       <c r="J28" s="191" t="s">
@@ -8628,7 +8639,7 @@
       </c>
       <c r="K28" s="191"/>
       <c r="L28" s="191" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="29" spans="1:12" s="73" customFormat="1" ht="48">
@@ -8662,7 +8673,7 @@
       </c>
       <c r="K29" s="80"/>
       <c r="L29" s="80" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="30" spans="1:12" s="73" customFormat="1" ht="24" customHeight="1">
@@ -8694,7 +8705,7 @@
       </c>
       <c r="K30" s="80"/>
       <c r="L30" s="80" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="31" spans="1:12" ht="44.25" customHeight="1">
@@ -8726,7 +8737,7 @@
       </c>
       <c r="K31" s="80"/>
       <c r="L31" s="80" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="32" spans="1:12" s="73" customFormat="1">
@@ -8794,7 +8805,7 @@
       </c>
       <c r="K33" s="80"/>
       <c r="L33" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="34" spans="1:12" ht="36">
@@ -8824,7 +8835,7 @@
       </c>
       <c r="K34" s="80"/>
       <c r="L34" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="35" spans="1:12">
@@ -8852,7 +8863,7 @@
       </c>
       <c r="K35" s="80"/>
       <c r="L35" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="36" spans="1:12">
@@ -8880,12 +8891,12 @@
       </c>
       <c r="K36" s="80"/>
       <c r="L36" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="37" spans="1:12">
       <c r="A37" s="153" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="B37" s="175" t="s">
         <v>5</v>
@@ -8897,7 +8908,7 @@
         <v>40</v>
       </c>
       <c r="E37" s="175" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
       <c r="F37" s="175">
         <v>409</v>
@@ -8910,7 +8921,7 @@
       </c>
       <c r="K37" s="191"/>
       <c r="L37" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="38" spans="1:12">
@@ -8940,7 +8951,7 @@
       </c>
       <c r="K38" s="80"/>
       <c r="L38" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="39" spans="1:12">
@@ -8968,7 +8979,7 @@
       </c>
       <c r="K39" s="80"/>
       <c r="L39" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="40" spans="1:12">
@@ -8996,7 +9007,7 @@
       </c>
       <c r="K40" s="80"/>
       <c r="L40" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="41" spans="1:12">
@@ -9024,7 +9035,7 @@
       </c>
       <c r="K41" s="80"/>
       <c r="L41" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="42" spans="1:12">
@@ -9052,7 +9063,7 @@
       </c>
       <c r="K42" s="80"/>
       <c r="L42" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="43" spans="1:12">
@@ -9080,7 +9091,7 @@
       </c>
       <c r="K43" s="80"/>
       <c r="L43" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="44" spans="1:12" ht="24">
@@ -9110,7 +9121,7 @@
       </c>
       <c r="K44" s="80"/>
       <c r="L44" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="45" spans="1:12">
@@ -9138,10 +9149,10 @@
       </c>
       <c r="K45" s="80"/>
       <c r="L45" s="191" t="s">
-        <v>1005</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" ht="24">
+        <v>1004</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" ht="36">
       <c r="A46" s="89" t="s">
         <v>646</v>
       </c>
@@ -9168,12 +9179,12 @@
       </c>
       <c r="K46" s="80"/>
       <c r="L46" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="47" spans="1:12">
       <c r="A47" s="153" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="B47" s="175" t="s">
         <v>553</v>
@@ -9185,12 +9196,12 @@
         <v>1.23</v>
       </c>
       <c r="E47" s="175" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="F47" s="175"/>
       <c r="G47" s="176"/>
       <c r="H47" s="179" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="I47" s="109"/>
       <c r="J47" s="191" t="s">
@@ -9224,7 +9235,7 @@
       </c>
       <c r="K48" s="80"/>
       <c r="L48" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="49" spans="1:12">
@@ -9252,7 +9263,7 @@
       </c>
       <c r="K49" s="80"/>
       <c r="L49" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="50" spans="1:12">
@@ -9280,7 +9291,7 @@
       </c>
       <c r="K50" s="80"/>
       <c r="L50" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="51" spans="1:12" ht="48">
@@ -9312,7 +9323,7 @@
       </c>
       <c r="K51" s="80"/>
       <c r="L51" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="52" spans="1:12">
@@ -9340,7 +9351,7 @@
       </c>
       <c r="K52" s="80"/>
       <c r="L52" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="53" spans="1:12" ht="24">
@@ -9370,7 +9381,7 @@
       </c>
       <c r="K53" s="80"/>
       <c r="L53" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="54" spans="1:12" ht="24">
@@ -9400,10 +9411,10 @@
       </c>
       <c r="K54" s="80"/>
       <c r="L54" s="191" t="s">
-        <v>1005</v>
-      </c>
-    </row>
-    <row r="55" spans="1:12" ht="24">
+        <v>1004</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" ht="36">
       <c r="A55" s="89" t="s">
         <v>649</v>
       </c>
@@ -9430,12 +9441,12 @@
       </c>
       <c r="K55" s="80"/>
       <c r="L55" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="56" spans="1:12">
       <c r="A56" s="153" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="B56" s="175" t="s">
         <v>553</v>
@@ -9447,12 +9458,12 @@
         <v>2.5299999999999998</v>
       </c>
       <c r="E56" s="175" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F56" s="175"/>
       <c r="G56" s="176"/>
       <c r="H56" s="179" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="I56" s="109"/>
       <c r="J56" s="191" t="s">
@@ -9461,7 +9472,7 @@
       <c r="K56" s="191"/>
       <c r="L56" s="191"/>
     </row>
-    <row r="57" spans="1:12">
+    <row r="57" spans="1:12" ht="24">
       <c r="A57" s="89" t="s">
         <v>670</v>
       </c>
@@ -9488,7 +9499,7 @@
       </c>
       <c r="K57" s="80"/>
       <c r="L57" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="58" spans="1:12">
@@ -9516,10 +9527,10 @@
       </c>
       <c r="K58" s="80"/>
       <c r="L58" s="191" t="s">
-        <v>1005</v>
-      </c>
-    </row>
-    <row r="59" spans="1:12">
+        <v>1004</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" ht="24">
       <c r="A59" s="89" t="s">
         <v>672</v>
       </c>
@@ -9546,7 +9557,7 @@
       </c>
       <c r="K59" s="80"/>
       <c r="L59" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="60" spans="1:12">
@@ -9574,10 +9585,10 @@
       </c>
       <c r="K60" s="80"/>
       <c r="L60" s="191" t="s">
-        <v>1005</v>
-      </c>
-    </row>
-    <row r="61" spans="1:12">
+        <v>1004</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" ht="24">
       <c r="A61" s="89" t="s">
         <v>674</v>
       </c>
@@ -9604,7 +9615,7 @@
       </c>
       <c r="K61" s="80"/>
       <c r="L61" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="62" spans="1:12">
@@ -9632,10 +9643,10 @@
       </c>
       <c r="K62" s="80"/>
       <c r="L62" s="191" t="s">
-        <v>1005</v>
-      </c>
-    </row>
-    <row r="63" spans="1:12">
+        <v>1004</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" ht="24">
       <c r="A63" s="89" t="s">
         <v>650</v>
       </c>
@@ -9662,7 +9673,7 @@
       </c>
       <c r="K63" s="80"/>
       <c r="L63" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="64" spans="1:12">
@@ -9694,7 +9705,7 @@
       </c>
       <c r="K64" s="80"/>
       <c r="L64" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="65" spans="1:12">
@@ -9724,7 +9735,7 @@
       </c>
       <c r="K65" s="80"/>
       <c r="L65" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="66" spans="1:12">
@@ -9752,7 +9763,7 @@
       </c>
       <c r="K66" s="80"/>
       <c r="L66" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="67" spans="1:12">
@@ -9782,7 +9793,7 @@
       </c>
       <c r="K67" s="80"/>
       <c r="L67" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="68" spans="1:12">
@@ -9810,10 +9821,10 @@
       </c>
       <c r="K68" s="80"/>
       <c r="L68" s="191" t="s">
-        <v>1005</v>
-      </c>
-    </row>
-    <row r="69" spans="1:12">
+        <v>1004</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" ht="24">
       <c r="A69" s="89" t="s">
         <v>676</v>
       </c>
@@ -9840,7 +9851,7 @@
       </c>
       <c r="K69" s="80"/>
       <c r="L69" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="70" spans="1:12">
@@ -9868,7 +9879,7 @@
       </c>
       <c r="K70" s="80"/>
       <c r="L70" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="71" spans="1:12">
@@ -9898,7 +9909,7 @@
       </c>
       <c r="K71" s="80"/>
       <c r="L71" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="72" spans="1:12">
@@ -9928,10 +9939,10 @@
       </c>
       <c r="K72" s="80"/>
       <c r="L72" s="191" t="s">
-        <v>1005</v>
-      </c>
-    </row>
-    <row r="73" spans="1:12">
+        <v>1004</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" ht="24">
       <c r="A73" s="89" t="s">
         <v>679</v>
       </c>
@@ -9958,7 +9969,7 @@
       </c>
       <c r="K73" s="80"/>
       <c r="L73" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="74" spans="1:12">
@@ -9986,7 +9997,7 @@
       </c>
       <c r="K74" s="80"/>
       <c r="L74" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="75" spans="1:12">
@@ -10018,10 +10029,10 @@
       </c>
       <c r="K75" s="80"/>
       <c r="L75" s="191" t="s">
-        <v>1005</v>
-      </c>
-    </row>
-    <row r="76" spans="1:12">
+        <v>1004</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" ht="24">
       <c r="A76" s="89" t="s">
         <v>682</v>
       </c>
@@ -10048,7 +10059,7 @@
       </c>
       <c r="K76" s="80"/>
       <c r="L76" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="77" spans="1:12">
@@ -10076,7 +10087,7 @@
       </c>
       <c r="K77" s="80"/>
       <c r="L77" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="78" spans="1:12" ht="36">
@@ -10108,10 +10119,10 @@
       </c>
       <c r="K78" s="80"/>
       <c r="L78" s="191" t="s">
-        <v>1005</v>
-      </c>
-    </row>
-    <row r="79" spans="1:12" ht="24">
+        <v>1004</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" ht="36">
       <c r="A79" s="89" t="s">
         <v>656</v>
       </c>
@@ -10138,12 +10149,12 @@
       </c>
       <c r="K79" s="80"/>
       <c r="L79" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="80" spans="1:12">
       <c r="A80" s="153" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="B80" s="175" t="s">
         <v>553</v>
@@ -10155,12 +10166,12 @@
         <v>1.23</v>
       </c>
       <c r="E80" s="175" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="F80" s="175"/>
       <c r="G80" s="176"/>
       <c r="H80" s="179" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="I80" s="109"/>
       <c r="J80" s="191" t="s">
@@ -10169,7 +10180,7 @@
       <c r="K80" s="191"/>
       <c r="L80" s="191"/>
     </row>
-    <row r="81" spans="1:12" ht="48">
+    <row r="81" spans="1:12" ht="60">
       <c r="A81" s="89" t="s">
         <v>685</v>
       </c>
@@ -10196,7 +10207,7 @@
       </c>
       <c r="K81" s="80"/>
       <c r="L81" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="82" spans="1:12" ht="24">
@@ -10224,7 +10235,7 @@
       </c>
       <c r="K82" s="80"/>
       <c r="L82" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="83" spans="1:12" ht="36">
@@ -10254,7 +10265,7 @@
       </c>
       <c r="K83" s="80"/>
       <c r="L83" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="84" spans="1:12">
@@ -10282,7 +10293,7 @@
       </c>
       <c r="K84" s="80"/>
       <c r="L84" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="85" spans="1:12">
@@ -10310,7 +10321,7 @@
       </c>
       <c r="K85" s="80"/>
       <c r="L85" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="86" spans="1:12" ht="24">
@@ -10340,7 +10351,7 @@
       </c>
       <c r="K86" s="80"/>
       <c r="L86" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="87" spans="1:12" ht="24">
@@ -10370,10 +10381,10 @@
       </c>
       <c r="K87" s="80"/>
       <c r="L87" s="191" t="s">
-        <v>1005</v>
-      </c>
-    </row>
-    <row r="88" spans="1:12" ht="24">
+        <v>1004</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12" ht="36">
       <c r="A88" s="89" t="s">
         <v>659</v>
       </c>
@@ -10400,12 +10411,12 @@
       </c>
       <c r="K88" s="80"/>
       <c r="L88" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="89" spans="1:12">
       <c r="A89" s="153" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="B89" s="175" t="s">
         <v>553</v>
@@ -10417,12 +10428,12 @@
         <v>2.5299999999999998</v>
       </c>
       <c r="E89" s="175" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F89" s="175"/>
       <c r="G89" s="176"/>
       <c r="H89" s="179" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="I89" s="109"/>
       <c r="J89" s="191" t="s">
@@ -10431,7 +10442,7 @@
       <c r="K89" s="191"/>
       <c r="L89" s="191"/>
     </row>
-    <row r="90" spans="1:12">
+    <row r="90" spans="1:12" ht="24">
       <c r="A90" s="89" t="s">
         <v>688</v>
       </c>
@@ -10458,7 +10469,7 @@
       </c>
       <c r="K90" s="80"/>
       <c r="L90" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="91" spans="1:12">
@@ -10486,10 +10497,10 @@
       </c>
       <c r="K91" s="80"/>
       <c r="L91" s="191" t="s">
-        <v>1005</v>
-      </c>
-    </row>
-    <row r="92" spans="1:12">
+        <v>1004</v>
+      </c>
+    </row>
+    <row r="92" spans="1:12" ht="24">
       <c r="A92" s="89" t="s">
         <v>690</v>
       </c>
@@ -10516,7 +10527,7 @@
       </c>
       <c r="K92" s="80"/>
       <c r="L92" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="93" spans="1:12">
@@ -10544,10 +10555,10 @@
       </c>
       <c r="K93" s="80"/>
       <c r="L93" s="191" t="s">
-        <v>1005</v>
-      </c>
-    </row>
-    <row r="94" spans="1:12">
+        <v>1004</v>
+      </c>
+    </row>
+    <row r="94" spans="1:12" ht="24">
       <c r="A94" s="89" t="s">
         <v>692</v>
       </c>
@@ -10574,7 +10585,7 @@
       </c>
       <c r="K94" s="80"/>
       <c r="L94" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="95" spans="1:12">
@@ -10602,10 +10613,10 @@
       </c>
       <c r="K95" s="80"/>
       <c r="L95" s="191" t="s">
-        <v>1005</v>
-      </c>
-    </row>
-    <row r="96" spans="1:12">
+        <v>1004</v>
+      </c>
+    </row>
+    <row r="96" spans="1:12" ht="24">
       <c r="A96" s="89" t="s">
         <v>660</v>
       </c>
@@ -10632,7 +10643,7 @@
       </c>
       <c r="K96" s="80"/>
       <c r="L96" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="97" spans="1:12">
@@ -10660,7 +10671,7 @@
       </c>
       <c r="K97" s="80"/>
       <c r="L97" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="98" spans="1:12">
@@ -10688,7 +10699,7 @@
       </c>
       <c r="K98" s="80"/>
       <c r="L98" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="99" spans="1:12">
@@ -10716,7 +10727,7 @@
       </c>
       <c r="K99" s="80"/>
       <c r="L99" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="100" spans="1:12">
@@ -10744,7 +10755,7 @@
       </c>
       <c r="K100" s="80"/>
       <c r="L100" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="101" spans="1:12">
@@ -10774,7 +10785,7 @@
       </c>
       <c r="K101" s="80"/>
       <c r="L101" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="102" spans="1:12">
@@ -10802,7 +10813,7 @@
       </c>
       <c r="K102" s="80"/>
       <c r="L102" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="103" spans="1:12">
@@ -10830,10 +10841,10 @@
       </c>
       <c r="K103" s="80"/>
       <c r="L103" s="191" t="s">
-        <v>1005</v>
-      </c>
-    </row>
-    <row r="104" spans="1:12">
+        <v>1004</v>
+      </c>
+    </row>
+    <row r="104" spans="1:12" ht="24">
       <c r="A104" s="89" t="s">
         <v>668</v>
       </c>
@@ -10860,7 +10871,7 @@
       </c>
       <c r="K104" s="80"/>
       <c r="L104" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="105" spans="1:12">
@@ -10888,7 +10899,7 @@
       </c>
       <c r="K105" s="80"/>
       <c r="L105" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="106" spans="1:12">
@@ -10920,20 +10931,20 @@
       <selection pane="bottomRight" activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" style="73" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.88671875" style="73" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.5546875" style="27" customWidth="1"/>
-    <col min="4" max="4" width="9.109375" style="27"/>
-    <col min="5" max="6" width="17.33203125" style="73" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.33203125" style="73" customWidth="1"/>
-    <col min="8" max="8" width="29.6640625" style="73" customWidth="1"/>
-    <col min="9" max="9" width="21.44140625" style="73" customWidth="1"/>
-    <col min="10" max="10" width="18.33203125" style="73" customWidth="1"/>
-    <col min="11" max="11" width="28.88671875" style="73" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="30.44140625" style="73" customWidth="1"/>
-    <col min="13" max="16384" width="9.109375" style="73"/>
+    <col min="1" max="1" width="20.7109375" style="73" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" style="73" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" style="27" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="27"/>
+    <col min="5" max="6" width="17.28515625" style="73" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.28515625" style="73" customWidth="1"/>
+    <col min="8" max="8" width="29.7109375" style="73" customWidth="1"/>
+    <col min="9" max="9" width="21.42578125" style="73" customWidth="1"/>
+    <col min="10" max="10" width="18.28515625" style="73" customWidth="1"/>
+    <col min="11" max="11" width="28.85546875" style="73" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="30.42578125" style="73" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="73"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="24">
@@ -10974,7 +10985,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="60">
+    <row r="2" spans="1:12" ht="72">
       <c r="A2" s="50" t="s">
         <v>178</v>
       </c>
@@ -11001,7 +11012,7 @@
       </c>
       <c r="K2" s="191"/>
       <c r="L2" s="191" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
     </row>
   </sheetData>
@@ -11018,19 +11029,19 @@
       <selection pane="topRight" activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="29.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.88671875" customWidth="1"/>
-    <col min="3" max="3" width="16.6640625" customWidth="1"/>
-    <col min="4" max="4" width="14.44140625" customWidth="1"/>
-    <col min="5" max="5" width="23.5546875" customWidth="1"/>
-    <col min="6" max="7" width="23.5546875" style="15" customWidth="1"/>
-    <col min="8" max="8" width="22.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="46.109375" customWidth="1"/>
-    <col min="10" max="10" width="9.109375" style="13"/>
-    <col min="11" max="11" width="28.88671875" style="73" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="30.44140625" style="73" customWidth="1"/>
+    <col min="1" max="1" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" customWidth="1"/>
+    <col min="5" max="5" width="23.5703125" customWidth="1"/>
+    <col min="6" max="7" width="23.5703125" style="15" customWidth="1"/>
+    <col min="8" max="8" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="46.140625" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" style="13"/>
+    <col min="11" max="11" width="28.85546875" style="73" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="30.42578125" style="73" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16384">
@@ -11115,7 +11126,7 @@
       </c>
       <c r="K3" s="80"/>
       <c r="L3" s="80" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="4" spans="1:16384">
@@ -11145,7 +11156,7 @@
       </c>
       <c r="K4" s="80"/>
       <c r="L4" s="80" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="5" spans="1:16384" s="81" customFormat="1">
@@ -27583,7 +27594,7 @@
       </c>
       <c r="K7" s="80"/>
       <c r="L7" s="80" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="8" spans="1:16384">
@@ -27611,7 +27622,7 @@
       </c>
       <c r="K8" s="80"/>
       <c r="L8" s="80" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="9" spans="1:16384">
@@ -27639,7 +27650,7 @@
       </c>
       <c r="K9" s="80"/>
       <c r="L9" s="80" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="10" spans="1:16384" s="15" customFormat="1">
@@ -27689,7 +27700,7 @@
       </c>
       <c r="K11" s="80"/>
       <c r="L11" s="80" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="12" spans="1:16384" s="81" customFormat="1" ht="24">
@@ -27729,21 +27740,21 @@
       <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12"/>
   <cols>
-    <col min="1" max="1" width="26.44140625" style="73" customWidth="1"/>
-    <col min="2" max="2" width="17.6640625" style="73" customWidth="1"/>
-    <col min="3" max="3" width="16.5546875" style="73" customWidth="1"/>
-    <col min="4" max="4" width="15.33203125" style="73" customWidth="1"/>
-    <col min="5" max="5" width="31.44140625" style="73" customWidth="1"/>
+    <col min="1" max="1" width="26.42578125" style="73" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" style="73" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" style="73" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" style="73" customWidth="1"/>
+    <col min="5" max="5" width="31.42578125" style="73" customWidth="1"/>
     <col min="6" max="6" width="12" style="73" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.109375" style="73" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="44.6640625" style="110" customWidth="1"/>
-    <col min="9" max="9" width="6.6640625" style="73" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.33203125" style="27" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="28.88671875" style="73" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="30.44140625" style="73" customWidth="1"/>
-    <col min="13" max="16384" width="9.109375" style="73"/>
+    <col min="7" max="7" width="5.140625" style="73" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="44.7109375" style="110" customWidth="1"/>
+    <col min="9" max="9" width="6.7109375" style="73" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.28515625" style="27" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="28.85546875" style="73" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="30.42578125" style="73" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="73"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -27786,7 +27797,7 @@
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="49" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="B2" s="86" t="s">
         <v>6</v>
@@ -27811,7 +27822,7 @@
       </c>
       <c r="K2" s="80"/>
       <c r="L2" s="80" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
   </sheetData>
@@ -27827,18 +27838,18 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12"/>
   <cols>
-    <col min="1" max="1" width="28.33203125" style="27" customWidth="1"/>
-    <col min="2" max="2" width="9.88671875" style="27" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.28515625" style="27" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" style="27" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20" style="27" customWidth="1"/>
-    <col min="4" max="4" width="9.109375" style="27"/>
-    <col min="5" max="6" width="17.33203125" style="27" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="14.6640625" style="27" customWidth="1"/>
-    <col min="9" max="10" width="9.109375" style="27"/>
-    <col min="11" max="11" width="28.88671875" style="73" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="30.44140625" style="73" customWidth="1"/>
-    <col min="13" max="16384" width="9.109375" style="27"/>
+    <col min="4" max="4" width="9.140625" style="27"/>
+    <col min="5" max="6" width="17.28515625" style="27" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="14.7109375" style="27" customWidth="1"/>
+    <col min="9" max="10" width="9.140625" style="27"/>
+    <col min="11" max="11" width="28.85546875" style="73" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="30.42578125" style="73" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="27"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="24">
@@ -27945,7 +27956,7 @@
     </row>
     <row r="6" spans="1:12">
       <c r="A6" s="30" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="B6" s="14"/>
       <c r="C6" s="14"/>
@@ -27961,7 +27972,7 @@
     </row>
     <row r="7" spans="1:12">
       <c r="A7" s="30" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="B7" s="14"/>
       <c r="C7" s="14"/>
@@ -27989,21 +28000,21 @@
       <selection pane="topRight" activeCell="I118" sqref="I118"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12"/>
   <cols>
-    <col min="1" max="1" width="38.44140625" style="9" customWidth="1"/>
-    <col min="2" max="2" width="14.88671875" style="9" customWidth="1"/>
-    <col min="3" max="3" width="17.44140625" style="9" customWidth="1"/>
-    <col min="4" max="4" width="19.6640625" style="111" customWidth="1"/>
-    <col min="5" max="5" width="24.5546875" style="111" customWidth="1"/>
-    <col min="6" max="6" width="28.5546875" style="73" customWidth="1"/>
+    <col min="1" max="1" width="38.42578125" style="9" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" style="9" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" style="9" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" style="111" customWidth="1"/>
+    <col min="5" max="5" width="24.5703125" style="111" customWidth="1"/>
+    <col min="6" max="6" width="28.5703125" style="73" customWidth="1"/>
     <col min="7" max="7" width="40" style="73" customWidth="1"/>
-    <col min="8" max="8" width="41.88671875" style="73" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="51.109375" style="73" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.44140625" style="74" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="28.88671875" style="73" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="30.44140625" style="73" customWidth="1"/>
-    <col min="13" max="16384" width="9.109375" style="73"/>
+    <col min="8" max="8" width="41.85546875" style="73" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="51.140625" style="73" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.42578125" style="74" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="28.85546875" style="73" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="30.42578125" style="73" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="73"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -28071,7 +28082,7 @@
       </c>
       <c r="K2" s="80"/>
       <c r="L2" s="80" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -28101,7 +28112,7 @@
       </c>
       <c r="K3" s="80"/>
       <c r="L3" s="80" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="24">
@@ -28131,7 +28142,7 @@
       </c>
       <c r="K4" s="80"/>
       <c r="L4" s="80" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -28163,10 +28174,10 @@
       </c>
       <c r="K5" s="80"/>
       <c r="L5" s="80" t="s">
-        <v>1005</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12">
+        <v>1004</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="24">
       <c r="A6" s="89" t="s">
         <v>357</v>
       </c>
@@ -28195,7 +28206,7 @@
       </c>
       <c r="K6" s="80"/>
       <c r="L6" s="80" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="24">
@@ -28254,7 +28265,7 @@
       </c>
       <c r="K8" s="80"/>
       <c r="L8" s="80" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -28284,7 +28295,7 @@
       </c>
       <c r="K9" s="80"/>
       <c r="L9" s="80" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -28314,7 +28325,7 @@
       </c>
       <c r="K10" s="80"/>
       <c r="L10" s="80" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="24">
@@ -28342,7 +28353,7 @@
       </c>
       <c r="K11" s="80"/>
       <c r="L11" s="80" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -28390,7 +28401,7 @@
       </c>
       <c r="K13" s="80"/>
       <c r="L13" s="80" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -28422,7 +28433,7 @@
       </c>
       <c r="K14" s="127"/>
       <c r="L14" s="80" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -28452,7 +28463,7 @@
       </c>
       <c r="K15" s="80"/>
       <c r="L15" s="80" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -28482,10 +28493,10 @@
       </c>
       <c r="K16" s="80"/>
       <c r="L16" s="80" t="s">
-        <v>1005</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12">
+        <v>1004</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="24">
       <c r="A17" s="94" t="s">
         <v>459</v>
       </c>
@@ -28514,7 +28525,7 @@
       </c>
       <c r="K17" s="127"/>
       <c r="L17" s="80" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="18" spans="1:12">
@@ -28544,7 +28555,7 @@
       </c>
       <c r="K18" s="80"/>
       <c r="L18" s="80" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="19" spans="1:12">
@@ -28574,7 +28585,7 @@
       </c>
       <c r="K19" s="80"/>
       <c r="L19" s="80" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="20" spans="1:12">
@@ -28604,7 +28615,7 @@
       </c>
       <c r="K20" s="80"/>
       <c r="L20" s="80" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="21" spans="1:12">
@@ -28636,7 +28647,7 @@
       </c>
       <c r="K21" s="80"/>
       <c r="L21" s="80" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="22" spans="1:12">
@@ -28668,7 +28679,7 @@
       </c>
       <c r="K22" s="80"/>
       <c r="L22" s="80" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="36">
@@ -28700,10 +28711,10 @@
       </c>
       <c r="K23" s="80"/>
       <c r="L23" s="80" t="s">
-        <v>1006</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12">
+        <v>1005</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="24">
       <c r="A24" s="23" t="s">
         <v>351</v>
       </c>
@@ -28758,7 +28769,7 @@
       </c>
       <c r="K25" s="80"/>
       <c r="L25" s="80" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="26" spans="1:12">
@@ -28788,7 +28799,7 @@
       </c>
       <c r="K26" s="80"/>
       <c r="L26" s="80" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="27" spans="1:12">
@@ -28818,7 +28829,7 @@
       </c>
       <c r="K27" s="80"/>
       <c r="L27" s="80" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="28" spans="1:12" ht="12" customHeight="1">
@@ -28848,7 +28859,7 @@
       </c>
       <c r="K28" s="80"/>
       <c r="L28" s="80" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="29" spans="1:12">
@@ -28880,7 +28891,7 @@
       </c>
       <c r="K29" s="80"/>
       <c r="L29" s="80" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="30" spans="1:12">
@@ -28912,7 +28923,7 @@
       </c>
       <c r="K30" s="80"/>
       <c r="L30" s="80" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="31" spans="1:12">
@@ -28943,7 +28954,7 @@
       <c r="K31" s="80"/>
       <c r="L31" s="80"/>
     </row>
-    <row r="32" spans="1:12">
+    <row r="32" spans="1:12" ht="24">
       <c r="A32" s="23" t="s">
         <v>354</v>
       </c>
@@ -29026,7 +29037,7 @@
       </c>
       <c r="K34" s="80"/>
       <c r="L34" s="80" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="35" spans="1:12">
@@ -29058,7 +29069,7 @@
       </c>
       <c r="K35" s="80"/>
       <c r="L35" s="191" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="36" spans="1:12">
@@ -29088,7 +29099,7 @@
       </c>
       <c r="K36" s="80"/>
       <c r="L36" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="37" spans="1:12">
@@ -29118,10 +29129,10 @@
       </c>
       <c r="K37" s="80"/>
       <c r="L37" s="191" t="s">
-        <v>1005</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12">
+        <v>1004</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" ht="24">
       <c r="A38" s="94" t="s">
         <v>461</v>
       </c>
@@ -29150,7 +29161,7 @@
       </c>
       <c r="K38" s="80"/>
       <c r="L38" s="191" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="39" spans="1:12">
@@ -29180,7 +29191,7 @@
       </c>
       <c r="K39" s="80"/>
       <c r="L39" s="191" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="40" spans="1:12">
@@ -29210,7 +29221,7 @@
       </c>
       <c r="K40" s="80"/>
       <c r="L40" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="41" spans="1:12">
@@ -29240,7 +29251,7 @@
       </c>
       <c r="K41" s="80"/>
       <c r="L41" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="42" spans="1:12">
@@ -29272,7 +29283,7 @@
       </c>
       <c r="K42" s="80"/>
       <c r="L42" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="43" spans="1:12">
@@ -29304,7 +29315,7 @@
       </c>
       <c r="K43" s="80"/>
       <c r="L43" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="44" spans="1:12" ht="36">
@@ -29336,10 +29347,10 @@
       </c>
       <c r="K44" s="80"/>
       <c r="L44" s="191" t="s">
-        <v>1006</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12">
+        <v>1005</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" ht="24">
       <c r="A45" s="23" t="s">
         <v>350</v>
       </c>
@@ -29394,7 +29405,7 @@
       </c>
       <c r="K46" s="80"/>
       <c r="L46" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="47" spans="1:12">
@@ -29424,7 +29435,7 @@
       </c>
       <c r="K47" s="80"/>
       <c r="L47" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="48" spans="1:12">
@@ -29454,7 +29465,7 @@
       </c>
       <c r="K48" s="80"/>
       <c r="L48" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="49" spans="1:12" ht="12" customHeight="1">
@@ -29484,7 +29495,7 @@
       </c>
       <c r="K49" s="80"/>
       <c r="L49" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="50" spans="1:12">
@@ -29516,7 +29527,7 @@
       </c>
       <c r="K50" s="80"/>
       <c r="L50" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="51" spans="1:12">
@@ -29548,7 +29559,7 @@
       </c>
       <c r="K51" s="80"/>
       <c r="L51" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="52" spans="1:12">
@@ -29577,7 +29588,7 @@
       <c r="K52" s="80"/>
       <c r="L52" s="191"/>
     </row>
-    <row r="53" spans="1:12">
+    <row r="53" spans="1:12" ht="24">
       <c r="A53" s="23" t="s">
         <v>353</v>
       </c>
@@ -29660,7 +29671,7 @@
       </c>
       <c r="K55" s="80"/>
       <c r="L55" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="56" spans="1:12">
@@ -29730,10 +29741,10 @@
       </c>
       <c r="K57" s="80"/>
       <c r="L57" s="191" t="s">
-        <v>1005</v>
-      </c>
-    </row>
-    <row r="58" spans="1:12" ht="36">
+        <v>1004</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" ht="48">
       <c r="A58" s="89" t="s">
         <v>743</v>
       </c>
@@ -29760,10 +29771,10 @@
       </c>
       <c r="K58" s="80"/>
       <c r="L58" s="191" t="s">
-        <v>1005</v>
-      </c>
-    </row>
-    <row r="59" spans="1:12" ht="36">
+        <v>1004</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" ht="48">
       <c r="A59" s="89" t="s">
         <v>744</v>
       </c>
@@ -29790,10 +29801,10 @@
       </c>
       <c r="K59" s="80"/>
       <c r="L59" s="191" t="s">
-        <v>1005</v>
-      </c>
-    </row>
-    <row r="60" spans="1:12" ht="36">
+        <v>1004</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" ht="48">
       <c r="A60" s="89" t="s">
         <v>745</v>
       </c>
@@ -29820,10 +29831,10 @@
       </c>
       <c r="K60" s="80"/>
       <c r="L60" s="191" t="s">
-        <v>1005</v>
-      </c>
-    </row>
-    <row r="61" spans="1:12" ht="36">
+        <v>1004</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" ht="48">
       <c r="A61" s="89" t="s">
         <v>746</v>
       </c>
@@ -29850,10 +29861,10 @@
       </c>
       <c r="K61" s="80"/>
       <c r="L61" s="191" t="s">
-        <v>1004</v>
-      </c>
-    </row>
-    <row r="62" spans="1:12" ht="36">
+        <v>1003</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" ht="48">
       <c r="A62" s="89" t="s">
         <v>747</v>
       </c>
@@ -29880,10 +29891,10 @@
       </c>
       <c r="K62" s="80"/>
       <c r="L62" s="191" t="s">
-        <v>1004</v>
-      </c>
-    </row>
-    <row r="63" spans="1:12" ht="36">
+        <v>1003</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" ht="48">
       <c r="A63" s="89" t="s">
         <v>748</v>
       </c>
@@ -29910,10 +29921,10 @@
       </c>
       <c r="K63" s="80"/>
       <c r="L63" s="191" t="s">
-        <v>1004</v>
-      </c>
-    </row>
-    <row r="64" spans="1:12" ht="36">
+        <v>1003</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" ht="48">
       <c r="A64" s="89" t="s">
         <v>732</v>
       </c>
@@ -29940,10 +29951,10 @@
       </c>
       <c r="K64" s="80"/>
       <c r="L64" s="191" t="s">
-        <v>1004</v>
-      </c>
-    </row>
-    <row r="65" spans="1:12" ht="36">
+        <v>1003</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" ht="48">
       <c r="A65" s="89" t="s">
         <v>733</v>
       </c>
@@ -29970,7 +29981,7 @@
       </c>
       <c r="K65" s="80"/>
       <c r="L65" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="66" spans="1:12" ht="36">
@@ -30002,7 +30013,7 @@
       </c>
       <c r="K66" s="80"/>
       <c r="L66" s="191" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="67" spans="1:12" ht="36">
@@ -30034,10 +30045,10 @@
       </c>
       <c r="K67" s="80"/>
       <c r="L67" s="191" t="s">
-        <v>1005</v>
-      </c>
-    </row>
-    <row r="68" spans="1:12" ht="36">
+        <v>1004</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" ht="48">
       <c r="A68" s="153" t="s">
         <v>750</v>
       </c>
@@ -30064,10 +30075,10 @@
       </c>
       <c r="K68" s="80"/>
       <c r="L68" s="191" t="s">
-        <v>1005</v>
-      </c>
-    </row>
-    <row r="69" spans="1:12" ht="36">
+        <v>1004</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" ht="48">
       <c r="A69" s="153" t="s">
         <v>751</v>
       </c>
@@ -30094,10 +30105,10 @@
       </c>
       <c r="K69" s="80"/>
       <c r="L69" s="191" t="s">
-        <v>1005</v>
-      </c>
-    </row>
-    <row r="70" spans="1:12" ht="36">
+        <v>1004</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" ht="48">
       <c r="A70" s="153" t="s">
         <v>752</v>
       </c>
@@ -30124,10 +30135,10 @@
       </c>
       <c r="K70" s="80"/>
       <c r="L70" s="191" t="s">
-        <v>1005</v>
-      </c>
-    </row>
-    <row r="71" spans="1:12" ht="36">
+        <v>1004</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" ht="48">
       <c r="A71" s="153" t="s">
         <v>753</v>
       </c>
@@ -30154,10 +30165,10 @@
       </c>
       <c r="K71" s="80"/>
       <c r="L71" s="191" t="s">
-        <v>1004</v>
-      </c>
-    </row>
-    <row r="72" spans="1:12" ht="36">
+        <v>1003</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" ht="48">
       <c r="A72" s="153" t="s">
         <v>754</v>
       </c>
@@ -30184,10 +30195,10 @@
       </c>
       <c r="K72" s="80"/>
       <c r="L72" s="191" t="s">
-        <v>1004</v>
-      </c>
-    </row>
-    <row r="73" spans="1:12" ht="36">
+        <v>1003</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" ht="48">
       <c r="A73" s="153" t="s">
         <v>755</v>
       </c>
@@ -30214,10 +30225,10 @@
       </c>
       <c r="K73" s="80"/>
       <c r="L73" s="191" t="s">
-        <v>1004</v>
-      </c>
-    </row>
-    <row r="74" spans="1:12" ht="36">
+        <v>1003</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" ht="48">
       <c r="A74" s="153" t="s">
         <v>735</v>
       </c>
@@ -30244,10 +30255,10 @@
       </c>
       <c r="K74" s="80"/>
       <c r="L74" s="191" t="s">
-        <v>1004</v>
-      </c>
-    </row>
-    <row r="75" spans="1:12" ht="36">
+        <v>1003</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" ht="48">
       <c r="A75" s="153" t="s">
         <v>736</v>
       </c>
@@ -30274,7 +30285,7 @@
       </c>
       <c r="K75" s="80"/>
       <c r="L75" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="76" spans="1:12" ht="36">
@@ -30304,7 +30315,7 @@
       </c>
       <c r="K76" s="80"/>
       <c r="L76" s="191" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="77" spans="1:12">
@@ -30336,7 +30347,7 @@
       </c>
       <c r="K77" s="80"/>
       <c r="L77" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="78" spans="1:12">
@@ -30368,7 +30379,7 @@
       </c>
       <c r="K78" s="80"/>
       <c r="L78" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="79" spans="1:12">
@@ -30400,7 +30411,7 @@
       </c>
       <c r="K79" s="80"/>
       <c r="L79" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="80" spans="1:12">
@@ -30432,7 +30443,7 @@
       </c>
       <c r="K80" s="80"/>
       <c r="L80" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="81" spans="1:12">
@@ -30464,7 +30475,7 @@
       </c>
       <c r="K81" s="80"/>
       <c r="L81" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="82" spans="1:12">
@@ -30495,7 +30506,7 @@
       </c>
       <c r="K82" s="80"/>
       <c r="L82" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="83" spans="1:12">
@@ -30527,7 +30538,7 @@
       </c>
       <c r="K83" s="80"/>
       <c r="L83" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="84" spans="1:12">
@@ -30557,7 +30568,7 @@
       </c>
       <c r="K84" s="80"/>
       <c r="L84" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="85" spans="1:12">
@@ -30589,7 +30600,7 @@
       </c>
       <c r="K85" s="80"/>
       <c r="L85" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="86" spans="1:12">
@@ -30621,7 +30632,7 @@
       </c>
       <c r="K86" s="80"/>
       <c r="L86" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="87" spans="1:12">
@@ -30653,7 +30664,7 @@
       </c>
       <c r="K87" s="80"/>
       <c r="L87" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="88" spans="1:12">
@@ -30685,7 +30696,7 @@
       </c>
       <c r="K88" s="80"/>
       <c r="L88" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="89" spans="1:12">
@@ -30717,7 +30728,7 @@
       </c>
       <c r="K89" s="80"/>
       <c r="L89" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="90" spans="1:12">
@@ -30749,7 +30760,7 @@
       </c>
       <c r="K90" s="80"/>
       <c r="L90" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="91" spans="1:12">
@@ -30781,7 +30792,7 @@
       </c>
       <c r="K91" s="80"/>
       <c r="L91" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="92" spans="1:12">
@@ -30811,7 +30822,7 @@
       </c>
       <c r="K92" s="80"/>
       <c r="L92" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="93" spans="1:12">
@@ -30843,7 +30854,7 @@
       </c>
       <c r="K93" s="80"/>
       <c r="L93" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="94" spans="1:12">
@@ -30873,7 +30884,7 @@
       </c>
       <c r="K94" s="80"/>
       <c r="L94" s="191" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="95" spans="1:12">
@@ -30905,7 +30916,7 @@
       </c>
       <c r="K95" s="80"/>
       <c r="L95" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="96" spans="1:12">
@@ -30935,7 +30946,7 @@
       </c>
       <c r="K96" s="80"/>
       <c r="L96" s="191" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="97" spans="1:12" ht="24">
@@ -30968,7 +30979,7 @@
       </c>
       <c r="K97" s="80"/>
       <c r="L97" s="191" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="98" spans="1:12" ht="24">
@@ -31000,7 +31011,7 @@
       </c>
       <c r="K98" s="80"/>
       <c r="L98" s="191" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="99" spans="1:12" ht="24">
@@ -31034,7 +31045,7 @@
       </c>
       <c r="K99" s="80"/>
       <c r="L99" s="191" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="100" spans="1:12" ht="24">
@@ -31066,7 +31077,7 @@
       </c>
       <c r="K100" s="80"/>
       <c r="L100" s="191" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="101" spans="1:12" ht="24">
@@ -31098,7 +31109,7 @@
       </c>
       <c r="K101" s="80"/>
       <c r="L101" s="191" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="102" spans="1:12" ht="36">
@@ -31130,7 +31141,7 @@
       </c>
       <c r="K102" s="80"/>
       <c r="L102" s="191" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="103" spans="1:12" ht="24">
@@ -31162,7 +31173,7 @@
       </c>
       <c r="K103" s="80"/>
       <c r="L103" s="191" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="104" spans="1:12" ht="24">
@@ -31194,7 +31205,7 @@
       </c>
       <c r="K104" s="80"/>
       <c r="L104" s="191" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="105" spans="1:12" ht="24">
@@ -31230,7 +31241,7 @@
       </c>
       <c r="K105" s="80"/>
       <c r="L105" s="191" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="106" spans="1:12" ht="24">
@@ -31262,7 +31273,7 @@
       </c>
       <c r="K106" s="80"/>
       <c r="L106" s="191" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="107" spans="1:12">
@@ -31292,7 +31303,7 @@
       </c>
       <c r="K107" s="80"/>
       <c r="L107" s="191" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="108" spans="1:12">
@@ -31333,9 +31344,9 @@
         <v>434</v>
       </c>
     </row>
-    <row r="109" spans="1:12" ht="24">
+    <row r="109" spans="1:12" ht="36">
       <c r="A109" s="89" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="B109" s="87" t="s">
         <v>58</v>
@@ -31362,12 +31373,12 @@
       </c>
       <c r="K109" s="80"/>
       <c r="L109" s="80" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="110" spans="1:12" ht="24">
       <c r="A110" s="89" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="B110" s="87" t="s">
         <v>58</v>
@@ -31401,7 +31412,7 @@
     </row>
     <row r="111" spans="1:12" ht="24">
       <c r="A111" s="89" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="B111" s="82"/>
       <c r="C111" s="82" t="s">
@@ -31424,12 +31435,12 @@
       </c>
       <c r="K111" s="80"/>
       <c r="L111" s="80" t="s">
-        <v>1003</v>
-      </c>
-    </row>
-    <row r="112" spans="1:12" ht="24">
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="112" spans="1:12" ht="36">
       <c r="A112" s="89" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="B112" s="87" t="s">
         <v>58</v>
@@ -31458,12 +31469,12 @@
       </c>
       <c r="K112" s="80"/>
       <c r="L112" s="80" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="113" spans="1:12">
       <c r="A113" s="89" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="B113" s="82" t="s">
         <v>328</v>
@@ -31490,12 +31501,12 @@
       </c>
       <c r="K113" s="80"/>
       <c r="L113" s="80" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="114" spans="1:12">
       <c r="A114" s="89" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="B114" s="82" t="s">
         <v>328</v>
@@ -31522,12 +31533,12 @@
       </c>
       <c r="K114" s="80"/>
       <c r="L114" s="80" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="115" spans="1:12">
       <c r="A115" s="89" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="B115" s="82" t="s">
         <v>328</v>
@@ -31554,12 +31565,12 @@
       </c>
       <c r="K115" s="80"/>
       <c r="L115" s="80" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="116" spans="1:12" ht="36">
       <c r="A116" s="89" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="B116" s="87" t="s">
         <v>58</v>
@@ -31586,12 +31597,12 @@
       </c>
       <c r="K116" s="80"/>
       <c r="L116" s="80" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="117" spans="1:12" ht="24">
       <c r="A117" s="89" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
       <c r="B117" s="82" t="s">
         <v>328</v>
@@ -31618,12 +31629,12 @@
       </c>
       <c r="K117" s="80"/>
       <c r="L117" s="80" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="118" spans="1:12">
       <c r="A118" s="89" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="B118" s="82" t="s">
         <v>328</v>
@@ -31650,12 +31661,12 @@
       </c>
       <c r="K118" s="80"/>
       <c r="L118" s="80" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="119" spans="1:12" ht="24">
       <c r="A119" s="89" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="B119" s="82" t="s">
         <v>328</v>
@@ -31682,12 +31693,12 @@
       </c>
       <c r="K119" s="80"/>
       <c r="L119" s="80" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="120" spans="1:12" ht="36">
       <c r="A120" s="89" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
       <c r="B120" s="87" t="s">
         <v>58</v>
@@ -31714,12 +31725,12 @@
       </c>
       <c r="K120" s="80"/>
       <c r="L120" s="80" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="121" spans="1:12" ht="24">
       <c r="A121" s="89" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="B121" s="82" t="s">
         <v>34</v>
@@ -31746,12 +31757,12 @@
       </c>
       <c r="K121" s="80"/>
       <c r="L121" s="80" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="122" spans="1:12" ht="24">
       <c r="A122" s="89" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
       <c r="B122" s="82" t="s">
         <v>34</v>
@@ -31778,12 +31789,12 @@
       </c>
       <c r="K122" s="80"/>
       <c r="L122" s="80" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="123" spans="1:12">
       <c r="A123" s="89" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="B123" s="82" t="s">
         <v>34</v>
@@ -31810,12 +31821,12 @@
       </c>
       <c r="K123" s="80"/>
       <c r="L123" s="80" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="124" spans="1:12" ht="48">
       <c r="A124" s="89" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="B124" s="87" t="s">
         <v>58</v>
@@ -31842,12 +31853,12 @@
       </c>
       <c r="K124" s="80"/>
       <c r="L124" s="80" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="125" spans="1:12" ht="24">
       <c r="A125" s="89" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="B125" s="82" t="s">
         <v>328</v>
@@ -31874,12 +31885,12 @@
       </c>
       <c r="K125" s="80"/>
       <c r="L125" s="80" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="126" spans="1:12">
       <c r="A126" s="89" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="B126" s="82" t="s">
         <v>328</v>
@@ -31906,12 +31917,12 @@
       </c>
       <c r="K126" s="80"/>
       <c r="L126" s="80" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="127" spans="1:12">
       <c r="A127" s="89" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
       <c r="B127" s="82"/>
       <c r="C127" s="82" t="s">
@@ -31933,12 +31944,12 @@
       </c>
       <c r="K127" s="80"/>
       <c r="L127" s="80" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="128" spans="1:12">
       <c r="A128" s="89" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="B128" s="82" t="s">
         <v>328</v>
@@ -31965,12 +31976,12 @@
       </c>
       <c r="K128" s="80"/>
       <c r="L128" s="80" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="129" spans="1:12" ht="24">
       <c r="A129" s="89" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="B129" s="82"/>
       <c r="C129" s="82" t="s">
@@ -31994,12 +32005,12 @@
       </c>
       <c r="K129" s="80"/>
       <c r="L129" s="80" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="130" spans="1:12" ht="36">
       <c r="A130" s="89" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="B130" s="87" t="s">
         <v>58</v>
@@ -32024,12 +32035,12 @@
       </c>
       <c r="K130" s="80"/>
       <c r="L130" s="80" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="131" spans="1:12" ht="36">
       <c r="A131" s="89" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="B131" s="87" t="s">
         <v>58</v>
@@ -32056,12 +32067,12 @@
       </c>
       <c r="K131" s="80"/>
       <c r="L131" s="80" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="132" spans="1:12">
       <c r="A132" s="89" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
       <c r="B132" s="82" t="s">
         <v>328</v>
@@ -32088,12 +32099,12 @@
       </c>
       <c r="K132" s="80"/>
       <c r="L132" s="80" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="133" spans="1:12">
       <c r="A133" s="89" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="B133" s="82" t="s">
         <v>328</v>
@@ -32120,12 +32131,12 @@
       </c>
       <c r="K133" s="80"/>
       <c r="L133" s="80" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="134" spans="1:12">
       <c r="A134" s="89" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="B134" s="82"/>
       <c r="C134" s="82" t="s">
@@ -32147,12 +32158,12 @@
       </c>
       <c r="K134" s="80"/>
       <c r="L134" s="80" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="135" spans="1:12">
       <c r="A135" s="89" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="B135" s="82" t="s">
         <v>328</v>
@@ -32179,12 +32190,12 @@
       </c>
       <c r="K135" s="80"/>
       <c r="L135" s="80" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="136" spans="1:12" ht="36">
       <c r="A136" s="89" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="B136" s="87" t="s">
         <v>58</v>
@@ -32211,12 +32222,12 @@
       </c>
       <c r="K136" s="80"/>
       <c r="L136" s="80" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="137" spans="1:12">
       <c r="A137" s="89" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="B137" s="82" t="s">
         <v>328</v>
@@ -32243,12 +32254,12 @@
       </c>
       <c r="K137" s="80"/>
       <c r="L137" s="80" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="138" spans="1:12">
       <c r="A138" s="89" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="B138" s="82" t="s">
         <v>328</v>
@@ -32275,12 +32286,12 @@
       </c>
       <c r="K138" s="80"/>
       <c r="L138" s="80" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="139" spans="1:12">
       <c r="A139" s="89" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="B139" s="82"/>
       <c r="C139" s="82" t="s">
@@ -32302,12 +32313,12 @@
       </c>
       <c r="K139" s="80"/>
       <c r="L139" s="80" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="140" spans="1:12">
       <c r="A140" s="89" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="B140" s="82" t="s">
         <v>328</v>
@@ -32334,12 +32345,12 @@
       </c>
       <c r="K140" s="80"/>
       <c r="L140" s="80" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="141" spans="1:12" ht="36">
       <c r="A141" s="89" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
       <c r="B141" s="87" t="s">
         <v>58</v>
@@ -32366,12 +32377,12 @@
       </c>
       <c r="K141" s="80"/>
       <c r="L141" s="80" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="142" spans="1:12">
       <c r="A142" s="89" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="B142" s="82" t="s">
         <v>34</v>
@@ -32396,12 +32407,12 @@
       </c>
       <c r="K142" s="80"/>
       <c r="L142" s="80" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="143" spans="1:12">
       <c r="A143" s="89" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="B143" s="82" t="s">
         <v>34</v>
@@ -32426,12 +32437,12 @@
       </c>
       <c r="K143" s="80"/>
       <c r="L143" s="80" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="144" spans="1:12">
       <c r="A144" s="89" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="B144" s="82" t="s">
         <v>34</v>
@@ -32458,10 +32469,10 @@
       </c>
       <c r="K144" s="80"/>
       <c r="L144" s="80" t="s">
-        <v>1005</v>
-      </c>
-    </row>
-    <row r="145" spans="1:12" s="81" customFormat="1" ht="14.4">
+        <v>1004</v>
+      </c>
+    </row>
+    <row r="145" spans="1:12" s="81" customFormat="1" ht="15">
       <c r="A145" s="12" t="s">
         <v>484</v>
       </c>
@@ -32499,7 +32510,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="146" spans="1:12" s="81" customFormat="1" ht="14.4">
+    <row r="146" spans="1:12" s="81" customFormat="1" ht="15">
       <c r="A146" s="104" t="s">
         <v>486</v>
       </c>
@@ -32527,7 +32538,7 @@
       </c>
       <c r="L146" s="80"/>
     </row>
-    <row r="147" spans="1:12" s="81" customFormat="1" ht="14.4">
+    <row r="147" spans="1:12" s="81" customFormat="1" ht="15">
       <c r="A147" s="104" t="s">
         <v>487</v>
       </c>
@@ -32547,7 +32558,7 @@
       </c>
       <c r="L147" s="80"/>
     </row>
-    <row r="148" spans="1:12" s="81" customFormat="1" ht="14.4">
+    <row r="148" spans="1:12" s="81" customFormat="1" ht="15">
       <c r="A148" s="104" t="s">
         <v>393</v>
       </c>
@@ -32575,7 +32586,7 @@
       </c>
       <c r="L148" s="80"/>
     </row>
-    <row r="149" spans="1:12" s="81" customFormat="1" ht="14.4">
+    <row r="149" spans="1:12" s="81" customFormat="1" ht="15">
       <c r="A149" s="104" t="s">
         <v>488</v>
       </c>
@@ -32603,7 +32614,7 @@
       </c>
       <c r="L149" s="80"/>
     </row>
-    <row r="150" spans="1:12" s="81" customFormat="1" ht="14.4">
+    <row r="150" spans="1:12" s="81" customFormat="1" ht="15">
       <c r="A150" s="104" t="s">
         <v>492</v>
       </c>
@@ -32623,7 +32634,7 @@
       </c>
       <c r="L150" s="80"/>
     </row>
-    <row r="151" spans="1:12" s="81" customFormat="1" ht="14.4">
+    <row r="151" spans="1:12" s="81" customFormat="1" ht="15">
       <c r="A151" s="104" t="s">
         <v>489</v>
       </c>
@@ -32657,7 +32668,7 @@
       </c>
       <c r="L151" s="80"/>
     </row>
-    <row r="152" spans="1:12" s="81" customFormat="1" ht="14.4">
+    <row r="152" spans="1:12" s="81" customFormat="1" ht="15">
       <c r="A152" s="104" t="s">
         <v>490</v>
       </c>
@@ -32685,7 +32696,7 @@
       </c>
       <c r="L152" s="80"/>
     </row>
-    <row r="153" spans="1:12" s="81" customFormat="1" ht="14.4">
+    <row r="153" spans="1:12" s="81" customFormat="1" ht="15">
       <c r="A153" s="104" t="s">
         <v>493</v>
       </c>
@@ -32705,7 +32716,7 @@
       </c>
       <c r="L153" s="80"/>
     </row>
-    <row r="154" spans="1:12" s="81" customFormat="1" ht="14.4">
+    <row r="154" spans="1:12" s="81" customFormat="1" ht="15">
       <c r="A154" s="104" t="s">
         <v>491</v>
       </c>
@@ -32733,7 +32744,7 @@
       </c>
       <c r="L154" s="80"/>
     </row>
-    <row r="155" spans="1:12" s="81" customFormat="1" ht="14.4">
+    <row r="155" spans="1:12" s="81" customFormat="1" ht="15">
       <c r="A155" s="104" t="s">
         <v>494</v>
       </c>
@@ -32753,7 +32764,7 @@
       </c>
       <c r="L155" s="80"/>
     </row>
-    <row r="156" spans="1:12" s="81" customFormat="1" ht="14.4">
+    <row r="156" spans="1:12" s="81" customFormat="1" ht="15">
       <c r="A156" s="104" t="s">
         <v>495</v>
       </c>
@@ -32773,7 +32784,7 @@
       </c>
       <c r="L156" s="80"/>
     </row>
-    <row r="157" spans="1:12" s="81" customFormat="1" ht="14.4">
+    <row r="157" spans="1:12" s="81" customFormat="1" ht="15">
       <c r="A157" s="104" t="s">
         <v>496</v>
       </c>
@@ -35329,21 +35340,21 @@
       <selection pane="bottomRight" activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="44.44140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.6640625" style="36" customWidth="1"/>
+    <col min="1" max="1" width="44.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" style="36" customWidth="1"/>
     <col min="3" max="3" width="30" style="36" customWidth="1"/>
-    <col min="4" max="4" width="18.5546875" style="36" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" style="36" customWidth="1"/>
     <col min="5" max="5" width="20" style="37" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.33203125" style="37" customWidth="1"/>
+    <col min="6" max="6" width="27.28515625" style="37" customWidth="1"/>
     <col min="7" max="7" width="24" style="37" customWidth="1"/>
-    <col min="8" max="8" width="37.5546875" style="36" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="37.5703125" style="36" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="52" style="9" customWidth="1"/>
-    <col min="10" max="10" width="24.6640625" style="105" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="28.88671875" style="73" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="30.44140625" style="73" customWidth="1"/>
-    <col min="13" max="16384" width="9.109375" style="1"/>
+    <col min="10" max="10" width="24.7109375" style="105" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="28.85546875" style="73" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="30.42578125" style="73" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24">
@@ -35396,9 +35407,9 @@
       <c r="W1" s="3"/>
       <c r="X1" s="3"/>
     </row>
-    <row r="2" spans="1:24" ht="36">
+    <row r="2" spans="1:24" ht="48">
       <c r="A2" s="17" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="B2" s="61" t="s">
         <v>5</v>
@@ -35407,15 +35418,15 @@
         <v>171</v>
       </c>
       <c r="D2" s="7" t="s">
+        <v>950</v>
+      </c>
+      <c r="E2" s="186" t="s">
         <v>951</v>
-      </c>
-      <c r="E2" s="186" t="s">
-        <v>952</v>
       </c>
       <c r="F2" s="62"/>
       <c r="G2" s="62"/>
       <c r="H2" s="65" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="I2" s="38"/>
       <c r="J2" s="106" t="s">
@@ -35440,7 +35451,7 @@
     </row>
     <row r="3" spans="1:24" s="3" customFormat="1">
       <c r="A3" s="153" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="B3" s="175" t="s">
         <v>5</v>
@@ -35455,10 +35466,10 @@
         <v>96</v>
       </c>
       <c r="F3" s="197" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="G3" s="197" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="H3" s="190"/>
       <c r="I3" s="38"/>
@@ -35502,7 +35513,7 @@
     </row>
     <row r="5" spans="1:24" s="3" customFormat="1">
       <c r="A5" s="23" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="B5" s="175"/>
       <c r="C5" s="156"/>
@@ -35522,7 +35533,7 @@
     </row>
     <row r="6" spans="1:24" s="3" customFormat="1" ht="15.75" customHeight="1">
       <c r="A6" s="68" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="B6" s="64" t="s">
         <v>24</v>
@@ -35582,7 +35593,7 @@
     </row>
     <row r="8" spans="1:24" s="3" customFormat="1">
       <c r="A8" s="68" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="B8" s="64" t="s">
         <v>24</v>
@@ -35716,7 +35727,7 @@
     </row>
     <row r="12" spans="1:24" s="81" customFormat="1">
       <c r="A12" s="23" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="B12" s="78"/>
       <c r="C12" s="78"/>
@@ -37240,7 +37251,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="57" spans="1:12" s="81" customFormat="1" ht="24.6">
+    <row r="57" spans="1:12" s="81" customFormat="1" ht="24.75">
       <c r="A57" s="104" t="s">
         <v>407</v>
       </c>
@@ -37522,7 +37533,7 @@
         <v>806</v>
       </c>
     </row>
-    <row r="66" spans="1:12" s="81" customFormat="1" ht="24.6">
+    <row r="66" spans="1:12" s="81" customFormat="1" ht="24.75">
       <c r="A66" s="104" t="s">
         <v>411</v>
       </c>
@@ -37586,7 +37597,7 @@
       </c>
       <c r="L67" s="80"/>
     </row>
-    <row r="68" spans="1:12" s="81" customFormat="1" ht="24.6">
+    <row r="68" spans="1:12" s="81" customFormat="1" ht="24.75">
       <c r="A68" s="104" t="s">
         <v>412</v>
       </c>
@@ -37694,20 +37705,20 @@
       <selection pane="topRight" activeCell="L39" sqref="L39:L76"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="31.109375" style="137" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9.109375" style="137"/>
-    <col min="4" max="4" width="14.88671875" style="137" customWidth="1"/>
-    <col min="5" max="5" width="26.44140625" style="138" customWidth="1"/>
-    <col min="6" max="6" width="30.6640625" style="137" customWidth="1"/>
-    <col min="7" max="7" width="26.109375" style="137" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="61.44140625" style="168" customWidth="1"/>
-    <col min="9" max="9" width="52.44140625" style="137" customWidth="1"/>
-    <col min="10" max="10" width="24.88671875" style="137" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.109375" style="137"/>
-    <col min="12" max="12" width="12.5546875" style="137" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.109375" style="137"/>
+    <col min="1" max="1" width="31.140625" style="137" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.140625" style="137"/>
+    <col min="4" max="4" width="14.85546875" style="137" customWidth="1"/>
+    <col min="5" max="5" width="26.42578125" style="138" customWidth="1"/>
+    <col min="6" max="6" width="30.7109375" style="137" customWidth="1"/>
+    <col min="7" max="7" width="26.140625" style="137" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="61.42578125" style="168" customWidth="1"/>
+    <col min="9" max="9" width="52.42578125" style="137" customWidth="1"/>
+    <col min="10" max="10" width="24.85546875" style="137" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" style="137"/>
+    <col min="12" max="12" width="12.5703125" style="137" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="137"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="73" customFormat="1" ht="26.25" customHeight="1">
@@ -37775,7 +37786,7 @@
       </c>
       <c r="K2" s="191"/>
       <c r="L2" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="3" spans="1:12" s="73" customFormat="1" ht="23.25" customHeight="1">
@@ -37810,7 +37821,7 @@
       </c>
       <c r="K3" s="191"/>
       <c r="L3" s="191" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="4" spans="1:12" s="73" customFormat="1">
@@ -37843,7 +37854,7 @@
       </c>
       <c r="K4" s="191"/>
       <c r="L4" s="191" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="5" spans="1:12" s="73" customFormat="1" ht="24">
@@ -37875,7 +37886,7 @@
       </c>
       <c r="K5" s="191"/>
       <c r="L5" s="191" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="6" spans="1:12" s="73" customFormat="1">
@@ -37907,7 +37918,7 @@
       </c>
       <c r="K6" s="191"/>
       <c r="L6" s="191" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="7" spans="1:12" s="81" customFormat="1">
@@ -37937,7 +37948,7 @@
       </c>
       <c r="K7" s="191"/>
       <c r="L7" s="191" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="8" spans="1:12" s="81" customFormat="1">
@@ -37969,7 +37980,7 @@
       </c>
       <c r="K8" s="191"/>
       <c r="L8" s="191" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="9" spans="1:12" s="136" customFormat="1" ht="26.25" customHeight="1">
@@ -38041,7 +38052,7 @@
       </c>
       <c r="K10" s="103"/>
       <c r="L10" s="103" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="11" spans="1:12" s="136" customFormat="1" ht="12">
@@ -38075,7 +38086,7 @@
       </c>
       <c r="K11" s="103"/>
       <c r="L11" s="103" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="12" spans="1:12" s="136" customFormat="1" ht="12">
@@ -38109,7 +38120,7 @@
       </c>
       <c r="K12" s="103"/>
       <c r="L12" s="103" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="13" spans="1:12" s="136" customFormat="1" ht="12">
@@ -38143,7 +38154,7 @@
       </c>
       <c r="K13" s="103"/>
       <c r="L13" s="103" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="14" spans="1:12" s="136" customFormat="1" ht="12">
@@ -38177,7 +38188,7 @@
       </c>
       <c r="K14" s="103"/>
       <c r="L14" s="103" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="15" spans="1:12" s="136" customFormat="1" ht="12">
@@ -38211,7 +38222,7 @@
       </c>
       <c r="K15" s="103"/>
       <c r="L15" s="103" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="16" spans="1:12" s="136" customFormat="1" ht="12">
@@ -38245,7 +38256,7 @@
       </c>
       <c r="K16" s="103"/>
       <c r="L16" s="103" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="17" spans="1:12" s="136" customFormat="1" ht="12">
@@ -38279,7 +38290,7 @@
       </c>
       <c r="K17" s="103"/>
       <c r="L17" s="103" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="18" spans="1:12" s="136" customFormat="1" ht="12">
@@ -38313,7 +38324,7 @@
       </c>
       <c r="K18" s="103"/>
       <c r="L18" s="103" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="19" spans="1:12" s="136" customFormat="1" ht="12">
@@ -38347,7 +38358,7 @@
       </c>
       <c r="K19" s="103"/>
       <c r="L19" s="103" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="20" spans="1:12" s="136" customFormat="1" ht="12">
@@ -38381,7 +38392,7 @@
       </c>
       <c r="K20" s="103"/>
       <c r="L20" s="103" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="21" spans="1:12" s="136" customFormat="1" ht="12">
@@ -38415,7 +38426,7 @@
       </c>
       <c r="K21" s="103"/>
       <c r="L21" s="103" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="22" spans="1:12" s="136" customFormat="1" ht="12">
@@ -38449,7 +38460,7 @@
       </c>
       <c r="K22" s="103"/>
       <c r="L22" s="103" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="23" spans="1:12" s="136" customFormat="1" ht="12">
@@ -38483,7 +38494,7 @@
       </c>
       <c r="K23" s="103"/>
       <c r="L23" s="103" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="24" spans="1:12" s="136" customFormat="1" ht="12">
@@ -38517,7 +38528,7 @@
       </c>
       <c r="K24" s="103"/>
       <c r="L24" s="103" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="25" spans="1:12" s="136" customFormat="1" ht="12">
@@ -38551,7 +38562,7 @@
       </c>
       <c r="K25" s="103"/>
       <c r="L25" s="103" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="26" spans="1:12" s="136" customFormat="1" ht="12">
@@ -38585,7 +38596,7 @@
       </c>
       <c r="K26" s="103"/>
       <c r="L26" s="103" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="27" spans="1:12" s="136" customFormat="1" ht="12">
@@ -38619,7 +38630,7 @@
       </c>
       <c r="K27" s="103"/>
       <c r="L27" s="103" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="28" spans="1:12" s="136" customFormat="1" ht="12">
@@ -38653,7 +38664,7 @@
       </c>
       <c r="K28" s="103"/>
       <c r="L28" s="103" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="29" spans="1:12" s="136" customFormat="1" ht="12">
@@ -38687,7 +38698,7 @@
       </c>
       <c r="K29" s="103"/>
       <c r="L29" s="103" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="30" spans="1:12">
@@ -38715,7 +38726,7 @@
       </c>
       <c r="K30" s="191"/>
       <c r="L30" s="103" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="31" spans="1:12">
@@ -38745,7 +38756,7 @@
       </c>
       <c r="K31" s="191"/>
       <c r="L31" s="103" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="32" spans="1:12" s="136" customFormat="1" ht="12">
@@ -38779,7 +38790,7 @@
       </c>
       <c r="K32" s="103"/>
       <c r="L32" s="103" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="33" spans="1:12" s="136" customFormat="1" ht="12">
@@ -38813,7 +38824,7 @@
       </c>
       <c r="K33" s="103"/>
       <c r="L33" s="103" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="34" spans="1:12" s="136" customFormat="1" ht="12">
@@ -38847,7 +38858,7 @@
       </c>
       <c r="K34" s="103"/>
       <c r="L34" s="103" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="35" spans="1:12" s="136" customFormat="1" ht="12">
@@ -38881,7 +38892,7 @@
       </c>
       <c r="K35" s="103"/>
       <c r="L35" s="103" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="36" spans="1:12" s="136" customFormat="1" ht="12">
@@ -38915,7 +38926,7 @@
       </c>
       <c r="K36" s="103"/>
       <c r="L36" s="103" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="37" spans="1:12" s="136" customFormat="1" ht="12">
@@ -38949,7 +38960,7 @@
       </c>
       <c r="K37" s="103"/>
       <c r="L37" s="103" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="38" spans="1:12">
@@ -38990,7 +39001,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="39" spans="1:12">
+    <row r="39" spans="1:12" ht="24.75">
       <c r="A39" s="142" t="s">
         <v>853</v>
       </c>
@@ -39017,7 +39028,7 @@
       </c>
       <c r="K39" s="191"/>
       <c r="L39" s="103" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="40" spans="1:12">
@@ -39045,7 +39056,7 @@
       </c>
       <c r="K40" s="191"/>
       <c r="L40" s="103" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="41" spans="1:12">
@@ -39077,7 +39088,7 @@
       </c>
       <c r="K41" s="191"/>
       <c r="L41" s="103" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="42" spans="1:12">
@@ -39109,7 +39120,7 @@
       </c>
       <c r="K42" s="191"/>
       <c r="L42" s="103" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="43" spans="1:12" ht="24">
@@ -39137,7 +39148,7 @@
       </c>
       <c r="K43" s="191"/>
       <c r="L43" s="103" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="44" spans="1:12">
@@ -39167,10 +39178,10 @@
       </c>
       <c r="K44" s="191"/>
       <c r="L44" s="103" t="s">
-        <v>1005</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" ht="36.6">
+        <v>1004</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" ht="36.75">
       <c r="A45" s="142" t="s">
         <v>860</v>
       </c>
@@ -39189,10 +39200,10 @@
       </c>
       <c r="K45" s="191"/>
       <c r="L45" s="103" t="s">
-        <v>1005</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" ht="60.6">
+        <v>1004</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" ht="72.75">
       <c r="A46" s="142" t="s">
         <v>861</v>
       </c>
@@ -39221,7 +39232,7 @@
       </c>
       <c r="K46" s="191"/>
       <c r="L46" s="103" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="47" spans="1:12">
@@ -39251,7 +39262,7 @@
       </c>
       <c r="K47" s="191"/>
       <c r="L47" s="103" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="48" spans="1:12">
@@ -39279,10 +39290,10 @@
       </c>
       <c r="K48" s="191"/>
       <c r="L48" s="103" t="s">
-        <v>1005</v>
-      </c>
-    </row>
-    <row r="49" spans="1:12" ht="24">
+        <v>1004</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" ht="24.75">
       <c r="A49" s="142" t="s">
         <v>864</v>
       </c>
@@ -39311,10 +39322,10 @@
       </c>
       <c r="K49" s="191"/>
       <c r="L49" s="103" t="s">
-        <v>1005</v>
-      </c>
-    </row>
-    <row r="50" spans="1:12" ht="36.6">
+        <v>1004</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" ht="48.75">
       <c r="A50" s="142" t="s">
         <v>865</v>
       </c>
@@ -39343,7 +39354,7 @@
       </c>
       <c r="K50" s="191"/>
       <c r="L50" s="103" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="51" spans="1:12" ht="24">
@@ -39365,7 +39376,7 @@
       </c>
       <c r="K51" s="191"/>
       <c r="L51" s="103" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="52" spans="1:12">
@@ -39395,7 +39406,7 @@
       </c>
       <c r="K52" s="191"/>
       <c r="L52" s="103" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="53" spans="1:12" ht="24">
@@ -39423,7 +39434,7 @@
       </c>
       <c r="K53" s="191"/>
       <c r="L53" s="103" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="54" spans="1:12">
@@ -39453,7 +39464,7 @@
       </c>
       <c r="K54" s="191"/>
       <c r="L54" s="103" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="55" spans="1:12">
@@ -39483,7 +39494,7 @@
       </c>
       <c r="K55" s="191"/>
       <c r="L55" s="103" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="56" spans="1:12">
@@ -39509,7 +39520,7 @@
       </c>
       <c r="K56" s="191"/>
       <c r="L56" s="103" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="57" spans="1:12" ht="36">
@@ -39539,10 +39550,10 @@
       </c>
       <c r="K57" s="191"/>
       <c r="L57" s="103" t="s">
-        <v>1005</v>
-      </c>
-    </row>
-    <row r="58" spans="1:12">
+        <v>1004</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" ht="24.75">
       <c r="A58" s="142" t="s">
         <v>873</v>
       </c>
@@ -39567,7 +39578,7 @@
       </c>
       <c r="K58" s="191"/>
       <c r="L58" s="103" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="59" spans="1:12">
@@ -39595,7 +39606,7 @@
       </c>
       <c r="K59" s="191"/>
       <c r="L59" s="103" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="60" spans="1:12">
@@ -39625,7 +39636,7 @@
       </c>
       <c r="K60" s="191"/>
       <c r="L60" s="103" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="61" spans="1:12">
@@ -39655,7 +39666,7 @@
       </c>
       <c r="K61" s="191"/>
       <c r="L61" s="103" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="62" spans="1:12" ht="24">
@@ -39683,7 +39694,7 @@
       </c>
       <c r="K62" s="191"/>
       <c r="L62" s="103" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="63" spans="1:12">
@@ -39713,10 +39724,10 @@
       </c>
       <c r="K63" s="191"/>
       <c r="L63" s="103" t="s">
-        <v>1005</v>
-      </c>
-    </row>
-    <row r="64" spans="1:12" ht="24.6">
+        <v>1004</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" ht="36.75">
       <c r="A64" s="142" t="s">
         <v>879</v>
       </c>
@@ -39739,10 +39750,10 @@
       </c>
       <c r="K64" s="191"/>
       <c r="L64" s="103" t="s">
-        <v>1005</v>
-      </c>
-    </row>
-    <row r="65" spans="1:12" ht="60.6">
+        <v>1004</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" ht="72.75">
       <c r="A65" s="142" t="s">
         <v>880</v>
       </c>
@@ -39771,7 +39782,7 @@
       </c>
       <c r="K65" s="191"/>
       <c r="L65" s="103" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="66" spans="1:12">
@@ -39801,7 +39812,7 @@
       </c>
       <c r="K66" s="191"/>
       <c r="L66" s="103" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="67" spans="1:12">
@@ -39829,10 +39840,10 @@
       </c>
       <c r="K67" s="191"/>
       <c r="L67" s="103" t="s">
-        <v>1005</v>
-      </c>
-    </row>
-    <row r="68" spans="1:12" ht="24">
+        <v>1004</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" ht="24.75">
       <c r="A68" s="142" t="s">
         <v>883</v>
       </c>
@@ -39861,10 +39872,10 @@
       </c>
       <c r="K68" s="191"/>
       <c r="L68" s="103" t="s">
-        <v>1005</v>
-      </c>
-    </row>
-    <row r="69" spans="1:12" ht="36.6">
+        <v>1004</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" ht="48.75">
       <c r="A69" s="142" t="s">
         <v>884</v>
       </c>
@@ -39893,7 +39904,7 @@
       </c>
       <c r="K69" s="191"/>
       <c r="L69" s="103" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="70" spans="1:12">
@@ -39917,7 +39928,7 @@
       </c>
       <c r="K70" s="191"/>
       <c r="L70" s="103" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="71" spans="1:12">
@@ -39947,7 +39958,7 @@
       </c>
       <c r="K71" s="191"/>
       <c r="L71" s="103" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="72" spans="1:12" ht="24">
@@ -39975,7 +39986,7 @@
       </c>
       <c r="K72" s="191"/>
       <c r="L72" s="103" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="73" spans="1:12">
@@ -40005,7 +40016,7 @@
       </c>
       <c r="K73" s="191"/>
       <c r="L73" s="103" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="74" spans="1:12">
@@ -40035,7 +40046,7 @@
       </c>
       <c r="K74" s="191"/>
       <c r="L74" s="103" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="75" spans="1:12">
@@ -40061,7 +40072,7 @@
       </c>
       <c r="K75" s="191"/>
       <c r="L75" s="103" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="76" spans="1:12" ht="36">
@@ -40091,7 +40102,7 @@
       </c>
       <c r="K76" s="191"/>
       <c r="L76" s="103" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated patient lung volumes to be based on ideal weight instead of actual weight. Updated respiratory compliance methodology. Added new respiratory system data setting and definitions. Added a new circuit test for adding volume and changing pressure on a compliance node.
</commit_message>
<xml_diff>
--- a/test/validation/SystemValidationData.xlsx
+++ b/test/validation/SystemValidationData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Programming\Pulse\engine-ingmar\test\validation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Source\IngMarPublicMaster\test\validation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A176E392-3F92-44FB-B1E7-8CFB44EBD3E5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04830A3C-03FA-4C61-86E4-138FE66A984D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="724" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="32040" tabRatio="724" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blood Chemistry" sheetId="4" r:id="rId1"/>
@@ -23,11 +23,12 @@
     <sheet name="Respiratory" sheetId="2" r:id="rId8"/>
     <sheet name="Tissue" sheetId="34" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3862" uniqueCount="1062">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3865" uniqueCount="1063">
   <si>
     <t>Output</t>
   </si>
@@ -3275,9 +3276,6 @@
     <t>ImposedPowerOfBreathing*</t>
   </si>
   <si>
-    <t>RespiratoryMuscleFatigue*</t>
-  </si>
-  <si>
     <t>ResistiveInspiratoryWorkOfBreathing*</t>
   </si>
   <si>
@@ -3347,6 +3345,12 @@
   </si>
   <si>
     <t>The normal human weighing 70kg has a body surface area of about 1.7 square meteres. Therefore, 0.14*1.7.</t>
+  </si>
+  <si>
+    <t>RespiratoryMuscleFatigue</t>
+  </si>
+  <si>
+    <t>roussos1979fatigue</t>
   </si>
 </sst>
 </file>
@@ -8165,7 +8169,7 @@
         <v>150</v>
       </c>
       <c r="G4" s="214" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="H4" s="196"/>
       <c r="I4" s="218"/>
@@ -8837,7 +8841,7 @@
         <v>931</v>
       </c>
       <c r="G28" s="196" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
       <c r="H28" s="216"/>
       <c r="I28" s="217"/>
@@ -35544,7 +35548,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B34" sqref="B34"/>
+      <selection pane="bottomRight" activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -36120,7 +36124,7 @@
     </row>
     <row r="20" spans="1:24" s="190" customFormat="1" ht="60">
       <c r="A20" s="145" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="B20" s="71" t="s">
         <v>8</v>
@@ -36330,16 +36334,16 @@
     </row>
     <row r="27" spans="1:24" s="3" customFormat="1">
       <c r="A27" s="145" t="s">
+        <v>1049</v>
+      </c>
+      <c r="B27" s="167" t="s">
         <v>1050</v>
-      </c>
-      <c r="B27" s="167" t="s">
-        <v>1051</v>
       </c>
       <c r="C27" s="168" t="s">
         <v>168</v>
       </c>
       <c r="D27" s="167" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
       <c r="E27" s="182" t="s">
         <v>245</v>
@@ -36349,7 +36353,7 @@
       </c>
       <c r="G27" s="182"/>
       <c r="H27" s="71" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="I27" s="37"/>
       <c r="J27" s="102" t="s">
@@ -36371,13 +36375,13 @@
         <v>168</v>
       </c>
       <c r="D28" s="6" t="s">
+        <v>1053</v>
+      </c>
+      <c r="E28" s="58" t="s">
+        <v>1046</v>
+      </c>
+      <c r="F28" s="58" t="s">
         <v>1054</v>
-      </c>
-      <c r="E28" s="58" t="s">
-        <v>1047</v>
-      </c>
-      <c r="F28" s="58" t="s">
-        <v>1055</v>
       </c>
       <c r="G28" s="58"/>
       <c r="H28" s="71"/>
@@ -36404,7 +36408,7 @@
     </row>
     <row r="29" spans="1:24" s="3" customFormat="1">
       <c r="A29" s="22" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="B29" s="167" t="s">
         <v>1029</v>
@@ -36426,7 +36430,7 @@
     </row>
     <row r="30" spans="1:24" s="3" customFormat="1">
       <c r="A30" s="22" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
       <c r="B30" s="167" t="s">
         <v>1029</v>
@@ -36457,7 +36461,7 @@
         <v>168</v>
       </c>
       <c r="D31" s="60" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="E31" s="30" t="s">
         <v>1025</v>
@@ -36490,7 +36494,7 @@
     </row>
     <row r="32" spans="1:24" s="14" customFormat="1">
       <c r="A32" s="22" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
       <c r="B32" s="67"/>
       <c r="C32" s="67"/>
@@ -36509,13 +36513,19 @@
       </c>
     </row>
     <row r="33" spans="1:24" s="3" customFormat="1">
-      <c r="A33" s="22" t="s">
-        <v>1038</v>
+      <c r="A33" s="201" t="s">
+        <v>1061</v>
       </c>
       <c r="B33" s="167"/>
-      <c r="C33" s="168"/>
-      <c r="D33" s="168"/>
-      <c r="E33" s="182"/>
+      <c r="C33" s="168" t="s">
+        <v>168</v>
+      </c>
+      <c r="D33" s="168">
+        <v>0</v>
+      </c>
+      <c r="E33" s="182" t="s">
+        <v>1062</v>
+      </c>
       <c r="F33" s="182"/>
       <c r="G33" s="182"/>
       <c r="H33" s="71"/>
@@ -36530,7 +36540,7 @@
     </row>
     <row r="34" spans="1:24" s="77" customFormat="1">
       <c r="A34" s="22" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="B34" s="74"/>
       <c r="C34" s="74"/>
@@ -36540,7 +36550,9 @@
       <c r="G34" s="182"/>
       <c r="H34" s="71"/>
       <c r="I34" s="38"/>
-      <c r="J34" s="102"/>
+      <c r="J34" s="102" t="s">
+        <v>394</v>
+      </c>
       <c r="K34" s="177"/>
       <c r="L34" s="99" t="s">
         <v>794</v>
@@ -36841,7 +36853,7 @@
     </row>
     <row r="43" spans="1:24" s="3" customFormat="1">
       <c r="A43" s="145" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="B43" s="82" t="s">
         <v>8</v>
@@ -36871,7 +36883,7 @@
     </row>
     <row r="44" spans="1:24" s="3" customFormat="1">
       <c r="A44" s="145" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="B44" s="82" t="s">
         <v>8</v>
@@ -36901,7 +36913,7 @@
     </row>
     <row r="45" spans="1:24" s="3" customFormat="1">
       <c r="A45" s="145" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="B45" s="167" t="s">
         <v>8</v>
@@ -36931,7 +36943,7 @@
     </row>
     <row r="46" spans="1:24" s="3" customFormat="1">
       <c r="A46" s="145" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="B46" s="167" t="s">
         <v>8</v>
@@ -36961,7 +36973,7 @@
     </row>
     <row r="47" spans="1:24" s="190" customFormat="1" ht="24">
       <c r="A47" s="145" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
       <c r="B47" s="82" t="s">
         <v>8</v>
@@ -36993,7 +37005,7 @@
     </row>
     <row r="48" spans="1:24" s="190" customFormat="1" ht="24">
       <c r="A48" s="145" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
       <c r="B48" s="82" t="s">
         <v>8</v>
@@ -37097,7 +37109,7 @@
     </row>
     <row r="51" spans="1:24" s="3" customFormat="1" ht="24">
       <c r="A51" s="145" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
       <c r="B51" s="82" t="s">
         <v>8</v>
@@ -37109,13 +37121,13 @@
         <v>0</v>
       </c>
       <c r="E51" s="182" t="s">
+        <v>1046</v>
+      </c>
+      <c r="F51" s="182" t="s">
         <v>1047</v>
       </c>
-      <c r="F51" s="182" t="s">
+      <c r="G51" s="182" t="s">
         <v>1048</v>
-      </c>
-      <c r="G51" s="182" t="s">
-        <v>1049</v>
       </c>
       <c r="H51" s="71"/>
       <c r="I51" s="40"/>
@@ -37129,7 +37141,7 @@
     </row>
     <row r="52" spans="1:24" s="3" customFormat="1" ht="24">
       <c r="A52" s="145" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
       <c r="B52" s="82" t="s">
         <v>8</v>
@@ -37141,13 +37153,13 @@
         <v>0</v>
       </c>
       <c r="E52" s="182" t="s">
+        <v>1046</v>
+      </c>
+      <c r="F52" s="182" t="s">
         <v>1047</v>
       </c>
-      <c r="F52" s="182" t="s">
+      <c r="G52" s="182" t="s">
         <v>1048</v>
-      </c>
-      <c r="G52" s="182" t="s">
-        <v>1049</v>
       </c>
       <c r="H52" s="71"/>
       <c r="I52" s="40"/>
@@ -37161,7 +37173,7 @@
     </row>
     <row r="53" spans="1:24" s="3" customFormat="1">
       <c r="A53" s="145" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
       <c r="B53" s="82" t="s">
         <v>8</v>
@@ -37191,7 +37203,7 @@
     </row>
     <row r="54" spans="1:24" s="3" customFormat="1">
       <c r="A54" s="145" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
       <c r="B54" s="82" t="s">
         <v>8</v>
@@ -39125,7 +39137,7 @@
     </row>
     <row r="9" spans="1:12" s="129" customFormat="1" ht="26.25" customHeight="1">
       <c r="A9" s="55" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="B9" s="62" t="s">
         <v>1</v>

</xml_diff>

<commit_message>
Fixed a sign issue on CO2 alveloar transfer validation.
</commit_message>
<xml_diff>
--- a/test/validation/SystemValidationData.xlsx
+++ b/test/validation/SystemValidationData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Source\engine\test\validation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA12706A-C6CA-4DF9-B5D2-F782F7C2053F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5EF7675-18F5-4CF2-957D-CBBE18BD18D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16260" yWindow="4350" windowWidth="34260" windowHeight="22800" tabRatio="724" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25155" yWindow="7125" windowWidth="23790" windowHeight="17370" tabRatio="724" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blood Chemistry" sheetId="4" r:id="rId1"/>
@@ -35527,7 +35527,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:X109"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -38814,9 +38814,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:L79"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="4" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B7" sqref="B7"/>
+      <selection pane="topRight" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -39146,7 +39146,7 @@
         <v>168</v>
       </c>
       <c r="D10" s="183">
-        <v>250</v>
+        <v>-250</v>
       </c>
       <c r="E10" s="181" t="s">
         <v>242</v>

</xml_diff>

<commit_message>
Updated scenarios with new stuff. Updated respiratory validation spreadsheet.
</commit_message>
<xml_diff>
--- a/test/validation/SystemValidationData.xlsx
+++ b/test/validation/SystemValidationData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Pulse\engine\test\validation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Source\engine\test\validation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91A05C50-0DF5-4BCF-86AF-85DBD4E81EC9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2136B69-C280-411B-B279-C5D90FBB28B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="724" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1830" yWindow="3450" windowWidth="27090" windowHeight="25230" tabRatio="724" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blood Chemistry" sheetId="4" r:id="rId1"/>
@@ -23,11 +23,12 @@
     <sheet name="Respiratory" sheetId="2" r:id="rId8"/>
     <sheet name="Tissue" sheetId="34" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3869" uniqueCount="1060">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3895" uniqueCount="1063">
   <si>
     <t>Output</t>
   </si>
@@ -3339,6 +3340,15 @@
   </si>
   <si>
     <t>ExpiratoryPulmonaryResistance</t>
+  </si>
+  <si>
+    <t>IntrapulmonaryPressure</t>
+  </si>
+  <si>
+    <t>TransMusclePressure</t>
+  </si>
+  <si>
+    <t>[Tidal Volume] / [Total Compliance]</t>
   </si>
 </sst>
 </file>
@@ -4095,7 +4105,7 @@
     <xf numFmtId="0" fontId="15" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="30" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="223">
+  <cellXfs count="224">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4708,6 +4718,9 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -35527,13 +35540,13 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:X110"/>
+  <dimension ref="A1:X114"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A14" sqref="A14"/>
+      <selection pane="bottomRight" activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -36147,175 +36160,173 @@
         <v>780</v>
       </c>
     </row>
-    <row r="21" spans="1:24" s="189" customFormat="1">
-      <c r="A21" s="144" t="s">
-        <v>990</v>
-      </c>
-      <c r="B21" s="166" t="s">
-        <v>27</v>
-      </c>
-      <c r="C21" s="187" t="s">
-        <v>168</v>
-      </c>
-      <c r="D21" s="191">
-        <v>0.2</v>
-      </c>
-      <c r="E21" s="181" t="s">
-        <v>242</v>
-      </c>
-      <c r="F21" s="181" t="s">
-        <v>999</v>
-      </c>
-      <c r="G21" s="181"/>
-      <c r="H21" s="70"/>
-      <c r="I21" s="113"/>
+    <row r="21" spans="1:24" s="3" customFormat="1">
+      <c r="A21" s="200" t="s">
+        <v>1060</v>
+      </c>
+      <c r="B21" s="81" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" s="212" t="s">
+        <v>1055</v>
+      </c>
+      <c r="D21" s="223">
+        <v>5.4</v>
+      </c>
+      <c r="E21" s="211" t="s">
+        <v>93</v>
+      </c>
+      <c r="F21" s="195"/>
+      <c r="G21" s="211"/>
+      <c r="H21" s="70" t="s">
+        <v>1062</v>
+      </c>
+      <c r="I21" s="40"/>
       <c r="J21" s="101" t="s">
         <v>385</v>
       </c>
-      <c r="K21" s="98"/>
+      <c r="K21" s="214"/>
       <c r="L21" s="98" t="s">
         <v>780</v>
       </c>
     </row>
-    <row r="22" spans="1:24" s="189" customFormat="1" ht="60">
-      <c r="A22" s="144" t="s">
-        <v>1038</v>
-      </c>
-      <c r="B22" s="70" t="s">
+    <row r="22" spans="1:24" s="3" customFormat="1">
+      <c r="A22" s="200" t="s">
+        <v>1060</v>
+      </c>
+      <c r="B22" s="81" t="s">
         <v>8</v>
       </c>
-      <c r="C22" s="187" t="s">
-        <v>168</v>
-      </c>
-      <c r="D22" s="192">
-        <v>-1</v>
-      </c>
-      <c r="E22" s="181" t="s">
-        <v>242</v>
-      </c>
-      <c r="F22" s="181" t="s">
-        <v>1008</v>
-      </c>
-      <c r="G22" s="181"/>
-      <c r="H22" s="70" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I22" s="113"/>
+      <c r="C22" s="212" t="s">
+        <v>1054</v>
+      </c>
+      <c r="D22" s="223">
+        <v>0</v>
+      </c>
+      <c r="E22" s="211" t="s">
+        <v>93</v>
+      </c>
+      <c r="F22" s="195"/>
+      <c r="G22" s="211"/>
+      <c r="H22" s="70"/>
+      <c r="I22" s="40"/>
       <c r="J22" s="101" t="s">
         <v>385</v>
       </c>
-      <c r="K22" s="98"/>
+      <c r="K22" s="214"/>
       <c r="L22" s="98" t="s">
         <v>780</v>
       </c>
     </row>
-    <row r="23" spans="1:24" s="3" customFormat="1">
-      <c r="A23" s="22" t="s">
-        <v>1020</v>
+    <row r="23" spans="1:24" s="189" customFormat="1">
+      <c r="A23" s="144" t="s">
+        <v>990</v>
       </c>
       <c r="B23" s="166" t="s">
-        <v>1014</v>
-      </c>
-      <c r="C23" s="167"/>
-      <c r="D23" s="167"/>
-      <c r="E23" s="181"/>
-      <c r="F23" s="181"/>
+        <v>27</v>
+      </c>
+      <c r="C23" s="187" t="s">
+        <v>168</v>
+      </c>
+      <c r="D23" s="191">
+        <v>0.2</v>
+      </c>
+      <c r="E23" s="181" t="s">
+        <v>242</v>
+      </c>
+      <c r="F23" s="181" t="s">
+        <v>999</v>
+      </c>
       <c r="G23" s="181"/>
       <c r="H23" s="70"/>
-      <c r="I23" s="40"/>
+      <c r="I23" s="113"/>
       <c r="J23" s="101" t="s">
         <v>385</v>
       </c>
-      <c r="K23" s="176"/>
+      <c r="K23" s="98"/>
       <c r="L23" s="98" t="s">
         <v>780</v>
       </c>
     </row>
-    <row r="24" spans="1:24" s="3" customFormat="1">
-      <c r="A24" s="22" t="s">
-        <v>1015</v>
-      </c>
-      <c r="B24" s="166" t="s">
-        <v>1013</v>
-      </c>
-      <c r="C24" s="167"/>
-      <c r="D24" s="167"/>
-      <c r="E24" s="181"/>
-      <c r="F24" s="181"/>
+    <row r="24" spans="1:24" s="189" customFormat="1" ht="60">
+      <c r="A24" s="144" t="s">
+        <v>1038</v>
+      </c>
+      <c r="B24" s="70" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24" s="187" t="s">
+        <v>168</v>
+      </c>
+      <c r="D24" s="192">
+        <v>-1</v>
+      </c>
+      <c r="E24" s="181" t="s">
+        <v>242</v>
+      </c>
+      <c r="F24" s="181" t="s">
+        <v>1008</v>
+      </c>
       <c r="G24" s="181"/>
-      <c r="H24" s="70"/>
-      <c r="I24" s="40"/>
+      <c r="H24" s="70" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I24" s="113"/>
       <c r="J24" s="101" t="s">
         <v>385</v>
       </c>
-      <c r="K24" s="176"/>
+      <c r="K24" s="98"/>
       <c r="L24" s="98" t="s">
         <v>780</v>
       </c>
     </row>
-    <row r="25" spans="1:24" s="189" customFormat="1" ht="24">
-      <c r="A25" s="144" t="s">
-        <v>994</v>
-      </c>
-      <c r="B25" s="70" t="s">
-        <v>8</v>
-      </c>
-      <c r="C25" s="187" t="s">
-        <v>168</v>
-      </c>
-      <c r="D25" s="192">
-        <v>1</v>
-      </c>
-      <c r="E25" s="181" t="s">
-        <v>242</v>
-      </c>
+    <row r="25" spans="1:24" s="3" customFormat="1">
+      <c r="A25" s="22" t="s">
+        <v>1020</v>
+      </c>
+      <c r="B25" s="166" t="s">
+        <v>1014</v>
+      </c>
+      <c r="C25" s="167"/>
+      <c r="D25" s="167"/>
+      <c r="E25" s="181"/>
       <c r="F25" s="181"/>
       <c r="G25" s="181"/>
-      <c r="H25" s="70" t="s">
-        <v>1006</v>
-      </c>
-      <c r="I25" s="113"/>
+      <c r="H25" s="70"/>
+      <c r="I25" s="40"/>
       <c r="J25" s="101" t="s">
         <v>385</v>
       </c>
-      <c r="K25" s="98"/>
+      <c r="K25" s="176"/>
       <c r="L25" s="98" t="s">
         <v>780</v>
       </c>
     </row>
-    <row r="26" spans="1:24" s="189" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A26" s="144" t="s">
-        <v>989</v>
-      </c>
-      <c r="B26" s="70" t="s">
-        <v>7</v>
-      </c>
-      <c r="C26" s="167" t="s">
-        <v>1045</v>
-      </c>
-      <c r="D26" s="71">
-        <v>2</v>
-      </c>
-      <c r="E26" s="181" t="s">
-        <v>242</v>
-      </c>
-      <c r="F26" s="171" t="s">
-        <v>247</v>
-      </c>
+    <row r="26" spans="1:24" s="3" customFormat="1">
+      <c r="A26" s="22" t="s">
+        <v>1015</v>
+      </c>
+      <c r="B26" s="166" t="s">
+        <v>1013</v>
+      </c>
+      <c r="C26" s="167"/>
+      <c r="D26" s="167"/>
+      <c r="E26" s="181"/>
+      <c r="F26" s="181"/>
       <c r="G26" s="181"/>
       <c r="H26" s="70"/>
-      <c r="I26" s="113"/>
+      <c r="I26" s="40"/>
       <c r="J26" s="101" t="s">
         <v>385</v>
       </c>
-      <c r="K26" s="98"/>
+      <c r="K26" s="176"/>
       <c r="L26" s="98" t="s">
         <v>780</v>
       </c>
     </row>
-    <row r="27" spans="1:24" s="189" customFormat="1" ht="120">
+    <row r="27" spans="1:24" s="189" customFormat="1" ht="24">
       <c r="A27" s="144" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="B27" s="70" t="s">
         <v>8</v>
@@ -36324,7 +36335,7 @@
         <v>168</v>
       </c>
       <c r="D27" s="192">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E27" s="181" t="s">
         <v>242</v>
@@ -36332,7 +36343,7 @@
       <c r="F27" s="181"/>
       <c r="G27" s="181"/>
       <c r="H27" s="70" t="s">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c r="I27" s="113"/>
       <c r="J27" s="101" t="s">
@@ -36343,118 +36354,134 @@
         <v>780</v>
       </c>
     </row>
-    <row r="28" spans="1:24" ht="96">
-      <c r="A28" s="16" t="s">
-        <v>232</v>
-      </c>
-      <c r="B28" s="57" t="s">
-        <v>27</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>168</v>
-      </c>
-      <c r="D28" s="57" t="s">
-        <v>362</v>
-      </c>
-      <c r="E28" s="58" t="s">
+    <row r="28" spans="1:24" s="189" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A28" s="144" t="s">
+        <v>989</v>
+      </c>
+      <c r="B28" s="70" t="s">
+        <v>7</v>
+      </c>
+      <c r="C28" s="167" t="s">
+        <v>1045</v>
+      </c>
+      <c r="D28" s="71">
+        <v>2</v>
+      </c>
+      <c r="E28" s="181" t="s">
         <v>242</v>
       </c>
-      <c r="F28" s="58" t="s">
-        <v>243</v>
-      </c>
-      <c r="G28" s="58"/>
-      <c r="H28" s="70" t="s">
-        <v>244</v>
-      </c>
-      <c r="I28" s="37"/>
+      <c r="F28" s="171" t="s">
+        <v>247</v>
+      </c>
+      <c r="G28" s="181"/>
+      <c r="H28" s="70"/>
+      <c r="I28" s="113"/>
       <c r="J28" s="101" t="s">
         <v>385</v>
       </c>
-      <c r="K28" s="75"/>
+      <c r="K28" s="98"/>
       <c r="L28" s="98" t="s">
         <v>780</v>
       </c>
-      <c r="M28" s="3"/>
-      <c r="N28" s="3"/>
-      <c r="O28" s="3"/>
-      <c r="P28" s="3"/>
-      <c r="Q28" s="3"/>
-      <c r="R28" s="3"/>
-      <c r="S28" s="3"/>
-      <c r="T28" s="3"/>
-      <c r="U28" s="3"/>
-      <c r="V28" s="3"/>
-      <c r="W28" s="3"/>
-      <c r="X28" s="3"/>
-    </row>
-    <row r="29" spans="1:24" s="3" customFormat="1">
+    </row>
+    <row r="29" spans="1:24" s="189" customFormat="1" ht="120">
       <c r="A29" s="144" t="s">
-        <v>1033</v>
-      </c>
-      <c r="B29" s="166" t="s">
-        <v>1034</v>
-      </c>
-      <c r="C29" s="167" t="s">
+        <v>995</v>
+      </c>
+      <c r="B29" s="70" t="s">
+        <v>8</v>
+      </c>
+      <c r="C29" s="187" t="s">
         <v>168</v>
       </c>
-      <c r="D29" s="166" t="s">
-        <v>1056</v>
+      <c r="D29" s="192">
+        <v>0</v>
       </c>
       <c r="E29" s="181" t="s">
         <v>242</v>
       </c>
-      <c r="F29" s="181" t="s">
-        <v>243</v>
-      </c>
+      <c r="F29" s="181"/>
       <c r="G29" s="181"/>
       <c r="H29" s="70" t="s">
-        <v>1035</v>
-      </c>
-      <c r="I29" s="37"/>
+        <v>1005</v>
+      </c>
+      <c r="I29" s="113"/>
       <c r="J29" s="101" t="s">
         <v>385</v>
       </c>
-      <c r="K29" s="176"/>
+      <c r="K29" s="98"/>
       <c r="L29" s="98" t="s">
         <v>780</v>
       </c>
     </row>
-    <row r="30" spans="1:24" s="3" customFormat="1">
-      <c r="A30" s="22" t="s">
-        <v>1023</v>
-      </c>
-      <c r="B30" s="166" t="s">
-        <v>1013</v>
-      </c>
-      <c r="C30" s="167"/>
-      <c r="D30" s="167"/>
-      <c r="E30" s="181"/>
-      <c r="F30" s="181"/>
-      <c r="G30" s="181"/>
-      <c r="H30" s="70"/>
-      <c r="I30" s="40"/>
+    <row r="30" spans="1:24" ht="96">
+      <c r="A30" s="16" t="s">
+        <v>232</v>
+      </c>
+      <c r="B30" s="57" t="s">
+        <v>27</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="D30" s="57" t="s">
+        <v>362</v>
+      </c>
+      <c r="E30" s="58" t="s">
+        <v>242</v>
+      </c>
+      <c r="F30" s="58" t="s">
+        <v>243</v>
+      </c>
+      <c r="G30" s="58"/>
+      <c r="H30" s="70" t="s">
+        <v>244</v>
+      </c>
+      <c r="I30" s="37"/>
       <c r="J30" s="101" t="s">
         <v>385</v>
       </c>
-      <c r="K30" s="176"/>
+      <c r="K30" s="75"/>
       <c r="L30" s="98" t="s">
         <v>780</v>
       </c>
+      <c r="M30" s="3"/>
+      <c r="N30" s="3"/>
+      <c r="O30" s="3"/>
+      <c r="P30" s="3"/>
+      <c r="Q30" s="3"/>
+      <c r="R30" s="3"/>
+      <c r="S30" s="3"/>
+      <c r="T30" s="3"/>
+      <c r="U30" s="3"/>
+      <c r="V30" s="3"/>
+      <c r="W30" s="3"/>
+      <c r="X30" s="3"/>
     </row>
     <row r="31" spans="1:24" s="3" customFormat="1">
-      <c r="A31" s="22" t="s">
-        <v>1022</v>
+      <c r="A31" s="144" t="s">
+        <v>1033</v>
       </c>
       <c r="B31" s="166" t="s">
-        <v>1013</v>
-      </c>
-      <c r="C31" s="167"/>
-      <c r="D31" s="167"/>
-      <c r="E31" s="181"/>
-      <c r="F31" s="181"/>
+        <v>1034</v>
+      </c>
+      <c r="C31" s="167" t="s">
+        <v>168</v>
+      </c>
+      <c r="D31" s="166" t="s">
+        <v>1056</v>
+      </c>
+      <c r="E31" s="181" t="s">
+        <v>242</v>
+      </c>
+      <c r="F31" s="181" t="s">
+        <v>243</v>
+      </c>
       <c r="G31" s="181"/>
-      <c r="H31" s="70"/>
-      <c r="I31" s="40"/>
+      <c r="H31" s="70" t="s">
+        <v>1035</v>
+      </c>
+      <c r="I31" s="37"/>
       <c r="J31" s="101" t="s">
         <v>385</v>
       </c>
@@ -36463,62 +36490,38 @@
         <v>780</v>
       </c>
     </row>
-    <row r="32" spans="1:24" ht="36">
-      <c r="A32" s="16" t="s">
-        <v>233</v>
-      </c>
-      <c r="B32" s="60" t="s">
-        <v>361</v>
-      </c>
-      <c r="C32" s="6" t="s">
-        <v>168</v>
-      </c>
-      <c r="D32" s="60" t="s">
-        <v>1024</v>
-      </c>
-      <c r="E32" s="30" t="s">
-        <v>1009</v>
-      </c>
-      <c r="F32" s="56" t="s">
-        <v>1010</v>
-      </c>
-      <c r="G32" s="58"/>
+    <row r="32" spans="1:24" s="3" customFormat="1">
+      <c r="A32" s="22" t="s">
+        <v>1023</v>
+      </c>
+      <c r="B32" s="166" t="s">
+        <v>1013</v>
+      </c>
+      <c r="C32" s="167"/>
+      <c r="D32" s="167"/>
+      <c r="E32" s="181"/>
+      <c r="F32" s="181"/>
+      <c r="G32" s="181"/>
       <c r="H32" s="70"/>
-      <c r="I32" s="39"/>
+      <c r="I32" s="40"/>
       <c r="J32" s="101" t="s">
         <v>385</v>
       </c>
-      <c r="K32" s="75"/>
-      <c r="L32" s="75" t="s">
+      <c r="K32" s="176"/>
+      <c r="L32" s="98" t="s">
         <v>780</v>
       </c>
-      <c r="M32" s="3"/>
-      <c r="N32" s="3"/>
-      <c r="O32" s="3"/>
-      <c r="P32" s="3"/>
-      <c r="Q32" s="3"/>
-      <c r="R32" s="3"/>
-      <c r="S32" s="3"/>
-      <c r="T32" s="3"/>
-      <c r="U32" s="3"/>
-      <c r="V32" s="3"/>
-      <c r="W32" s="3"/>
-      <c r="X32" s="3"/>
     </row>
     <row r="33" spans="1:24" s="3" customFormat="1">
-      <c r="A33" s="200" t="s">
-        <v>1043</v>
-      </c>
-      <c r="B33" s="166"/>
-      <c r="C33" s="167" t="s">
-        <v>168</v>
-      </c>
-      <c r="D33" s="167">
-        <v>0</v>
-      </c>
-      <c r="E33" s="181" t="s">
-        <v>1044</v>
-      </c>
+      <c r="A33" s="22" t="s">
+        <v>1022</v>
+      </c>
+      <c r="B33" s="166" t="s">
+        <v>1013</v>
+      </c>
+      <c r="C33" s="167"/>
+      <c r="D33" s="167"/>
+      <c r="E33" s="181"/>
       <c r="F33" s="181"/>
       <c r="G33" s="181"/>
       <c r="H33" s="70"/>
@@ -36531,122 +36534,104 @@
         <v>780</v>
       </c>
     </row>
-    <row r="34" spans="1:24" s="76" customFormat="1">
-      <c r="A34" s="22" t="s">
-        <v>1040</v>
-      </c>
-      <c r="B34" s="73"/>
-      <c r="C34" s="73"/>
-      <c r="D34" s="73"/>
-      <c r="E34" s="73"/>
-      <c r="F34" s="73"/>
-      <c r="G34" s="181"/>
+    <row r="34" spans="1:24" ht="36">
+      <c r="A34" s="16" t="s">
+        <v>233</v>
+      </c>
+      <c r="B34" s="60" t="s">
+        <v>361</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="D34" s="60" t="s">
+        <v>1024</v>
+      </c>
+      <c r="E34" s="30" t="s">
+        <v>1009</v>
+      </c>
+      <c r="F34" s="56" t="s">
+        <v>1010</v>
+      </c>
+      <c r="G34" s="58"/>
       <c r="H34" s="70"/>
-      <c r="I34" s="38"/>
+      <c r="I34" s="39"/>
       <c r="J34" s="101" t="s">
         <v>385</v>
       </c>
-      <c r="K34" s="176"/>
-      <c r="L34" s="98" t="s">
+      <c r="K34" s="75"/>
+      <c r="L34" s="75" t="s">
         <v>780</v>
       </c>
-    </row>
-    <row r="35" spans="1:24" ht="24">
-      <c r="A35" s="16" t="s">
-        <v>234</v>
-      </c>
-      <c r="B35" s="57"/>
-      <c r="C35" s="6" t="s">
+      <c r="M34" s="3"/>
+      <c r="N34" s="3"/>
+      <c r="O34" s="3"/>
+      <c r="P34" s="3"/>
+      <c r="Q34" s="3"/>
+      <c r="R34" s="3"/>
+      <c r="S34" s="3"/>
+      <c r="T34" s="3"/>
+      <c r="U34" s="3"/>
+      <c r="V34" s="3"/>
+      <c r="W34" s="3"/>
+      <c r="X34" s="3"/>
+    </row>
+    <row r="35" spans="1:24" s="3" customFormat="1">
+      <c r="A35" s="200" t="s">
+        <v>1043</v>
+      </c>
+      <c r="B35" s="166"/>
+      <c r="C35" s="167" t="s">
         <v>168</v>
       </c>
-      <c r="D35" s="58">
-        <v>0.23</v>
-      </c>
-      <c r="E35" s="58" t="s">
-        <v>242</v>
-      </c>
-      <c r="F35" s="56" t="s">
-        <v>247</v>
-      </c>
-      <c r="G35" s="58"/>
-      <c r="H35" s="70" t="s">
-        <v>321</v>
-      </c>
-      <c r="I35" s="36"/>
+      <c r="D35" s="167">
+        <v>0</v>
+      </c>
+      <c r="E35" s="181" t="s">
+        <v>1044</v>
+      </c>
+      <c r="F35" s="181"/>
+      <c r="G35" s="181"/>
+      <c r="H35" s="70"/>
+      <c r="I35" s="40"/>
       <c r="J35" s="101" t="s">
         <v>385</v>
       </c>
-      <c r="K35" s="75"/>
+      <c r="K35" s="176"/>
       <c r="L35" s="98" t="s">
         <v>780</v>
       </c>
-      <c r="M35" s="3"/>
-      <c r="N35" s="3"/>
-      <c r="O35" s="3"/>
-      <c r="P35" s="3"/>
-      <c r="Q35" s="3"/>
-      <c r="R35" s="3"/>
-      <c r="S35" s="3"/>
-      <c r="T35" s="3"/>
-      <c r="U35" s="3"/>
-      <c r="V35" s="3"/>
-      <c r="W35" s="3"/>
-      <c r="X35" s="3"/>
-    </row>
-    <row r="36" spans="1:24">
-      <c r="A36" s="16" t="s">
-        <v>235</v>
-      </c>
-      <c r="B36" s="57" t="s">
-        <v>7</v>
-      </c>
-      <c r="C36" s="197" t="s">
-        <v>1045</v>
-      </c>
-      <c r="D36" s="6">
-        <v>7</v>
-      </c>
-      <c r="E36" s="58" t="s">
-        <v>242</v>
-      </c>
-      <c r="F36" s="56" t="s">
-        <v>247</v>
-      </c>
-      <c r="G36" s="58"/>
+    </row>
+    <row r="36" spans="1:24" s="76" customFormat="1">
+      <c r="A36" s="22" t="s">
+        <v>1040</v>
+      </c>
+      <c r="B36" s="73"/>
+      <c r="C36" s="73"/>
+      <c r="D36" s="73"/>
+      <c r="E36" s="73"/>
+      <c r="F36" s="73"/>
+      <c r="G36" s="181"/>
       <c r="H36" s="70"/>
-      <c r="I36" s="40"/>
+      <c r="I36" s="38"/>
       <c r="J36" s="101" t="s">
         <v>385</v>
       </c>
-      <c r="K36" s="75"/>
-      <c r="L36" s="75" t="s">
-        <v>779</v>
-      </c>
-      <c r="M36" s="3"/>
-      <c r="N36" s="3"/>
-      <c r="O36" s="3"/>
-      <c r="P36" s="3"/>
-      <c r="Q36" s="3"/>
-      <c r="R36" s="3"/>
-      <c r="S36" s="3"/>
-      <c r="T36" s="3"/>
-      <c r="U36" s="3"/>
-      <c r="V36" s="3"/>
-      <c r="W36" s="3"/>
-      <c r="X36" s="3"/>
+      <c r="K36" s="176"/>
+      <c r="L36" s="98" t="s">
+        <v>780</v>
+      </c>
     </row>
     <row r="37" spans="1:24" ht="24">
       <c r="A37" s="16" t="s">
-        <v>236</v>
-      </c>
-      <c r="B37" s="57" t="s">
-        <v>363</v>
-      </c>
-      <c r="C37" s="197" t="s">
-        <v>1045</v>
-      </c>
-      <c r="D37" s="6">
-        <v>0.08</v>
+        <v>234</v>
+      </c>
+      <c r="B37" s="57"/>
+      <c r="C37" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="D37" s="58">
+        <v>0.23</v>
       </c>
       <c r="E37" s="58" t="s">
         <v>242</v>
@@ -36656,9 +36641,9 @@
       </c>
       <c r="G37" s="58"/>
       <c r="H37" s="70" t="s">
-        <v>245</v>
-      </c>
-      <c r="I37" s="40"/>
+        <v>321</v>
+      </c>
+      <c r="I37" s="36"/>
       <c r="J37" s="101" t="s">
         <v>385</v>
       </c>
@@ -36679,19 +36664,18 @@
       <c r="W37" s="3"/>
       <c r="X37" s="3"/>
     </row>
-    <row r="38" spans="1:24" ht="24">
+    <row r="38" spans="1:24">
       <c r="A38" s="16" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B38" s="57" t="s">
-        <v>363</v>
+        <v>7</v>
       </c>
       <c r="C38" s="197" t="s">
         <v>1045</v>
       </c>
       <c r="D38" s="6">
-        <f>0.002*12</f>
-        <v>2.4E-2</v>
+        <v>7</v>
       </c>
       <c r="E38" s="58" t="s">
         <v>242</v>
@@ -36700,16 +36684,14 @@
         <v>247</v>
       </c>
       <c r="G38" s="58"/>
-      <c r="H38" s="70" t="s">
-        <v>30</v>
-      </c>
-      <c r="I38" s="41"/>
+      <c r="H38" s="70"/>
+      <c r="I38" s="40"/>
       <c r="J38" s="101" t="s">
         <v>385</v>
       </c>
       <c r="K38" s="75"/>
-      <c r="L38" s="98" t="s">
-        <v>780</v>
+      <c r="L38" s="75" t="s">
+        <v>779</v>
       </c>
       <c r="M38" s="3"/>
       <c r="N38" s="3"/>
@@ -36724,18 +36706,18 @@
       <c r="W38" s="3"/>
       <c r="X38" s="3"/>
     </row>
-    <row r="39" spans="1:24" s="14" customFormat="1" ht="36">
-      <c r="A39" s="48" t="s">
-        <v>238</v>
-      </c>
-      <c r="B39" s="60" t="s">
-        <v>364</v>
+    <row r="39" spans="1:24" ht="24">
+      <c r="A39" s="16" t="s">
+        <v>236</v>
+      </c>
+      <c r="B39" s="57" t="s">
+        <v>363</v>
       </c>
       <c r="C39" s="197" t="s">
         <v>1045</v>
       </c>
-      <c r="D39" s="58">
-        <v>3.3500000000000002E-2</v>
+      <c r="D39" s="6">
+        <v>0.08</v>
       </c>
       <c r="E39" s="58" t="s">
         <v>242</v>
@@ -36745,9 +36727,9 @@
       </c>
       <c r="G39" s="58"/>
       <c r="H39" s="70" t="s">
-        <v>262</v>
-      </c>
-      <c r="I39" s="38"/>
+        <v>245</v>
+      </c>
+      <c r="I39" s="40"/>
       <c r="J39" s="101" t="s">
         <v>385</v>
       </c>
@@ -36755,42 +36737,76 @@
       <c r="L39" s="98" t="s">
         <v>780</v>
       </c>
-    </row>
-    <row r="40" spans="1:24" s="3" customFormat="1">
-      <c r="A40" s="22" t="s">
-        <v>1019</v>
-      </c>
-      <c r="B40" s="166" t="s">
-        <v>1014</v>
-      </c>
-      <c r="C40" s="167"/>
-      <c r="D40" s="167"/>
-      <c r="E40" s="181"/>
-      <c r="F40" s="181"/>
-      <c r="G40" s="181"/>
-      <c r="H40" s="70"/>
-      <c r="I40" s="40"/>
+      <c r="M39" s="3"/>
+      <c r="N39" s="3"/>
+      <c r="O39" s="3"/>
+      <c r="P39" s="3"/>
+      <c r="Q39" s="3"/>
+      <c r="R39" s="3"/>
+      <c r="S39" s="3"/>
+      <c r="T39" s="3"/>
+      <c r="U39" s="3"/>
+      <c r="V39" s="3"/>
+      <c r="W39" s="3"/>
+      <c r="X39" s="3"/>
+    </row>
+    <row r="40" spans="1:24" ht="24">
+      <c r="A40" s="16" t="s">
+        <v>237</v>
+      </c>
+      <c r="B40" s="57" t="s">
+        <v>363</v>
+      </c>
+      <c r="C40" s="197" t="s">
+        <v>1045</v>
+      </c>
+      <c r="D40" s="6">
+        <f>0.002*12</f>
+        <v>2.4E-2</v>
+      </c>
+      <c r="E40" s="58" t="s">
+        <v>242</v>
+      </c>
+      <c r="F40" s="56" t="s">
+        <v>247</v>
+      </c>
+      <c r="G40" s="58"/>
+      <c r="H40" s="70" t="s">
+        <v>30</v>
+      </c>
+      <c r="I40" s="41"/>
       <c r="J40" s="101" t="s">
         <v>385</v>
       </c>
-      <c r="K40" s="176"/>
+      <c r="K40" s="75"/>
       <c r="L40" s="98" t="s">
         <v>780</v>
       </c>
-    </row>
-    <row r="41" spans="1:24" ht="45.75" customHeight="1">
-      <c r="A41" s="16" t="s">
-        <v>239</v>
-      </c>
-      <c r="B41" s="57" t="s">
-        <v>363</v>
+      <c r="M40" s="3"/>
+      <c r="N40" s="3"/>
+      <c r="O40" s="3"/>
+      <c r="P40" s="3"/>
+      <c r="Q40" s="3"/>
+      <c r="R40" s="3"/>
+      <c r="S40" s="3"/>
+      <c r="T40" s="3"/>
+      <c r="U40" s="3"/>
+      <c r="V40" s="3"/>
+      <c r="W40" s="3"/>
+      <c r="X40" s="3"/>
+    </row>
+    <row r="41" spans="1:24" s="14" customFormat="1" ht="36">
+      <c r="A41" s="48" t="s">
+        <v>238</v>
+      </c>
+      <c r="B41" s="60" t="s">
+        <v>364</v>
       </c>
       <c r="C41" s="197" t="s">
         <v>1045</v>
       </c>
-      <c r="D41" s="6">
-        <f>0.007*12</f>
-        <v>8.4000000000000005E-2</v>
+      <c r="D41" s="58">
+        <v>3.3500000000000002E-2</v>
       </c>
       <c r="E41" s="58" t="s">
         <v>242</v>
@@ -36800,35 +36816,23 @@
       </c>
       <c r="G41" s="58"/>
       <c r="H41" s="70" t="s">
-        <v>261</v>
-      </c>
-      <c r="I41" s="40"/>
+        <v>262</v>
+      </c>
+      <c r="I41" s="38"/>
       <c r="J41" s="101" t="s">
         <v>385</v>
       </c>
       <c r="K41" s="75"/>
-      <c r="L41" s="75" t="s">
+      <c r="L41" s="98" t="s">
         <v>780</v>
       </c>
-      <c r="M41" s="3"/>
-      <c r="N41" s="3"/>
-      <c r="O41" s="3"/>
-      <c r="P41" s="3"/>
-      <c r="Q41" s="3"/>
-      <c r="R41" s="3"/>
-      <c r="S41" s="3"/>
-      <c r="T41" s="3"/>
-      <c r="U41" s="3"/>
-      <c r="V41" s="3"/>
-      <c r="W41" s="3"/>
-      <c r="X41" s="3"/>
     </row>
     <row r="42" spans="1:24" s="3" customFormat="1">
       <c r="A42" s="22" t="s">
-        <v>1016</v>
+        <v>1019</v>
       </c>
       <c r="B42" s="166" t="s">
-        <v>1013</v>
+        <v>1014</v>
       </c>
       <c r="C42" s="167"/>
       <c r="D42" s="167"/>
@@ -36845,55 +36849,62 @@
         <v>780</v>
       </c>
     </row>
-    <row r="43" spans="1:24" s="3" customFormat="1">
-      <c r="A43" s="144" t="s">
-        <v>1027</v>
-      </c>
-      <c r="B43" s="81" t="s">
-        <v>8</v>
-      </c>
-      <c r="C43" s="147" t="s">
-        <v>1054</v>
-      </c>
-      <c r="D43" s="167">
-        <v>-1</v>
-      </c>
-      <c r="E43" s="181" t="s">
+    <row r="43" spans="1:24" ht="45.75" customHeight="1">
+      <c r="A43" s="16" t="s">
+        <v>239</v>
+      </c>
+      <c r="B43" s="57" t="s">
+        <v>363</v>
+      </c>
+      <c r="C43" s="197" t="s">
+        <v>1045</v>
+      </c>
+      <c r="D43" s="6">
+        <f>0.007*12</f>
+        <v>8.4000000000000005E-2</v>
+      </c>
+      <c r="E43" s="58" t="s">
         <v>242</v>
       </c>
-      <c r="F43" s="181" t="s">
-        <v>1008</v>
-      </c>
-      <c r="G43" s="181"/>
-      <c r="H43" s="70"/>
+      <c r="F43" s="56" t="s">
+        <v>247</v>
+      </c>
+      <c r="G43" s="58"/>
+      <c r="H43" s="70" t="s">
+        <v>261</v>
+      </c>
       <c r="I43" s="40"/>
       <c r="J43" s="101" t="s">
         <v>385</v>
       </c>
-      <c r="K43" s="176"/>
-      <c r="L43" s="98" t="s">
+      <c r="K43" s="75"/>
+      <c r="L43" s="75" t="s">
         <v>780</v>
       </c>
+      <c r="M43" s="3"/>
+      <c r="N43" s="3"/>
+      <c r="O43" s="3"/>
+      <c r="P43" s="3"/>
+      <c r="Q43" s="3"/>
+      <c r="R43" s="3"/>
+      <c r="S43" s="3"/>
+      <c r="T43" s="3"/>
+      <c r="U43" s="3"/>
+      <c r="V43" s="3"/>
+      <c r="W43" s="3"/>
+      <c r="X43" s="3"/>
     </row>
     <row r="44" spans="1:24" s="3" customFormat="1">
-      <c r="A44" s="144" t="s">
-        <v>1027</v>
-      </c>
-      <c r="B44" s="81" t="s">
-        <v>8</v>
-      </c>
-      <c r="C44" s="147" t="s">
-        <v>1055</v>
-      </c>
-      <c r="D44" s="167">
-        <v>1</v>
-      </c>
-      <c r="E44" s="181" t="s">
-        <v>242</v>
-      </c>
-      <c r="F44" s="181" t="s">
-        <v>1008</v>
-      </c>
+      <c r="A44" s="22" t="s">
+        <v>1016</v>
+      </c>
+      <c r="B44" s="166" t="s">
+        <v>1013</v>
+      </c>
+      <c r="C44" s="167"/>
+      <c r="D44" s="167"/>
+      <c r="E44" s="181"/>
+      <c r="F44" s="181"/>
       <c r="G44" s="181"/>
       <c r="H44" s="70"/>
       <c r="I44" s="40"/>
@@ -36907,22 +36918,22 @@
     </row>
     <row r="45" spans="1:24" s="3" customFormat="1">
       <c r="A45" s="144" t="s">
-        <v>1028</v>
-      </c>
-      <c r="B45" s="166" t="s">
+        <v>1027</v>
+      </c>
+      <c r="B45" s="81" t="s">
         <v>8</v>
       </c>
-      <c r="C45" s="212" t="s">
+      <c r="C45" s="147" t="s">
         <v>1054</v>
       </c>
       <c r="D45" s="167">
-        <v>5.2</v>
+        <v>-1</v>
       </c>
       <c r="E45" s="181" t="s">
-        <v>93</v>
+        <v>242</v>
       </c>
       <c r="F45" s="181" t="s">
-        <v>241</v>
+        <v>1008</v>
       </c>
       <c r="G45" s="181"/>
       <c r="H45" s="70"/>
@@ -36937,22 +36948,22 @@
     </row>
     <row r="46" spans="1:24" s="3" customFormat="1">
       <c r="A46" s="144" t="s">
-        <v>1028</v>
-      </c>
-      <c r="B46" s="166" t="s">
+        <v>1027</v>
+      </c>
+      <c r="B46" s="81" t="s">
         <v>8</v>
       </c>
-      <c r="C46" s="212" t="s">
+      <c r="C46" s="147" t="s">
         <v>1055</v>
       </c>
       <c r="D46" s="167">
-        <v>7.2</v>
+        <v>1</v>
       </c>
       <c r="E46" s="181" t="s">
-        <v>93</v>
+        <v>242</v>
       </c>
       <c r="F46" s="181" t="s">
-        <v>241</v>
+        <v>1008</v>
       </c>
       <c r="G46" s="181"/>
       <c r="H46" s="70"/>
@@ -36965,29 +36976,27 @@
         <v>780</v>
       </c>
     </row>
-    <row r="47" spans="1:24" s="189" customFormat="1" ht="24">
+    <row r="47" spans="1:24" s="3" customFormat="1">
       <c r="A47" s="144" t="s">
-        <v>1029</v>
-      </c>
-      <c r="B47" s="81" t="s">
+        <v>1028</v>
+      </c>
+      <c r="B47" s="166" t="s">
         <v>8</v>
       </c>
       <c r="C47" s="212" t="s">
         <v>1054</v>
       </c>
-      <c r="D47" s="190">
-        <v>-8</v>
+      <c r="D47" s="167">
+        <v>5.2</v>
       </c>
       <c r="E47" s="181" t="s">
-        <v>242</v>
-      </c>
-      <c r="F47" s="171" t="s">
-        <v>997</v>
+        <v>93</v>
+      </c>
+      <c r="F47" s="181" t="s">
+        <v>241</v>
       </c>
       <c r="G47" s="181"/>
-      <c r="H47" s="70" t="s">
-        <v>1004</v>
-      </c>
+      <c r="H47" s="70"/>
       <c r="I47" s="40"/>
       <c r="J47" s="101" t="s">
         <v>385</v>
@@ -36997,29 +37006,27 @@
         <v>780</v>
       </c>
     </row>
-    <row r="48" spans="1:24" s="189" customFormat="1" ht="24">
+    <row r="48" spans="1:24" s="3" customFormat="1">
       <c r="A48" s="144" t="s">
-        <v>1029</v>
-      </c>
-      <c r="B48" s="81" t="s">
+        <v>1028</v>
+      </c>
+      <c r="B48" s="166" t="s">
         <v>8</v>
       </c>
       <c r="C48" s="212" t="s">
         <v>1055</v>
       </c>
-      <c r="D48" s="190">
-        <v>-5</v>
+      <c r="D48" s="167">
+        <v>7.2</v>
       </c>
       <c r="E48" s="181" t="s">
-        <v>242</v>
-      </c>
-      <c r="F48" s="171" t="s">
-        <v>997</v>
+        <v>93</v>
+      </c>
+      <c r="F48" s="181" t="s">
+        <v>241</v>
       </c>
       <c r="G48" s="181"/>
-      <c r="H48" s="70" t="s">
-        <v>1004</v>
-      </c>
+      <c r="H48" s="70"/>
       <c r="I48" s="40"/>
       <c r="J48" s="101" t="s">
         <v>385</v>
@@ -37029,69 +37036,61 @@
         <v>780</v>
       </c>
     </row>
-    <row r="49" spans="1:24">
-      <c r="A49" s="16" t="s">
-        <v>240</v>
-      </c>
-      <c r="B49" s="57" t="s">
+    <row r="49" spans="1:24" s="189" customFormat="1" ht="24">
+      <c r="A49" s="144" t="s">
+        <v>1029</v>
+      </c>
+      <c r="B49" s="81" t="s">
         <v>8</v>
       </c>
       <c r="C49" s="212" t="s">
         <v>1054</v>
       </c>
-      <c r="D49" s="6">
-        <v>5</v>
-      </c>
-      <c r="E49" s="58" t="s">
-        <v>93</v>
-      </c>
-      <c r="F49" s="58" t="s">
-        <v>241</v>
-      </c>
-      <c r="G49" s="58"/>
-      <c r="H49" s="70"/>
+      <c r="D49" s="190">
+        <v>-8</v>
+      </c>
+      <c r="E49" s="181" t="s">
+        <v>242</v>
+      </c>
+      <c r="F49" s="171" t="s">
+        <v>997</v>
+      </c>
+      <c r="G49" s="181"/>
+      <c r="H49" s="70" t="s">
+        <v>1004</v>
+      </c>
       <c r="I49" s="40"/>
       <c r="J49" s="101" t="s">
         <v>385</v>
       </c>
-      <c r="K49" s="75"/>
+      <c r="K49" s="176"/>
       <c r="L49" s="98" t="s">
         <v>780</v>
       </c>
-      <c r="M49" s="3"/>
-      <c r="N49" s="3"/>
-      <c r="O49" s="3"/>
-      <c r="P49" s="3"/>
-      <c r="Q49" s="3"/>
-      <c r="R49" s="3"/>
-      <c r="S49" s="3"/>
-      <c r="T49" s="3"/>
-      <c r="U49" s="3"/>
-      <c r="V49" s="3"/>
-      <c r="W49" s="3"/>
-      <c r="X49" s="3"/>
-    </row>
-    <row r="50" spans="1:24" s="3" customFormat="1">
+    </row>
+    <row r="50" spans="1:24" s="189" customFormat="1" ht="24">
       <c r="A50" s="144" t="s">
-        <v>240</v>
-      </c>
-      <c r="B50" s="166" t="s">
+        <v>1029</v>
+      </c>
+      <c r="B50" s="81" t="s">
         <v>8</v>
       </c>
       <c r="C50" s="212" t="s">
         <v>1055</v>
       </c>
-      <c r="D50" s="167">
-        <v>7.5</v>
+      <c r="D50" s="190">
+        <v>-5</v>
       </c>
       <c r="E50" s="181" t="s">
-        <v>93</v>
-      </c>
-      <c r="F50" s="181" t="s">
-        <v>241</v>
+        <v>242</v>
+      </c>
+      <c r="F50" s="171" t="s">
+        <v>997</v>
       </c>
       <c r="G50" s="181"/>
-      <c r="H50" s="70"/>
+      <c r="H50" s="70" t="s">
+        <v>1004</v>
+      </c>
       <c r="I50" s="40"/>
       <c r="J50" s="101" t="s">
         <v>385</v>
@@ -37101,9 +37100,9 @@
         <v>780</v>
       </c>
     </row>
-    <row r="51" spans="1:24" s="3" customFormat="1" ht="24">
-      <c r="A51" s="144" t="s">
-        <v>1025</v>
+    <row r="51" spans="1:24" s="189" customFormat="1">
+      <c r="A51" s="200" t="s">
+        <v>1061</v>
       </c>
       <c r="B51" s="81" t="s">
         <v>8</v>
@@ -37111,31 +37110,29 @@
       <c r="C51" s="212" t="s">
         <v>1054</v>
       </c>
-      <c r="D51" s="167">
-        <v>0</v>
-      </c>
-      <c r="E51" s="181" t="s">
-        <v>1030</v>
-      </c>
-      <c r="F51" s="181" t="s">
-        <v>1031</v>
-      </c>
-      <c r="G51" s="181" t="s">
-        <v>1032</v>
-      </c>
-      <c r="H51" s="70"/>
+      <c r="D51" s="223">
+        <v>-5.4</v>
+      </c>
+      <c r="E51" s="211" t="s">
+        <v>93</v>
+      </c>
+      <c r="F51" s="195"/>
+      <c r="G51" s="211"/>
+      <c r="H51" s="70" t="s">
+        <v>1062</v>
+      </c>
       <c r="I51" s="40"/>
       <c r="J51" s="101" t="s">
         <v>385</v>
       </c>
-      <c r="K51" s="176"/>
+      <c r="K51" s="214"/>
       <c r="L51" s="98" t="s">
         <v>780</v>
       </c>
     </row>
-    <row r="52" spans="1:24" s="3" customFormat="1" ht="24">
-      <c r="A52" s="144" t="s">
-        <v>1025</v>
+    <row r="52" spans="1:24" s="189" customFormat="1">
+      <c r="A52" s="200" t="s">
+        <v>1061</v>
       </c>
       <c r="B52" s="81" t="s">
         <v>8</v>
@@ -37143,76 +37140,84 @@
       <c r="C52" s="212" t="s">
         <v>1055</v>
       </c>
-      <c r="D52" s="167">
+      <c r="D52" s="223">
         <v>0</v>
       </c>
-      <c r="E52" s="181" t="s">
-        <v>1030</v>
-      </c>
-      <c r="F52" s="181" t="s">
-        <v>1031</v>
-      </c>
-      <c r="G52" s="181" t="s">
-        <v>1032</v>
-      </c>
+      <c r="E52" s="211" t="s">
+        <v>93</v>
+      </c>
+      <c r="F52" s="195"/>
+      <c r="G52" s="211"/>
       <c r="H52" s="70"/>
       <c r="I52" s="40"/>
       <c r="J52" s="101" t="s">
         <v>385</v>
       </c>
-      <c r="K52" s="176"/>
+      <c r="K52" s="214"/>
       <c r="L52" s="98" t="s">
         <v>780</v>
       </c>
     </row>
-    <row r="53" spans="1:24" s="3" customFormat="1">
-      <c r="A53" s="144" t="s">
-        <v>1026</v>
-      </c>
-      <c r="B53" s="81" t="s">
+    <row r="53" spans="1:24">
+      <c r="A53" s="16" t="s">
+        <v>240</v>
+      </c>
+      <c r="B53" s="57" t="s">
         <v>8</v>
       </c>
       <c r="C53" s="212" t="s">
         <v>1054</v>
       </c>
-      <c r="D53" s="167">
-        <v>-1</v>
-      </c>
-      <c r="E53" s="181" t="s">
-        <v>242</v>
-      </c>
-      <c r="F53" s="181" t="s">
-        <v>1008</v>
-      </c>
-      <c r="G53" s="181"/>
+      <c r="D53" s="6">
+        <v>5</v>
+      </c>
+      <c r="E53" s="58" t="s">
+        <v>93</v>
+      </c>
+      <c r="F53" s="58" t="s">
+        <v>241</v>
+      </c>
+      <c r="G53" s="58"/>
       <c r="H53" s="70"/>
       <c r="I53" s="40"/>
       <c r="J53" s="101" t="s">
         <v>385</v>
       </c>
-      <c r="K53" s="176"/>
+      <c r="K53" s="75"/>
       <c r="L53" s="98" t="s">
         <v>780</v>
       </c>
+      <c r="M53" s="3"/>
+      <c r="N53" s="3"/>
+      <c r="O53" s="3"/>
+      <c r="P53" s="3"/>
+      <c r="Q53" s="3"/>
+      <c r="R53" s="3"/>
+      <c r="S53" s="3"/>
+      <c r="T53" s="3"/>
+      <c r="U53" s="3"/>
+      <c r="V53" s="3"/>
+      <c r="W53" s="3"/>
+      <c r="X53" s="3"/>
     </row>
     <row r="54" spans="1:24" s="3" customFormat="1">
       <c r="A54" s="144" t="s">
-        <v>1026</v>
-      </c>
-      <c r="B54" s="81" t="s">
+        <v>240</v>
+      </c>
+      <c r="B54" s="166" t="s">
         <v>8</v>
       </c>
       <c r="C54" s="212" t="s">
         <v>1055</v>
       </c>
       <c r="D54" s="167">
-        <v>1</v>
+        <v>7.5</v>
       </c>
       <c r="E54" s="181" t="s">
-        <v>242</v>
+        <v>93</v>
       </c>
       <c r="F54" s="181" t="s">
-        <v>1008</v>
+        <v>241</v>
       </c>
       <c r="G54" s="181"/>
       <c r="H54" s="70"/>
@@ -37225,226 +37230,226 @@
         <v>780</v>
       </c>
     </row>
-    <row r="55" spans="1:24" s="14" customFormat="1">
-      <c r="A55" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="B55" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="C55" s="49" t="s">
-        <v>222</v>
-      </c>
-      <c r="D55" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="E55" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="F55" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="G55" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="H55" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="I55" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="J55" s="67" t="s">
-        <v>370</v>
-      </c>
-      <c r="K55" s="67" t="s">
-        <v>411</v>
-      </c>
-      <c r="L55" s="67" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="56" spans="1:24" s="3" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A56" s="64" t="s">
-        <v>678</v>
-      </c>
-      <c r="B56" s="57" t="s">
+    <row r="55" spans="1:24" s="3" customFormat="1" ht="24">
+      <c r="A55" s="144" t="s">
+        <v>1025</v>
+      </c>
+      <c r="B55" s="81" t="s">
+        <v>8</v>
+      </c>
+      <c r="C55" s="212" t="s">
+        <v>1054</v>
+      </c>
+      <c r="D55" s="167">
+        <v>0</v>
+      </c>
+      <c r="E55" s="181" t="s">
+        <v>1030</v>
+      </c>
+      <c r="F55" s="181" t="s">
+        <v>1031</v>
+      </c>
+      <c r="G55" s="181" t="s">
+        <v>1032</v>
+      </c>
+      <c r="H55" s="70"/>
+      <c r="I55" s="40"/>
+      <c r="J55" s="101" t="s">
+        <v>385</v>
+      </c>
+      <c r="K55" s="176"/>
+      <c r="L55" s="98" t="s">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="56" spans="1:24" s="3" customFormat="1" ht="24">
+      <c r="A56" s="144" t="s">
+        <v>1025</v>
+      </c>
+      <c r="B56" s="81" t="s">
         <v>8</v>
       </c>
       <c r="C56" s="212" t="s">
         <v>1055</v>
       </c>
-      <c r="D56" s="53" t="s">
-        <v>416</v>
-      </c>
-      <c r="E56" s="58" t="s">
-        <v>93</v>
-      </c>
-      <c r="F56" s="58" t="s">
-        <v>263</v>
-      </c>
-      <c r="G56" s="79" t="s">
-        <v>498</v>
-      </c>
-      <c r="H56" s="61" t="s">
-        <v>264</v>
-      </c>
-      <c r="I56" s="113"/>
+      <c r="D56" s="167">
+        <v>0</v>
+      </c>
+      <c r="E56" s="181" t="s">
+        <v>1030</v>
+      </c>
+      <c r="F56" s="181" t="s">
+        <v>1031</v>
+      </c>
+      <c r="G56" s="181" t="s">
+        <v>1032</v>
+      </c>
+      <c r="H56" s="70"/>
+      <c r="I56" s="40"/>
       <c r="J56" s="101" t="s">
-        <v>386</v>
-      </c>
-      <c r="K56" s="75"/>
-      <c r="L56" s="75" t="s">
-        <v>781</v>
-      </c>
-    </row>
-    <row r="57" spans="1:24" s="3" customFormat="1" ht="24">
-      <c r="A57" s="64" t="s">
-        <v>678</v>
-      </c>
-      <c r="B57" s="57" t="s">
+        <v>385</v>
+      </c>
+      <c r="K56" s="176"/>
+      <c r="L56" s="98" t="s">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="57" spans="1:24" s="3" customFormat="1">
+      <c r="A57" s="144" t="s">
+        <v>1026</v>
+      </c>
+      <c r="B57" s="81" t="s">
         <v>8</v>
       </c>
       <c r="C57" s="212" t="s">
         <v>1054</v>
       </c>
-      <c r="D57" s="53" t="s">
-        <v>417</v>
-      </c>
-      <c r="E57" s="58" t="s">
-        <v>93</v>
-      </c>
-      <c r="F57" s="58" t="s">
-        <v>263</v>
-      </c>
-      <c r="G57" s="79" t="s">
-        <v>498</v>
-      </c>
-      <c r="H57" s="61" t="s">
-        <v>264</v>
-      </c>
-      <c r="I57" s="113"/>
+      <c r="D57" s="167">
+        <v>-1</v>
+      </c>
+      <c r="E57" s="181" t="s">
+        <v>242</v>
+      </c>
+      <c r="F57" s="181" t="s">
+        <v>1008</v>
+      </c>
+      <c r="G57" s="181"/>
+      <c r="H57" s="70"/>
+      <c r="I57" s="40"/>
       <c r="J57" s="101" t="s">
-        <v>386</v>
-      </c>
-      <c r="K57" s="75"/>
-      <c r="L57" s="75" t="s">
-        <v>781</v>
-      </c>
-    </row>
-    <row r="58" spans="1:24" s="3" customFormat="1" ht="24">
-      <c r="A58" s="64" t="s">
-        <v>679</v>
-      </c>
-      <c r="B58" s="57" t="s">
-        <v>5</v>
+        <v>385</v>
+      </c>
+      <c r="K57" s="176"/>
+      <c r="L57" s="98" t="s">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="58" spans="1:24" s="3" customFormat="1">
+      <c r="A58" s="144" t="s">
+        <v>1026</v>
+      </c>
+      <c r="B58" s="81" t="s">
+        <v>8</v>
       </c>
       <c r="C58" s="212" t="s">
         <v>1055</v>
       </c>
-      <c r="D58" s="57" t="s">
-        <v>250</v>
-      </c>
-      <c r="E58" s="30" t="s">
-        <v>251</v>
-      </c>
-      <c r="F58" s="58" t="s">
-        <v>252</v>
-      </c>
-      <c r="G58" s="58"/>
-      <c r="H58" s="61" t="s">
-        <v>248</v>
-      </c>
-      <c r="I58" s="113"/>
+      <c r="D58" s="167">
+        <v>1</v>
+      </c>
+      <c r="E58" s="181" t="s">
+        <v>242</v>
+      </c>
+      <c r="F58" s="181" t="s">
+        <v>1008</v>
+      </c>
+      <c r="G58" s="181"/>
+      <c r="H58" s="70"/>
+      <c r="I58" s="40"/>
       <c r="J58" s="101" t="s">
-        <v>386</v>
-      </c>
-      <c r="K58" s="75"/>
-      <c r="L58" s="75" t="s">
-        <v>782</v>
-      </c>
-    </row>
-    <row r="59" spans="1:24" s="3" customFormat="1">
-      <c r="A59" s="64" t="s">
-        <v>679</v>
-      </c>
-      <c r="B59" s="57" t="s">
-        <v>5</v>
-      </c>
-      <c r="C59" s="212" t="s">
-        <v>1054</v>
-      </c>
-      <c r="D59" s="110">
-        <v>120</v>
-      </c>
-      <c r="E59" s="6" t="s">
-        <v>242</v>
-      </c>
-      <c r="F59" s="58" t="s">
-        <v>253</v>
-      </c>
-      <c r="G59" s="58"/>
-      <c r="H59" s="63"/>
-      <c r="I59" s="114"/>
-      <c r="J59" s="101" t="s">
-        <v>386</v>
-      </c>
-      <c r="K59" s="75"/>
-      <c r="L59" s="75" t="s">
-        <v>782</v>
-      </c>
-    </row>
-    <row r="60" spans="1:24" s="3" customFormat="1">
+        <v>385</v>
+      </c>
+      <c r="K58" s="176"/>
+      <c r="L58" s="98" t="s">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="59" spans="1:24" s="14" customFormat="1">
+      <c r="A59" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B59" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C59" s="49" t="s">
+        <v>222</v>
+      </c>
+      <c r="D59" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="E59" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="F59" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="G59" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="H59" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="I59" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="J59" s="67" t="s">
+        <v>370</v>
+      </c>
+      <c r="K59" s="67" t="s">
+        <v>411</v>
+      </c>
+      <c r="L59" s="67" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="60" spans="1:24" s="3" customFormat="1" ht="25.5" customHeight="1">
       <c r="A60" s="64" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="B60" s="57" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C60" s="212" t="s">
         <v>1055</v>
       </c>
-      <c r="D60" s="6" t="s">
-        <v>255</v>
-      </c>
-      <c r="E60" s="6" t="s">
-        <v>242</v>
+      <c r="D60" s="53" t="s">
+        <v>416</v>
+      </c>
+      <c r="E60" s="58" t="s">
+        <v>93</v>
       </c>
       <c r="F60" s="58" t="s">
-        <v>254</v>
-      </c>
-      <c r="G60" s="58"/>
-      <c r="H60" s="57"/>
+        <v>263</v>
+      </c>
+      <c r="G60" s="79" t="s">
+        <v>498</v>
+      </c>
+      <c r="H60" s="61" t="s">
+        <v>264</v>
+      </c>
       <c r="I60" s="113"/>
       <c r="J60" s="101" t="s">
         <v>386</v>
       </c>
       <c r="K60" s="75"/>
       <c r="L60" s="75" t="s">
-        <v>780</v>
-      </c>
-    </row>
-    <row r="61" spans="1:24" s="3" customFormat="1" ht="30" customHeight="1">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="61" spans="1:24" s="3" customFormat="1" ht="24">
       <c r="A61" s="64" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="B61" s="57" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C61" s="212" t="s">
         <v>1054</v>
       </c>
-      <c r="D61" s="57" t="s">
-        <v>420</v>
-      </c>
-      <c r="E61" s="30" t="s">
-        <v>251</v>
+      <c r="D61" s="53" t="s">
+        <v>417</v>
+      </c>
+      <c r="E61" s="58" t="s">
+        <v>93</v>
       </c>
       <c r="F61" s="58" t="s">
-        <v>252</v>
-      </c>
-      <c r="G61" s="58"/>
+        <v>263</v>
+      </c>
+      <c r="G61" s="79" t="s">
+        <v>498</v>
+      </c>
       <c r="H61" s="61" t="s">
-        <v>249</v>
+        <v>264</v>
       </c>
       <c r="I61" s="113"/>
       <c r="J61" s="101" t="s">
@@ -37452,212 +37457,204 @@
       </c>
       <c r="K61" s="75"/>
       <c r="L61" s="75" t="s">
-        <v>780</v>
-      </c>
-    </row>
-    <row r="62" spans="1:24" s="54" customFormat="1" ht="24">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="62" spans="1:24" s="3" customFormat="1" ht="24">
       <c r="A62" s="64" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="B62" s="57" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C62" s="212" t="s">
         <v>1055</v>
       </c>
-      <c r="D62" s="6">
-        <v>1028.2</v>
-      </c>
-      <c r="E62" s="58" t="s">
-        <v>93</v>
+      <c r="D62" s="57" t="s">
+        <v>250</v>
+      </c>
+      <c r="E62" s="30" t="s">
+        <v>251</v>
       </c>
       <c r="F62" s="58" t="s">
-        <v>241</v>
-      </c>
-      <c r="G62" s="79" t="s">
-        <v>498</v>
-      </c>
+        <v>252</v>
+      </c>
+      <c r="G62" s="58"/>
       <c r="H62" s="61" t="s">
-        <v>13</v>
-      </c>
-      <c r="I62" s="115"/>
+        <v>248</v>
+      </c>
+      <c r="I62" s="113"/>
       <c r="J62" s="101" t="s">
         <v>386</v>
       </c>
       <c r="K62" s="75"/>
       <c r="L62" s="75" t="s">
-        <v>781</v>
-      </c>
-    </row>
-    <row r="63" spans="1:24" s="54" customFormat="1" ht="24">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="63" spans="1:24" s="3" customFormat="1">
       <c r="A63" s="64" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="B63" s="57" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C63" s="212" t="s">
         <v>1054</v>
       </c>
-      <c r="D63" s="6">
-        <v>1025.7</v>
-      </c>
-      <c r="E63" s="58" t="s">
-        <v>93</v>
+      <c r="D63" s="110">
+        <v>120</v>
+      </c>
+      <c r="E63" s="6" t="s">
+        <v>242</v>
       </c>
       <c r="F63" s="58" t="s">
-        <v>241</v>
-      </c>
-      <c r="G63" s="79" t="s">
-        <v>498</v>
-      </c>
-      <c r="H63" s="61" t="s">
-        <v>13</v>
-      </c>
-      <c r="I63" s="115"/>
+        <v>253</v>
+      </c>
+      <c r="G63" s="58"/>
+      <c r="H63" s="63"/>
+      <c r="I63" s="114"/>
       <c r="J63" s="101" t="s">
         <v>386</v>
       </c>
       <c r="K63" s="75"/>
       <c r="L63" s="75" t="s">
-        <v>781</v>
-      </c>
-    </row>
-    <row r="64" spans="1:24" s="54" customFormat="1" ht="24">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="64" spans="1:24" s="3" customFormat="1">
       <c r="A64" s="64" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="B64" s="57" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C64" s="212" t="s">
         <v>1055</v>
       </c>
-      <c r="D64" s="6">
-        <v>1028.2</v>
-      </c>
-      <c r="E64" s="58" t="s">
-        <v>93</v>
+      <c r="D64" s="6" t="s">
+        <v>255</v>
+      </c>
+      <c r="E64" s="6" t="s">
+        <v>242</v>
       </c>
       <c r="F64" s="58" t="s">
-        <v>241</v>
-      </c>
-      <c r="G64" s="79" t="s">
-        <v>498</v>
-      </c>
-      <c r="H64" s="61" t="s">
-        <v>13</v>
-      </c>
-      <c r="I64" s="115"/>
+        <v>254</v>
+      </c>
+      <c r="G64" s="58"/>
+      <c r="H64" s="57"/>
+      <c r="I64" s="113"/>
       <c r="J64" s="101" t="s">
         <v>386</v>
       </c>
       <c r="K64" s="75"/>
       <c r="L64" s="75" t="s">
-        <v>781</v>
-      </c>
-    </row>
-    <row r="65" spans="1:12" s="54" customFormat="1" ht="24">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" s="3" customFormat="1" ht="30" customHeight="1">
       <c r="A65" s="64" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="B65" s="57" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C65" s="212" t="s">
         <v>1054</v>
       </c>
-      <c r="D65" s="6">
-        <v>1025.7</v>
-      </c>
-      <c r="E65" s="58" t="s">
-        <v>93</v>
+      <c r="D65" s="57" t="s">
+        <v>420</v>
+      </c>
+      <c r="E65" s="30" t="s">
+        <v>251</v>
       </c>
       <c r="F65" s="58" t="s">
-        <v>241</v>
-      </c>
-      <c r="G65" s="79" t="s">
-        <v>498</v>
-      </c>
+        <v>252</v>
+      </c>
+      <c r="G65" s="58"/>
       <c r="H65" s="61" t="s">
-        <v>13</v>
-      </c>
-      <c r="I65" s="115"/>
+        <v>249</v>
+      </c>
+      <c r="I65" s="113"/>
       <c r="J65" s="101" t="s">
         <v>386</v>
       </c>
       <c r="K65" s="75"/>
       <c r="L65" s="75" t="s">
-        <v>781</v>
-      </c>
-    </row>
-    <row r="66" spans="1:12" s="3" customFormat="1">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" s="54" customFormat="1" ht="24">
       <c r="A66" s="64" t="s">
-        <v>691</v>
-      </c>
-      <c r="B66" s="60" t="s">
-        <v>364</v>
-      </c>
-      <c r="C66" s="6" t="s">
-        <v>1046</v>
-      </c>
-      <c r="D66" s="111">
-        <v>0.03</v>
-      </c>
-      <c r="E66" s="6" t="s">
-        <v>242</v>
-      </c>
-      <c r="F66" s="56" t="s">
-        <v>247</v>
-      </c>
-      <c r="G66" s="58"/>
-      <c r="H66" s="7" t="s">
-        <v>324</v>
-      </c>
-      <c r="I66" s="116"/>
+        <v>681</v>
+      </c>
+      <c r="B66" s="57" t="s">
+        <v>8</v>
+      </c>
+      <c r="C66" s="212" t="s">
+        <v>1055</v>
+      </c>
+      <c r="D66" s="6">
+        <v>1028.2</v>
+      </c>
+      <c r="E66" s="58" t="s">
+        <v>93</v>
+      </c>
+      <c r="F66" s="58" t="s">
+        <v>241</v>
+      </c>
+      <c r="G66" s="79" t="s">
+        <v>498</v>
+      </c>
+      <c r="H66" s="61" t="s">
+        <v>13</v>
+      </c>
+      <c r="I66" s="115"/>
       <c r="J66" s="101" t="s">
         <v>386</v>
       </c>
       <c r="K66" s="75"/>
       <c r="L66" s="75" t="s">
-        <v>779</v>
-      </c>
-    </row>
-    <row r="67" spans="1:12" s="3" customFormat="1">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" s="54" customFormat="1" ht="24">
       <c r="A67" s="64" t="s">
-        <v>691</v>
-      </c>
-      <c r="B67" s="60" t="s">
-        <v>364</v>
-      </c>
-      <c r="C67" s="6" t="s">
-        <v>1047</v>
-      </c>
-      <c r="D67" s="71">
-        <v>3.6999999999999998E-2</v>
-      </c>
-      <c r="E67" s="6" t="s">
-        <v>242</v>
-      </c>
-      <c r="F67" s="56" t="s">
-        <v>247</v>
-      </c>
-      <c r="G67" s="58"/>
-      <c r="H67" s="7" t="s">
-        <v>260</v>
-      </c>
-      <c r="I67" s="116"/>
+        <v>681</v>
+      </c>
+      <c r="B67" s="57" t="s">
+        <v>8</v>
+      </c>
+      <c r="C67" s="212" t="s">
+        <v>1054</v>
+      </c>
+      <c r="D67" s="6">
+        <v>1025.7</v>
+      </c>
+      <c r="E67" s="58" t="s">
+        <v>93</v>
+      </c>
+      <c r="F67" s="58" t="s">
+        <v>241</v>
+      </c>
+      <c r="G67" s="79" t="s">
+        <v>498</v>
+      </c>
+      <c r="H67" s="61" t="s">
+        <v>13</v>
+      </c>
+      <c r="I67" s="115"/>
       <c r="J67" s="101" t="s">
         <v>386</v>
       </c>
       <c r="K67" s="75"/>
       <c r="L67" s="75" t="s">
-        <v>779</v>
-      </c>
-    </row>
-    <row r="68" spans="1:12" s="3" customFormat="1" ht="24">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" s="54" customFormat="1" ht="24">
       <c r="A68" s="64" t="s">
-        <v>692</v>
+        <v>682</v>
       </c>
       <c r="B68" s="57" t="s">
         <v>8</v>
@@ -37665,22 +37662,22 @@
       <c r="C68" s="212" t="s">
         <v>1055</v>
       </c>
-      <c r="D68" s="57" t="s">
-        <v>418</v>
+      <c r="D68" s="6">
+        <v>1028.2</v>
       </c>
       <c r="E68" s="58" t="s">
-        <v>258</v>
+        <v>93</v>
       </c>
       <c r="F68" s="58" t="s">
-        <v>259</v>
+        <v>241</v>
       </c>
       <c r="G68" s="79" t="s">
         <v>498</v>
       </c>
       <c r="H68" s="61" t="s">
-        <v>268</v>
-      </c>
-      <c r="I68" s="113"/>
+        <v>13</v>
+      </c>
+      <c r="I68" s="115"/>
       <c r="J68" s="101" t="s">
         <v>386</v>
       </c>
@@ -37689,9 +37686,9 @@
         <v>781</v>
       </c>
     </row>
-    <row r="69" spans="1:12" s="3" customFormat="1" ht="24">
+    <row r="69" spans="1:12" s="54" customFormat="1" ht="24">
       <c r="A69" s="64" t="s">
-        <v>692</v>
+        <v>682</v>
       </c>
       <c r="B69" s="57" t="s">
         <v>8</v>
@@ -37699,22 +37696,22 @@
       <c r="C69" s="212" t="s">
         <v>1054</v>
       </c>
-      <c r="D69" s="57" t="s">
-        <v>419</v>
+      <c r="D69" s="6">
+        <v>1025.7</v>
       </c>
       <c r="E69" s="58" t="s">
-        <v>258</v>
+        <v>93</v>
       </c>
       <c r="F69" s="58" t="s">
-        <v>259</v>
+        <v>241</v>
       </c>
       <c r="G69" s="79" t="s">
         <v>498</v>
       </c>
       <c r="H69" s="61" t="s">
-        <v>268</v>
-      </c>
-      <c r="I69" s="113"/>
+        <v>13</v>
+      </c>
+      <c r="I69" s="115"/>
       <c r="J69" s="101" t="s">
         <v>386</v>
       </c>
@@ -37723,96 +37720,94 @@
         <v>781</v>
       </c>
     </row>
-    <row r="70" spans="1:12" s="3" customFormat="1" ht="24">
+    <row r="70" spans="1:12" s="3" customFormat="1">
       <c r="A70" s="64" t="s">
-        <v>693</v>
-      </c>
-      <c r="B70" s="57" t="s">
-        <v>8</v>
-      </c>
-      <c r="C70" s="212" t="s">
-        <v>1055</v>
-      </c>
-      <c r="D70" s="78" t="s">
-        <v>418</v>
-      </c>
-      <c r="E70" s="58" t="s">
-        <v>258</v>
-      </c>
-      <c r="F70" s="58" t="s">
-        <v>259</v>
-      </c>
-      <c r="G70" s="79" t="s">
-        <v>498</v>
-      </c>
-      <c r="H70" s="61" t="s">
-        <v>267</v>
-      </c>
-      <c r="I70" s="113"/>
+        <v>691</v>
+      </c>
+      <c r="B70" s="60" t="s">
+        <v>364</v>
+      </c>
+      <c r="C70" s="6" t="s">
+        <v>1046</v>
+      </c>
+      <c r="D70" s="111">
+        <v>0.03</v>
+      </c>
+      <c r="E70" s="6" t="s">
+        <v>242</v>
+      </c>
+      <c r="F70" s="56" t="s">
+        <v>247</v>
+      </c>
+      <c r="G70" s="58"/>
+      <c r="H70" s="7" t="s">
+        <v>324</v>
+      </c>
+      <c r="I70" s="116"/>
       <c r="J70" s="101" t="s">
         <v>386</v>
       </c>
       <c r="K70" s="75"/>
       <c r="L70" s="75" t="s">
-        <v>781</v>
-      </c>
-    </row>
-    <row r="71" spans="1:12" s="3" customFormat="1" ht="24">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" s="3" customFormat="1">
       <c r="A71" s="64" t="s">
-        <v>693</v>
-      </c>
-      <c r="B71" s="57" t="s">
-        <v>8</v>
-      </c>
-      <c r="C71" s="212" t="s">
-        <v>1054</v>
-      </c>
-      <c r="D71" s="78" t="s">
-        <v>419</v>
-      </c>
-      <c r="E71" s="58" t="s">
-        <v>258</v>
-      </c>
-      <c r="F71" s="58" t="s">
-        <v>259</v>
-      </c>
-      <c r="G71" s="79" t="s">
-        <v>498</v>
-      </c>
-      <c r="H71" s="61" t="s">
-        <v>267</v>
-      </c>
-      <c r="I71" s="113"/>
+        <v>691</v>
+      </c>
+      <c r="B71" s="60" t="s">
+        <v>364</v>
+      </c>
+      <c r="C71" s="6" t="s">
+        <v>1047</v>
+      </c>
+      <c r="D71" s="71">
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="E71" s="6" t="s">
+        <v>242</v>
+      </c>
+      <c r="F71" s="56" t="s">
+        <v>247</v>
+      </c>
+      <c r="G71" s="58"/>
+      <c r="H71" s="7" t="s">
+        <v>260</v>
+      </c>
+      <c r="I71" s="116"/>
       <c r="J71" s="101" t="s">
         <v>386</v>
       </c>
       <c r="K71" s="75"/>
       <c r="L71" s="75" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
     </row>
     <row r="72" spans="1:12" s="3" customFormat="1" ht="24">
-      <c r="A72" s="144" t="s">
-        <v>683</v>
-      </c>
-      <c r="B72" s="60" t="s">
-        <v>364</v>
-      </c>
-      <c r="C72" s="197" t="s">
-        <v>1046</v>
-      </c>
-      <c r="D72" s="71">
-        <v>1.2599999999999998E-2</v>
-      </c>
-      <c r="E72" s="6" t="s">
-        <v>242</v>
-      </c>
-      <c r="F72" s="56" t="s">
-        <v>247</v>
-      </c>
-      <c r="G72" s="58"/>
-      <c r="H72" s="57" t="s">
-        <v>265</v>
+      <c r="A72" s="64" t="s">
+        <v>692</v>
+      </c>
+      <c r="B72" s="57" t="s">
+        <v>8</v>
+      </c>
+      <c r="C72" s="212" t="s">
+        <v>1055</v>
+      </c>
+      <c r="D72" s="57" t="s">
+        <v>418</v>
+      </c>
+      <c r="E72" s="58" t="s">
+        <v>258</v>
+      </c>
+      <c r="F72" s="58" t="s">
+        <v>259</v>
+      </c>
+      <c r="G72" s="79" t="s">
+        <v>498</v>
+      </c>
+      <c r="H72" s="61" t="s">
+        <v>268</v>
       </c>
       <c r="I72" s="113"/>
       <c r="J72" s="101" t="s">
@@ -37820,31 +37815,33 @@
       </c>
       <c r="K72" s="75"/>
       <c r="L72" s="75" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
     </row>
     <row r="73" spans="1:12" s="3" customFormat="1" ht="24">
       <c r="A73" s="64" t="s">
-        <v>683</v>
-      </c>
-      <c r="B73" s="60" t="s">
-        <v>364</v>
-      </c>
-      <c r="C73" s="197" t="s">
-        <v>1047</v>
-      </c>
-      <c r="D73" s="71">
-        <v>1.5800000000000002E-2</v>
-      </c>
-      <c r="E73" s="6" t="s">
-        <v>242</v>
-      </c>
-      <c r="F73" s="56" t="s">
-        <v>247</v>
-      </c>
-      <c r="G73" s="58"/>
-      <c r="H73" s="57" t="s">
-        <v>266</v>
+        <v>692</v>
+      </c>
+      <c r="B73" s="57" t="s">
+        <v>8</v>
+      </c>
+      <c r="C73" s="212" t="s">
+        <v>1054</v>
+      </c>
+      <c r="D73" s="57" t="s">
+        <v>419</v>
+      </c>
+      <c r="E73" s="58" t="s">
+        <v>258</v>
+      </c>
+      <c r="F73" s="58" t="s">
+        <v>259</v>
+      </c>
+      <c r="G73" s="79" t="s">
+        <v>498</v>
+      </c>
+      <c r="H73" s="61" t="s">
+        <v>268</v>
       </c>
       <c r="I73" s="113"/>
       <c r="J73" s="101" t="s">
@@ -37852,12 +37849,12 @@
       </c>
       <c r="K73" s="75"/>
       <c r="L73" s="75" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
     </row>
     <row r="74" spans="1:12" s="3" customFormat="1" ht="24">
       <c r="A74" s="64" t="s">
-        <v>684</v>
+        <v>693</v>
       </c>
       <c r="B74" s="57" t="s">
         <v>8</v>
@@ -37877,7 +37874,9 @@
       <c r="G74" s="79" t="s">
         <v>498</v>
       </c>
-      <c r="H74" s="61"/>
+      <c r="H74" s="61" t="s">
+        <v>267</v>
+      </c>
       <c r="I74" s="113"/>
       <c r="J74" s="101" t="s">
         <v>386</v>
@@ -37889,7 +37888,7 @@
     </row>
     <row r="75" spans="1:12" s="3" customFormat="1" ht="24">
       <c r="A75" s="64" t="s">
-        <v>684</v>
+        <v>693</v>
       </c>
       <c r="B75" s="57" t="s">
         <v>8</v>
@@ -37909,7 +37908,9 @@
       <c r="G75" s="79" t="s">
         <v>498</v>
       </c>
-      <c r="H75" s="61"/>
+      <c r="H75" s="61" t="s">
+        <v>267</v>
+      </c>
       <c r="I75" s="113"/>
       <c r="J75" s="101" t="s">
         <v>386</v>
@@ -37919,56 +37920,61 @@
         <v>781</v>
       </c>
     </row>
-    <row r="76" spans="1:12" s="3" customFormat="1" ht="36">
-      <c r="A76" s="64" t="s">
-        <v>685</v>
-      </c>
-      <c r="B76" s="57" t="s">
-        <v>5</v>
-      </c>
-      <c r="C76" s="6" t="s">
-        <v>168</v>
-      </c>
-      <c r="D76" s="72" t="s">
-        <v>325</v>
-      </c>
-      <c r="E76" s="30" t="s">
-        <v>326</v>
-      </c>
-      <c r="F76" s="58" t="s">
-        <v>327</v>
+    <row r="76" spans="1:12" s="3" customFormat="1" ht="24">
+      <c r="A76" s="144" t="s">
+        <v>683</v>
+      </c>
+      <c r="B76" s="60" t="s">
+        <v>364</v>
+      </c>
+      <c r="C76" s="197" t="s">
+        <v>1046</v>
+      </c>
+      <c r="D76" s="71">
+        <v>1.2599999999999998E-2</v>
+      </c>
+      <c r="E76" s="6" t="s">
+        <v>242</v>
+      </c>
+      <c r="F76" s="56" t="s">
+        <v>247</v>
       </c>
       <c r="G76" s="58"/>
-      <c r="H76" s="61"/>
+      <c r="H76" s="57" t="s">
+        <v>265</v>
+      </c>
       <c r="I76" s="113"/>
       <c r="J76" s="101" t="s">
         <v>386</v>
       </c>
       <c r="K76" s="75"/>
       <c r="L76" s="75" t="s">
-        <v>782</v>
-      </c>
-    </row>
-    <row r="77" spans="1:12" s="3" customFormat="1" ht="39" customHeight="1">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" s="3" customFormat="1" ht="24">
       <c r="A77" s="64" t="s">
-        <v>686</v>
-      </c>
-      <c r="B77" s="57" t="s">
-        <v>5</v>
-      </c>
-      <c r="C77" s="6" t="s">
-        <v>168</v>
-      </c>
-      <c r="D77" s="58" t="s">
-        <v>328</v>
-      </c>
-      <c r="E77" s="30" t="s">
-        <v>329</v>
-      </c>
-      <c r="F77" s="58" t="s">
-        <v>330</v>
+        <v>683</v>
+      </c>
+      <c r="B77" s="60" t="s">
+        <v>364</v>
+      </c>
+      <c r="C77" s="197" t="s">
+        <v>1047</v>
+      </c>
+      <c r="D77" s="71">
+        <v>1.5800000000000002E-2</v>
+      </c>
+      <c r="E77" s="6" t="s">
+        <v>242</v>
+      </c>
+      <c r="F77" s="56" t="s">
+        <v>247</v>
       </c>
       <c r="G77" s="58"/>
+      <c r="H77" s="57" t="s">
+        <v>266</v>
+      </c>
       <c r="I77" s="113"/>
       <c r="J77" s="101" t="s">
         <v>386</v>
@@ -37980,90 +37986,88 @@
     </row>
     <row r="78" spans="1:12" s="3" customFormat="1" ht="24">
       <c r="A78" s="64" t="s">
-        <v>687</v>
-      </c>
-      <c r="B78" s="60" t="s">
-        <v>364</v>
-      </c>
-      <c r="C78" s="197" t="s">
-        <v>1046</v>
-      </c>
-      <c r="D78" s="71">
-        <v>1.54E-2</v>
-      </c>
-      <c r="E78" s="6" t="s">
-        <v>242</v>
-      </c>
-      <c r="F78" s="56" t="s">
-        <v>247</v>
-      </c>
-      <c r="G78" s="58"/>
-      <c r="H78" s="57" t="s">
-        <v>265</v>
-      </c>
+        <v>684</v>
+      </c>
+      <c r="B78" s="57" t="s">
+        <v>8</v>
+      </c>
+      <c r="C78" s="212" t="s">
+        <v>1055</v>
+      </c>
+      <c r="D78" s="78" t="s">
+        <v>418</v>
+      </c>
+      <c r="E78" s="58" t="s">
+        <v>258</v>
+      </c>
+      <c r="F78" s="58" t="s">
+        <v>259</v>
+      </c>
+      <c r="G78" s="79" t="s">
+        <v>498</v>
+      </c>
+      <c r="H78" s="61"/>
       <c r="I78" s="113"/>
       <c r="J78" s="101" t="s">
         <v>386</v>
       </c>
       <c r="K78" s="75"/>
       <c r="L78" s="75" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
     </row>
     <row r="79" spans="1:12" s="3" customFormat="1" ht="24">
       <c r="A79" s="64" t="s">
-        <v>687</v>
-      </c>
-      <c r="B79" s="60" t="s">
-        <v>364</v>
-      </c>
-      <c r="C79" s="197" t="s">
-        <v>1047</v>
-      </c>
-      <c r="D79" s="71">
-        <v>1.9300000000000001E-2</v>
-      </c>
-      <c r="E79" s="6" t="s">
-        <v>242</v>
-      </c>
-      <c r="F79" s="56" t="s">
-        <v>247</v>
-      </c>
-      <c r="G79" s="58"/>
-      <c r="H79" s="57" t="s">
-        <v>266</v>
-      </c>
+        <v>684</v>
+      </c>
+      <c r="B79" s="57" t="s">
+        <v>8</v>
+      </c>
+      <c r="C79" s="212" t="s">
+        <v>1054</v>
+      </c>
+      <c r="D79" s="78" t="s">
+        <v>419</v>
+      </c>
+      <c r="E79" s="58" t="s">
+        <v>258</v>
+      </c>
+      <c r="F79" s="58" t="s">
+        <v>259</v>
+      </c>
+      <c r="G79" s="79" t="s">
+        <v>498</v>
+      </c>
+      <c r="H79" s="61"/>
       <c r="I79" s="113"/>
       <c r="J79" s="101" t="s">
         <v>386</v>
       </c>
       <c r="K79" s="75"/>
       <c r="L79" s="75" t="s">
-        <v>780</v>
-      </c>
-    </row>
-    <row r="80" spans="1:12" s="3" customFormat="1" ht="24">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" s="3" customFormat="1" ht="36">
       <c r="A80" s="64" t="s">
-        <v>688</v>
+        <v>685</v>
       </c>
       <c r="B80" s="57" t="s">
-        <v>8</v>
-      </c>
-      <c r="C80" s="212" t="s">
-        <v>1055</v>
-      </c>
-      <c r="D80" s="78" t="s">
-        <v>418</v>
-      </c>
-      <c r="E80" s="58" t="s">
-        <v>258</v>
+        <v>5</v>
+      </c>
+      <c r="C80" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="D80" s="72" t="s">
+        <v>325</v>
+      </c>
+      <c r="E80" s="30" t="s">
+        <v>326</v>
       </c>
       <c r="F80" s="58" t="s">
-        <v>259</v>
-      </c>
-      <c r="G80" s="79" t="s">
-        <v>498</v>
-      </c>
+        <v>327</v>
+      </c>
+      <c r="G80" s="58"/>
       <c r="H80" s="61"/>
       <c r="I80" s="113"/>
       <c r="J80" s="101" t="s">
@@ -38071,92 +38075,93 @@
       </c>
       <c r="K80" s="75"/>
       <c r="L80" s="75" t="s">
-        <v>781</v>
-      </c>
-    </row>
-    <row r="81" spans="1:12" s="3" customFormat="1" ht="24">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12" s="3" customFormat="1" ht="39" customHeight="1">
       <c r="A81" s="64" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="B81" s="57" t="s">
-        <v>8</v>
-      </c>
-      <c r="C81" s="212" t="s">
-        <v>1054</v>
-      </c>
-      <c r="D81" s="78" t="s">
-        <v>419</v>
-      </c>
-      <c r="E81" s="58" t="s">
-        <v>258</v>
+        <v>5</v>
+      </c>
+      <c r="C81" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="D81" s="58" t="s">
+        <v>328</v>
+      </c>
+      <c r="E81" s="30" t="s">
+        <v>329</v>
       </c>
       <c r="F81" s="58" t="s">
-        <v>259</v>
-      </c>
-      <c r="G81" s="79" t="s">
-        <v>498</v>
-      </c>
-      <c r="H81" s="61"/>
+        <v>330</v>
+      </c>
+      <c r="G81" s="58"/>
       <c r="I81" s="113"/>
       <c r="J81" s="101" t="s">
         <v>386</v>
       </c>
       <c r="K81" s="75"/>
       <c r="L81" s="75" t="s">
-        <v>781</v>
-      </c>
-    </row>
-    <row r="82" spans="1:12" s="3" customFormat="1" ht="36">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12" s="3" customFormat="1" ht="24">
       <c r="A82" s="64" t="s">
-        <v>689</v>
-      </c>
-      <c r="B82" s="57" t="s">
-        <v>5</v>
-      </c>
-      <c r="C82" s="6" t="s">
-        <v>168</v>
-      </c>
-      <c r="D82" s="52" t="s">
-        <v>325</v>
-      </c>
-      <c r="E82" s="30" t="s">
-        <v>326</v>
-      </c>
-      <c r="F82" s="58" t="s">
-        <v>327</v>
+        <v>687</v>
+      </c>
+      <c r="B82" s="60" t="s">
+        <v>364</v>
+      </c>
+      <c r="C82" s="197" t="s">
+        <v>1046</v>
+      </c>
+      <c r="D82" s="71">
+        <v>1.54E-2</v>
+      </c>
+      <c r="E82" s="6" t="s">
+        <v>242</v>
+      </c>
+      <c r="F82" s="56" t="s">
+        <v>247</v>
       </c>
       <c r="G82" s="58"/>
-      <c r="H82" s="61"/>
+      <c r="H82" s="57" t="s">
+        <v>265</v>
+      </c>
       <c r="I82" s="113"/>
       <c r="J82" s="101" t="s">
         <v>386</v>
       </c>
       <c r="K82" s="75"/>
       <c r="L82" s="75" t="s">
-        <v>782</v>
-      </c>
-    </row>
-    <row r="83" spans="1:12" s="3" customFormat="1" ht="36.75" customHeight="1">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" s="3" customFormat="1" ht="24">
       <c r="A83" s="64" t="s">
-        <v>690</v>
-      </c>
-      <c r="B83" s="57" t="s">
-        <v>5</v>
-      </c>
-      <c r="C83" s="6" t="s">
-        <v>168</v>
-      </c>
-      <c r="D83" s="58" t="s">
-        <v>328</v>
-      </c>
-      <c r="E83" s="30" t="s">
-        <v>329</v>
-      </c>
-      <c r="F83" s="58" t="s">
-        <v>330</v>
+        <v>687</v>
+      </c>
+      <c r="B83" s="60" t="s">
+        <v>364</v>
+      </c>
+      <c r="C83" s="197" t="s">
+        <v>1047</v>
+      </c>
+      <c r="D83" s="71">
+        <v>1.9300000000000001E-2</v>
+      </c>
+      <c r="E83" s="6" t="s">
+        <v>242</v>
+      </c>
+      <c r="F83" s="56" t="s">
+        <v>247</v>
       </c>
       <c r="G83" s="58"/>
-      <c r="H83" s="61"/>
+      <c r="H83" s="57" t="s">
+        <v>266</v>
+      </c>
       <c r="I83" s="113"/>
       <c r="J83" s="101" t="s">
         <v>386</v>
@@ -38166,156 +38171,152 @@
         <v>780</v>
       </c>
     </row>
-    <row r="84" spans="1:12" s="3" customFormat="1">
+    <row r="84" spans="1:12" s="3" customFormat="1" ht="24">
       <c r="A84" s="64" t="s">
-        <v>1048</v>
-      </c>
-      <c r="B84" s="60" t="s">
-        <v>364</v>
-      </c>
-      <c r="C84" s="197" t="s">
-        <v>1045</v>
-      </c>
-      <c r="D84" s="112">
-        <v>8.9999999999999998E-4</v>
-      </c>
-      <c r="E84" s="6" t="s">
-        <v>242</v>
-      </c>
-      <c r="F84" s="56" t="s">
-        <v>247</v>
-      </c>
-      <c r="G84" s="58"/>
-      <c r="H84" s="57" t="s">
-        <v>257</v>
-      </c>
-      <c r="I84" s="40"/>
+        <v>688</v>
+      </c>
+      <c r="B84" s="57" t="s">
+        <v>8</v>
+      </c>
+      <c r="C84" s="212" t="s">
+        <v>1055</v>
+      </c>
+      <c r="D84" s="78" t="s">
+        <v>418</v>
+      </c>
+      <c r="E84" s="58" t="s">
+        <v>258</v>
+      </c>
+      <c r="F84" s="58" t="s">
+        <v>259</v>
+      </c>
+      <c r="G84" s="79" t="s">
+        <v>498</v>
+      </c>
+      <c r="H84" s="61"/>
+      <c r="I84" s="113"/>
       <c r="J84" s="101" t="s">
         <v>386</v>
       </c>
       <c r="K84" s="75"/>
       <c r="L84" s="75" t="s">
-        <v>779</v>
-      </c>
-    </row>
-    <row r="85" spans="1:12" s="3" customFormat="1">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12" s="3" customFormat="1" ht="24">
       <c r="A85" s="64" t="s">
-        <v>1049</v>
+        <v>688</v>
       </c>
       <c r="B85" s="57" t="s">
-        <v>5</v>
-      </c>
-      <c r="C85" s="59" t="s">
-        <v>168</v>
-      </c>
-      <c r="D85" s="57" t="s">
-        <v>331</v>
-      </c>
-      <c r="E85" s="30" t="s">
-        <v>242</v>
+        <v>8</v>
+      </c>
+      <c r="C85" s="212" t="s">
+        <v>1054</v>
+      </c>
+      <c r="D85" s="78" t="s">
+        <v>419</v>
+      </c>
+      <c r="E85" s="58" t="s">
+        <v>258</v>
       </c>
       <c r="F85" s="58" t="s">
-        <v>332</v>
-      </c>
-      <c r="G85" s="58"/>
-      <c r="H85" s="61" t="s">
-        <v>333</v>
-      </c>
-      <c r="I85" s="40"/>
+        <v>259</v>
+      </c>
+      <c r="G85" s="79" t="s">
+        <v>498</v>
+      </c>
+      <c r="H85" s="61"/>
+      <c r="I85" s="113"/>
       <c r="J85" s="101" t="s">
         <v>386</v>
       </c>
       <c r="K85" s="75"/>
       <c r="L85" s="75" t="s">
-        <v>782</v>
-      </c>
-    </row>
-    <row r="86" spans="1:12" s="3" customFormat="1">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12" s="3" customFormat="1" ht="36">
       <c r="A86" s="64" t="s">
-        <v>1050</v>
+        <v>689</v>
       </c>
       <c r="B86" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="C86" s="59" t="s">
+      <c r="C86" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="D86" s="6" t="s">
-        <v>334</v>
-      </c>
-      <c r="E86" s="6" t="s">
-        <v>242</v>
+      <c r="D86" s="52" t="s">
+        <v>325</v>
+      </c>
+      <c r="E86" s="30" t="s">
+        <v>326</v>
       </c>
       <c r="F86" s="58" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="G86" s="58"/>
-      <c r="H86" s="61" t="s">
-        <v>333</v>
-      </c>
-      <c r="I86" s="40"/>
+      <c r="H86" s="61"/>
+      <c r="I86" s="113"/>
       <c r="J86" s="101" t="s">
         <v>386</v>
       </c>
       <c r="K86" s="75"/>
       <c r="L86" s="75" t="s">
-        <v>780</v>
-      </c>
-    </row>
-    <row r="87" spans="1:12" s="3" customFormat="1">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12" s="3" customFormat="1" ht="36.75" customHeight="1">
       <c r="A87" s="64" t="s">
-        <v>1051</v>
-      </c>
-      <c r="B87" s="60" t="s">
-        <v>364</v>
-      </c>
-      <c r="C87" s="197" t="s">
-        <v>1045</v>
-      </c>
-      <c r="D87" s="5">
-        <v>1.1000000000000001E-3</v>
-      </c>
-      <c r="E87" s="6" t="s">
-        <v>242</v>
-      </c>
-      <c r="F87" s="56" t="s">
-        <v>247</v>
+        <v>690</v>
+      </c>
+      <c r="B87" s="57" t="s">
+        <v>5</v>
+      </c>
+      <c r="C87" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="D87" s="58" t="s">
+        <v>328</v>
+      </c>
+      <c r="E87" s="30" t="s">
+        <v>329</v>
+      </c>
+      <c r="F87" s="58" t="s">
+        <v>330</v>
       </c>
       <c r="G87" s="58"/>
-      <c r="H87" s="57" t="s">
-        <v>256</v>
-      </c>
-      <c r="I87" s="40"/>
+      <c r="H87" s="61"/>
+      <c r="I87" s="113"/>
       <c r="J87" s="101" t="s">
         <v>386</v>
       </c>
       <c r="K87" s="75"/>
       <c r="L87" s="75" t="s">
-        <v>779</v>
+        <v>780</v>
       </c>
     </row>
     <row r="88" spans="1:12" s="3" customFormat="1">
       <c r="A88" s="64" t="s">
-        <v>1052</v>
-      </c>
-      <c r="B88" s="57" t="s">
-        <v>5</v>
-      </c>
-      <c r="C88" s="59" t="s">
-        <v>168</v>
-      </c>
-      <c r="D88" s="57" t="s">
-        <v>331</v>
-      </c>
-      <c r="E88" s="30" t="s">
+        <v>1048</v>
+      </c>
+      <c r="B88" s="60" t="s">
+        <v>364</v>
+      </c>
+      <c r="C88" s="197" t="s">
+        <v>1045</v>
+      </c>
+      <c r="D88" s="112">
+        <v>8.9999999999999998E-4</v>
+      </c>
+      <c r="E88" s="6" t="s">
         <v>242</v>
       </c>
-      <c r="F88" s="58" t="s">
-        <v>332</v>
+      <c r="F88" s="56" t="s">
+        <v>247</v>
       </c>
       <c r="G88" s="58"/>
-      <c r="H88" s="61" t="s">
-        <v>333</v>
+      <c r="H88" s="57" t="s">
+        <v>257</v>
       </c>
       <c r="I88" s="40"/>
       <c r="J88" s="101" t="s">
@@ -38323,12 +38324,12 @@
       </c>
       <c r="K88" s="75"/>
       <c r="L88" s="75" t="s">
-        <v>782</v>
-      </c>
-    </row>
-    <row r="89" spans="1:12" s="3" customFormat="1" ht="14.25" customHeight="1">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12" s="3" customFormat="1">
       <c r="A89" s="64" t="s">
-        <v>1053</v>
+        <v>1049</v>
       </c>
       <c r="B89" s="57" t="s">
         <v>5</v>
@@ -38336,10 +38337,10 @@
       <c r="C89" s="59" t="s">
         <v>168</v>
       </c>
-      <c r="D89" s="6" t="s">
-        <v>334</v>
-      </c>
-      <c r="E89" s="6" t="s">
+      <c r="D89" s="57" t="s">
+        <v>331</v>
+      </c>
+      <c r="E89" s="30" t="s">
         <v>242</v>
       </c>
       <c r="F89" s="58" t="s">
@@ -38355,197 +38356,201 @@
       </c>
       <c r="K89" s="75"/>
       <c r="L89" s="75" t="s">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12" s="3" customFormat="1">
+      <c r="A90" s="64" t="s">
+        <v>1050</v>
+      </c>
+      <c r="B90" s="57" t="s">
+        <v>5</v>
+      </c>
+      <c r="C90" s="59" t="s">
+        <v>168</v>
+      </c>
+      <c r="D90" s="6" t="s">
+        <v>334</v>
+      </c>
+      <c r="E90" s="6" t="s">
+        <v>242</v>
+      </c>
+      <c r="F90" s="58" t="s">
+        <v>332</v>
+      </c>
+      <c r="G90" s="58"/>
+      <c r="H90" s="61" t="s">
+        <v>333</v>
+      </c>
+      <c r="I90" s="40"/>
+      <c r="J90" s="101" t="s">
+        <v>386</v>
+      </c>
+      <c r="K90" s="75"/>
+      <c r="L90" s="75" t="s">
         <v>780</v>
       </c>
     </row>
-    <row r="90" spans="1:12" s="76" customFormat="1">
-      <c r="A90" s="11" t="s">
-        <v>387</v>
-      </c>
-      <c r="B90" s="67" t="s">
-        <v>1</v>
-      </c>
-      <c r="C90" s="67" t="s">
-        <v>222</v>
-      </c>
-      <c r="D90" s="67" t="s">
-        <v>2</v>
-      </c>
-      <c r="E90" s="67" t="s">
-        <v>3</v>
-      </c>
-      <c r="F90" s="67" t="s">
-        <v>63</v>
-      </c>
-      <c r="G90" s="67" t="s">
-        <v>19</v>
-      </c>
-      <c r="H90" s="67" t="s">
-        <v>72</v>
-      </c>
-      <c r="I90" s="67" t="s">
-        <v>14</v>
-      </c>
-      <c r="J90" s="67" t="s">
-        <v>370</v>
-      </c>
-      <c r="K90" s="67" t="s">
-        <v>411</v>
-      </c>
-      <c r="L90" s="67" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="91" spans="1:12" s="76" customFormat="1" ht="24.75">
-      <c r="A91" s="99" t="s">
-        <v>388</v>
-      </c>
-      <c r="B91" s="75" t="s">
+    <row r="91" spans="1:12" s="3" customFormat="1">
+      <c r="A91" s="64" t="s">
+        <v>1051</v>
+      </c>
+      <c r="B91" s="60" t="s">
         <v>364</v>
       </c>
       <c r="C91" s="197" t="s">
         <v>1045</v>
       </c>
-      <c r="D91" s="75">
-        <v>1.4999999999999999E-2</v>
+      <c r="D91" s="5">
+        <v>1.1000000000000001E-3</v>
       </c>
       <c r="E91" s="6" t="s">
-        <v>429</v>
-      </c>
-      <c r="F91" s="83"/>
-      <c r="G91" s="83"/>
-      <c r="H91" s="125" t="s">
-        <v>448</v>
-      </c>
-      <c r="I91" s="10"/>
-      <c r="J91" s="13" t="s">
-        <v>403</v>
-      </c>
-      <c r="K91" s="26" t="s">
-        <v>458</v>
-      </c>
+        <v>242</v>
+      </c>
+      <c r="F91" s="56" t="s">
+        <v>247</v>
+      </c>
+      <c r="G91" s="58"/>
+      <c r="H91" s="57" t="s">
+        <v>256</v>
+      </c>
+      <c r="I91" s="40"/>
+      <c r="J91" s="101" t="s">
+        <v>386</v>
+      </c>
+      <c r="K91" s="75"/>
       <c r="L91" s="75" t="s">
         <v>779</v>
       </c>
     </row>
-    <row r="92" spans="1:12" s="76" customFormat="1">
-      <c r="A92" s="29" t="s">
-        <v>459</v>
-      </c>
-      <c r="B92" s="75" t="s">
-        <v>7</v>
-      </c>
-      <c r="C92" s="197" t="s">
-        <v>1045</v>
-      </c>
-      <c r="D92" s="126">
-        <v>0.06</v>
-      </c>
-      <c r="E92" s="6" t="s">
+    <row r="92" spans="1:12" s="3" customFormat="1">
+      <c r="A92" s="64" t="s">
+        <v>1052</v>
+      </c>
+      <c r="B92" s="57" t="s">
+        <v>5</v>
+      </c>
+      <c r="C92" s="59" t="s">
+        <v>168</v>
+      </c>
+      <c r="D92" s="57" t="s">
+        <v>331</v>
+      </c>
+      <c r="E92" s="30" t="s">
         <v>242</v>
       </c>
-      <c r="F92" s="77" t="s">
-        <v>247</v>
-      </c>
-      <c r="G92" s="79"/>
-      <c r="H92" s="7" t="s">
-        <v>449</v>
-      </c>
-      <c r="I92" s="10"/>
-      <c r="J92" s="13" t="s">
-        <v>403</v>
-      </c>
-      <c r="K92" s="13" t="s">
-        <v>458</v>
-      </c>
-      <c r="L92" s="75"/>
-    </row>
-    <row r="93" spans="1:12" s="76" customFormat="1">
-      <c r="A93" s="29" t="s">
-        <v>460</v>
-      </c>
-      <c r="B93" s="75" t="s">
-        <v>364</v>
-      </c>
-      <c r="C93" s="6" t="s">
+      <c r="F92" s="58" t="s">
+        <v>332</v>
+      </c>
+      <c r="G92" s="58"/>
+      <c r="H92" s="61" t="s">
+        <v>333</v>
+      </c>
+      <c r="I92" s="40"/>
+      <c r="J92" s="101" t="s">
+        <v>386</v>
+      </c>
+      <c r="K92" s="75"/>
+      <c r="L92" s="75" t="s">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="93" spans="1:12" s="3" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A93" s="64" t="s">
+        <v>1053</v>
+      </c>
+      <c r="B93" s="57" t="s">
+        <v>5</v>
+      </c>
+      <c r="C93" s="59" t="s">
         <v>168</v>
       </c>
-      <c r="D93" s="13" t="s">
-        <v>457</v>
+      <c r="D93" s="6" t="s">
+        <v>334</v>
       </c>
       <c r="E93" s="6" t="s">
-        <v>450</v>
-      </c>
-      <c r="F93" s="83"/>
-      <c r="G93" s="83"/>
-      <c r="H93" s="13" t="s">
-        <v>451</v>
-      </c>
-      <c r="I93" s="10"/>
-      <c r="J93" s="13" t="s">
-        <v>403</v>
-      </c>
-      <c r="K93" s="13" t="s">
-        <v>458</v>
-      </c>
-      <c r="L93" s="75"/>
+        <v>242</v>
+      </c>
+      <c r="F93" s="58" t="s">
+        <v>332</v>
+      </c>
+      <c r="G93" s="58"/>
+      <c r="H93" s="61" t="s">
+        <v>333</v>
+      </c>
+      <c r="I93" s="40"/>
+      <c r="J93" s="101" t="s">
+        <v>386</v>
+      </c>
+      <c r="K93" s="75"/>
+      <c r="L93" s="75" t="s">
+        <v>780</v>
+      </c>
     </row>
     <row r="94" spans="1:12" s="76" customFormat="1">
-      <c r="A94" s="29" t="s">
-        <v>461</v>
-      </c>
-      <c r="B94" s="75" t="s">
-        <v>22</v>
-      </c>
-      <c r="C94" s="6" t="s">
-        <v>168</v>
-      </c>
-      <c r="D94" s="13" t="s">
-        <v>452</v>
-      </c>
-      <c r="E94" s="6" t="s">
-        <v>450</v>
-      </c>
-      <c r="F94" s="83"/>
-      <c r="G94" s="83"/>
-      <c r="H94" s="75" t="s">
-        <v>453</v>
-      </c>
-      <c r="I94" s="10"/>
-      <c r="J94" s="13" t="s">
-        <v>403</v>
-      </c>
-      <c r="K94" s="13" t="s">
-        <v>458</v>
-      </c>
-      <c r="L94" s="75"/>
-    </row>
-    <row r="95" spans="1:12" s="76" customFormat="1">
+      <c r="A94" s="11" t="s">
+        <v>387</v>
+      </c>
+      <c r="B94" s="67" t="s">
+        <v>1</v>
+      </c>
+      <c r="C94" s="67" t="s">
+        <v>222</v>
+      </c>
+      <c r="D94" s="67" t="s">
+        <v>2</v>
+      </c>
+      <c r="E94" s="67" t="s">
+        <v>3</v>
+      </c>
+      <c r="F94" s="67" t="s">
+        <v>63</v>
+      </c>
+      <c r="G94" s="67" t="s">
+        <v>19</v>
+      </c>
+      <c r="H94" s="67" t="s">
+        <v>72</v>
+      </c>
+      <c r="I94" s="67" t="s">
+        <v>14</v>
+      </c>
+      <c r="J94" s="67" t="s">
+        <v>370</v>
+      </c>
+      <c r="K94" s="67" t="s">
+        <v>411</v>
+      </c>
+      <c r="L94" s="67" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="95" spans="1:12" s="76" customFormat="1" ht="24.75">
       <c r="A95" s="99" t="s">
-        <v>389</v>
-      </c>
-      <c r="B95" s="70" t="s">
+        <v>388</v>
+      </c>
+      <c r="B95" s="75" t="s">
         <v>364</v>
       </c>
       <c r="C95" s="197" t="s">
         <v>1045</v>
       </c>
-      <c r="D95" s="126">
-        <v>0.03</v>
+      <c r="D95" s="75">
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="E95" s="6" t="s">
-        <v>242</v>
-      </c>
-      <c r="F95" s="77" t="s">
-        <v>247</v>
-      </c>
-      <c r="G95" s="79"/>
-      <c r="H95" s="7"/>
-      <c r="I95" s="116"/>
+        <v>429</v>
+      </c>
+      <c r="F95" s="83"/>
+      <c r="G95" s="83"/>
+      <c r="H95" s="125" t="s">
+        <v>448</v>
+      </c>
+      <c r="I95" s="10"/>
       <c r="J95" s="13" t="s">
         <v>403</v>
       </c>
-      <c r="K95" s="13" t="s">
+      <c r="K95" s="26" t="s">
         <v>458</v>
       </c>
       <c r="L95" s="75" t="s">
@@ -38553,25 +38558,27 @@
       </c>
     </row>
     <row r="96" spans="1:12" s="76" customFormat="1">
-      <c r="A96" s="99" t="s">
-        <v>390</v>
-      </c>
-      <c r="B96" s="98" t="s">
-        <v>364</v>
+      <c r="A96" s="29" t="s">
+        <v>459</v>
+      </c>
+      <c r="B96" s="75" t="s">
+        <v>7</v>
       </c>
       <c r="C96" s="197" t="s">
         <v>1045</v>
       </c>
       <c r="D96" s="126">
-        <v>0.05</v>
+        <v>0.06</v>
       </c>
       <c r="E96" s="6" t="s">
-        <v>429</v>
-      </c>
-      <c r="F96" s="83"/>
-      <c r="G96" s="83"/>
-      <c r="H96" s="13" t="s">
-        <v>421</v>
+        <v>242</v>
+      </c>
+      <c r="F96" s="77" t="s">
+        <v>247</v>
+      </c>
+      <c r="G96" s="79"/>
+      <c r="H96" s="7" t="s">
+        <v>449</v>
       </c>
       <c r="I96" s="10"/>
       <c r="J96" s="13" t="s">
@@ -38580,30 +38587,28 @@
       <c r="K96" s="13" t="s">
         <v>458</v>
       </c>
-      <c r="L96" s="75" t="s">
-        <v>779</v>
-      </c>
+      <c r="L96" s="75"/>
     </row>
     <row r="97" spans="1:12" s="76" customFormat="1">
-      <c r="A97" s="99" t="s">
-        <v>391</v>
-      </c>
-      <c r="B97" s="98" t="s">
+      <c r="A97" s="29" t="s">
+        <v>460</v>
+      </c>
+      <c r="B97" s="75" t="s">
         <v>364</v>
       </c>
-      <c r="C97" s="197" t="s">
-        <v>1045</v>
-      </c>
-      <c r="D97" s="13">
-        <v>4.2999999999999997E-2</v>
+      <c r="C97" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="D97" s="13" t="s">
+        <v>457</v>
       </c>
       <c r="E97" s="6" t="s">
-        <v>429</v>
+        <v>450</v>
       </c>
       <c r="F97" s="83"/>
       <c r="G97" s="83"/>
       <c r="H97" s="13" t="s">
-        <v>421</v>
+        <v>451</v>
       </c>
       <c r="I97" s="10"/>
       <c r="J97" s="13" t="s">
@@ -38612,13 +38617,11 @@
       <c r="K97" s="13" t="s">
         <v>458</v>
       </c>
-      <c r="L97" s="75" t="s">
-        <v>779</v>
-      </c>
+      <c r="L97" s="75"/>
     </row>
     <row r="98" spans="1:12" s="76" customFormat="1">
       <c r="A98" s="29" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B98" s="75" t="s">
         <v>22</v>
@@ -38627,15 +38630,15 @@
         <v>168</v>
       </c>
       <c r="D98" s="13" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="E98" s="6" t="s">
-        <v>429</v>
+        <v>450</v>
       </c>
       <c r="F98" s="83"/>
       <c r="G98" s="83"/>
-      <c r="H98" s="13" t="s">
-        <v>421</v>
+      <c r="H98" s="75" t="s">
+        <v>453</v>
       </c>
       <c r="I98" s="10"/>
       <c r="J98" s="13" t="s">
@@ -38647,27 +38650,27 @@
       <c r="L98" s="75"/>
     </row>
     <row r="99" spans="1:12" s="76" customFormat="1">
-      <c r="A99" s="29" t="s">
-        <v>463</v>
-      </c>
-      <c r="B99" s="81" t="s">
-        <v>22</v>
-      </c>
-      <c r="C99" s="80" t="s">
-        <v>1055</v>
-      </c>
-      <c r="D99" s="13">
-        <v>0.44</v>
-      </c>
-      <c r="E99" s="79" t="s">
-        <v>322</v>
+      <c r="A99" s="99" t="s">
+        <v>389</v>
+      </c>
+      <c r="B99" s="70" t="s">
+        <v>364</v>
+      </c>
+      <c r="C99" s="197" t="s">
+        <v>1045</v>
+      </c>
+      <c r="D99" s="126">
+        <v>0.03</v>
+      </c>
+      <c r="E99" s="6" t="s">
+        <v>242</v>
       </c>
       <c r="F99" s="77" t="s">
-        <v>323</v>
+        <v>247</v>
       </c>
       <c r="G99" s="79"/>
-      <c r="H99" s="31"/>
-      <c r="I99" s="113"/>
+      <c r="H99" s="7"/>
+      <c r="I99" s="116"/>
       <c r="J99" s="13" t="s">
         <v>403</v>
       </c>
@@ -38678,9 +38681,9 @@
         <v>779</v>
       </c>
     </row>
-    <row r="100" spans="1:12" s="76" customFormat="1" ht="24.75">
+    <row r="100" spans="1:12" s="76" customFormat="1">
       <c r="A100" s="99" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="B100" s="98" t="s">
         <v>364</v>
@@ -38688,16 +38691,16 @@
       <c r="C100" s="197" t="s">
         <v>1045</v>
       </c>
-      <c r="D100" s="75">
-        <v>1.4999999999999999E-2</v>
+      <c r="D100" s="126">
+        <v>0.05</v>
       </c>
       <c r="E100" s="6" t="s">
         <v>429</v>
       </c>
       <c r="F100" s="83"/>
       <c r="G100" s="83"/>
-      <c r="H100" s="125" t="s">
-        <v>448</v>
+      <c r="H100" s="13" t="s">
+        <v>421</v>
       </c>
       <c r="I100" s="10"/>
       <c r="J100" s="13" t="s">
@@ -38711,8 +38714,8 @@
       </c>
     </row>
     <row r="101" spans="1:12" s="76" customFormat="1">
-      <c r="A101" s="29" t="s">
-        <v>464</v>
+      <c r="A101" s="99" t="s">
+        <v>391</v>
       </c>
       <c r="B101" s="98" t="s">
         <v>364</v>
@@ -38720,18 +38723,16 @@
       <c r="C101" s="197" t="s">
         <v>1045</v>
       </c>
-      <c r="D101" s="127">
-        <v>0.06</v>
+      <c r="D101" s="13">
+        <v>4.2999999999999997E-2</v>
       </c>
       <c r="E101" s="6" t="s">
-        <v>242</v>
-      </c>
-      <c r="F101" s="77" t="s">
-        <v>247</v>
-      </c>
-      <c r="G101" s="79"/>
-      <c r="H101" s="7" t="s">
-        <v>455</v>
+        <v>429</v>
+      </c>
+      <c r="F101" s="83"/>
+      <c r="G101" s="83"/>
+      <c r="H101" s="13" t="s">
+        <v>421</v>
       </c>
       <c r="I101" s="10"/>
       <c r="J101" s="13" t="s">
@@ -38740,28 +38741,30 @@
       <c r="K101" s="13" t="s">
         <v>458</v>
       </c>
-      <c r="L101" s="75"/>
-    </row>
-    <row r="102" spans="1:12" s="76" customFormat="1" ht="24.75">
-      <c r="A102" s="99" t="s">
-        <v>393</v>
-      </c>
-      <c r="B102" s="98" t="s">
-        <v>364</v>
-      </c>
-      <c r="C102" s="197" t="s">
-        <v>1045</v>
-      </c>
-      <c r="D102" s="75">
-        <v>0.08</v>
+      <c r="L101" s="75" t="s">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="102" spans="1:12" s="76" customFormat="1">
+      <c r="A102" s="29" t="s">
+        <v>462</v>
+      </c>
+      <c r="B102" s="75" t="s">
+        <v>22</v>
+      </c>
+      <c r="C102" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="D102" s="13" t="s">
+        <v>454</v>
       </c>
       <c r="E102" s="6" t="s">
         <v>429</v>
       </c>
       <c r="F102" s="83"/>
       <c r="G102" s="83"/>
-      <c r="H102" s="125" t="s">
-        <v>456</v>
+      <c r="H102" s="13" t="s">
+        <v>421</v>
       </c>
       <c r="I102" s="10"/>
       <c r="J102" s="13" t="s">
@@ -38770,32 +38773,30 @@
       <c r="K102" s="13" t="s">
         <v>458</v>
       </c>
-      <c r="L102" s="75" t="s">
-        <v>779</v>
-      </c>
+      <c r="L102" s="75"/>
     </row>
     <row r="103" spans="1:12" s="76" customFormat="1">
-      <c r="A103" s="99" t="s">
-        <v>394</v>
-      </c>
-      <c r="B103" s="70" t="s">
-        <v>364</v>
-      </c>
-      <c r="C103" s="197" t="s">
-        <v>1045</v>
-      </c>
-      <c r="D103" s="127">
-        <v>0.06</v>
-      </c>
-      <c r="E103" s="6" t="s">
-        <v>242</v>
+      <c r="A103" s="29" t="s">
+        <v>463</v>
+      </c>
+      <c r="B103" s="81" t="s">
+        <v>22</v>
+      </c>
+      <c r="C103" s="80" t="s">
+        <v>1055</v>
+      </c>
+      <c r="D103" s="13">
+        <v>0.44</v>
+      </c>
+      <c r="E103" s="79" t="s">
+        <v>322</v>
       </c>
       <c r="F103" s="77" t="s">
-        <v>247</v>
+        <v>323</v>
       </c>
       <c r="G103" s="79"/>
-      <c r="H103" s="7"/>
-      <c r="I103" s="116"/>
+      <c r="H103" s="31"/>
+      <c r="I103" s="113"/>
       <c r="J103" s="13" t="s">
         <v>403</v>
       </c>
@@ -38806,17 +38807,27 @@
         <v>779</v>
       </c>
     </row>
-    <row r="104" spans="1:12" s="76" customFormat="1">
-      <c r="A104" s="29" t="s">
-        <v>410</v>
-      </c>
-      <c r="B104" s="83"/>
-      <c r="C104" s="6"/>
-      <c r="D104" s="13"/>
-      <c r="E104" s="83"/>
+    <row r="104" spans="1:12" s="76" customFormat="1" ht="24.75">
+      <c r="A104" s="99" t="s">
+        <v>392</v>
+      </c>
+      <c r="B104" s="98" t="s">
+        <v>364</v>
+      </c>
+      <c r="C104" s="197" t="s">
+        <v>1045</v>
+      </c>
+      <c r="D104" s="75">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="E104" s="6" t="s">
+        <v>429</v>
+      </c>
       <c r="F104" s="83"/>
       <c r="G104" s="83"/>
-      <c r="H104" s="83"/>
+      <c r="H104" s="125" t="s">
+        <v>448</v>
+      </c>
       <c r="I104" s="10"/>
       <c r="J104" s="13" t="s">
         <v>403</v>
@@ -38824,16 +38835,134 @@
       <c r="K104" s="13" t="s">
         <v>458</v>
       </c>
-      <c r="L104" s="75"/>
-    </row>
-    <row r="108" spans="1:12">
-      <c r="E108" s="34"/>
-    </row>
-    <row r="109" spans="1:12">
-      <c r="E109" s="34"/>
-    </row>
-    <row r="110" spans="1:12">
-      <c r="E110" s="34"/>
+      <c r="L104" s="75" t="s">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="105" spans="1:12" s="76" customFormat="1">
+      <c r="A105" s="29" t="s">
+        <v>464</v>
+      </c>
+      <c r="B105" s="98" t="s">
+        <v>364</v>
+      </c>
+      <c r="C105" s="197" t="s">
+        <v>1045</v>
+      </c>
+      <c r="D105" s="127">
+        <v>0.06</v>
+      </c>
+      <c r="E105" s="6" t="s">
+        <v>242</v>
+      </c>
+      <c r="F105" s="77" t="s">
+        <v>247</v>
+      </c>
+      <c r="G105" s="79"/>
+      <c r="H105" s="7" t="s">
+        <v>455</v>
+      </c>
+      <c r="I105" s="10"/>
+      <c r="J105" s="13" t="s">
+        <v>403</v>
+      </c>
+      <c r="K105" s="13" t="s">
+        <v>458</v>
+      </c>
+      <c r="L105" s="75"/>
+    </row>
+    <row r="106" spans="1:12" s="76" customFormat="1" ht="24.75">
+      <c r="A106" s="99" t="s">
+        <v>393</v>
+      </c>
+      <c r="B106" s="98" t="s">
+        <v>364</v>
+      </c>
+      <c r="C106" s="197" t="s">
+        <v>1045</v>
+      </c>
+      <c r="D106" s="75">
+        <v>0.08</v>
+      </c>
+      <c r="E106" s="6" t="s">
+        <v>429</v>
+      </c>
+      <c r="F106" s="83"/>
+      <c r="G106" s="83"/>
+      <c r="H106" s="125" t="s">
+        <v>456</v>
+      </c>
+      <c r="I106" s="10"/>
+      <c r="J106" s="13" t="s">
+        <v>403</v>
+      </c>
+      <c r="K106" s="13" t="s">
+        <v>458</v>
+      </c>
+      <c r="L106" s="75" t="s">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="107" spans="1:12" s="76" customFormat="1">
+      <c r="A107" s="99" t="s">
+        <v>394</v>
+      </c>
+      <c r="B107" s="70" t="s">
+        <v>364</v>
+      </c>
+      <c r="C107" s="197" t="s">
+        <v>1045</v>
+      </c>
+      <c r="D107" s="127">
+        <v>0.06</v>
+      </c>
+      <c r="E107" s="6" t="s">
+        <v>242</v>
+      </c>
+      <c r="F107" s="77" t="s">
+        <v>247</v>
+      </c>
+      <c r="G107" s="79"/>
+      <c r="H107" s="7"/>
+      <c r="I107" s="116"/>
+      <c r="J107" s="13" t="s">
+        <v>403</v>
+      </c>
+      <c r="K107" s="13" t="s">
+        <v>458</v>
+      </c>
+      <c r="L107" s="75" t="s">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="108" spans="1:12" s="76" customFormat="1">
+      <c r="A108" s="29" t="s">
+        <v>410</v>
+      </c>
+      <c r="B108" s="83"/>
+      <c r="C108" s="6"/>
+      <c r="D108" s="13"/>
+      <c r="E108" s="83"/>
+      <c r="F108" s="83"/>
+      <c r="G108" s="83"/>
+      <c r="H108" s="83"/>
+      <c r="I108" s="10"/>
+      <c r="J108" s="13" t="s">
+        <v>403</v>
+      </c>
+      <c r="K108" s="13" t="s">
+        <v>458</v>
+      </c>
+      <c r="L108" s="75"/>
+    </row>
+    <row r="112" spans="1:12">
+      <c r="E112" s="34"/>
+    </row>
+    <row r="113" spans="5:5">
+      <c r="E113" s="34"/>
+    </row>
+    <row r="114" spans="5:5">
+      <c r="E114" s="34"/>
     </row>
   </sheetData>
   <phoneticPr fontId="36" type="noConversion"/>

</xml_diff>

<commit_message>
Set inspiratory vs. expiratory respiratory resistance properly. Update scenarios with PulmonaryResistance data request. Tweaks to respirtory system validation data.
</commit_message>
<xml_diff>
--- a/test/validation/SystemValidationData.xlsx
+++ b/test/validation/SystemValidationData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Source\engine\test\validation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2136B69-C280-411B-B279-C5D90FBB28B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAEB3C5F-1DB9-4466-8D76-BE940CA06CA6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1830" yWindow="3450" windowWidth="27090" windowHeight="25230" tabRatio="724" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3291,9 +3291,6 @@
     <t>The normal human weighing 70kg has a body surface area of about 1.7 square meteres. Therefore, 0.14*1.7.</t>
   </si>
   <si>
-    <t>RespiratoryMuscleFatigue</t>
-  </si>
-  <si>
     <t>roussos1979fatigue</t>
   </si>
   <si>
@@ -3349,6 +3346,9 @@
   </si>
   <si>
     <t>[Tidal Volume] / [Total Compliance]</t>
+  </si>
+  <si>
+    <t>RespiratoryMuscleFatigue*</t>
   </si>
 </sst>
 </file>
@@ -9427,7 +9427,7 @@
         <v>7</v>
       </c>
       <c r="C48" s="212" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="D48" s="209" t="s">
         <v>166</v>
@@ -9455,7 +9455,7 @@
         <v>7</v>
       </c>
       <c r="C49" s="212" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="D49" s="209" t="s">
         <v>525</v>
@@ -9483,7 +9483,7 @@
         <v>5</v>
       </c>
       <c r="C50" s="212" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="D50" s="209" t="s">
         <v>516</v>
@@ -9511,7 +9511,7 @@
         <v>5</v>
       </c>
       <c r="C51" s="212" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="D51" s="209" t="s">
         <v>167</v>
@@ -10099,7 +10099,7 @@
         <v>5</v>
       </c>
       <c r="C71" s="212" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="D71" s="209" t="s">
         <v>516</v>
@@ -10129,7 +10129,7 @@
         <v>5</v>
       </c>
       <c r="C72" s="212" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="D72" s="209" t="s">
         <v>169</v>
@@ -10397,7 +10397,7 @@
         <v>7</v>
       </c>
       <c r="C81" s="212" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="D81" s="209" t="s">
         <v>529</v>
@@ -10427,7 +10427,7 @@
         <v>7</v>
       </c>
       <c r="C82" s="212" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="D82" s="209" t="s">
         <v>530</v>
@@ -10455,7 +10455,7 @@
         <v>5</v>
       </c>
       <c r="C83" s="212" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="D83" s="209" t="s">
         <v>521</v>
@@ -10485,7 +10485,7 @@
         <v>5</v>
       </c>
       <c r="C84" s="212" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="D84" s="209" t="s">
         <v>169</v>
@@ -35543,10 +35543,10 @@
   <dimension ref="A1:X114"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B26" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E29" sqref="E29"/>
+      <selection pane="bottomRight" activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -35806,7 +35806,7 @@
     </row>
     <row r="8" spans="1:24" s="3" customFormat="1">
       <c r="A8" s="202" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="B8" s="166"/>
       <c r="C8" s="147"/>
@@ -35902,7 +35902,7 @@
         <v>22</v>
       </c>
       <c r="C12" s="59" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="D12" s="5">
         <v>0.44</v>
@@ -35926,7 +35926,7 @@
     </row>
     <row r="13" spans="1:24" s="3" customFormat="1">
       <c r="A13" s="200" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="B13" s="210" t="s">
         <v>28</v>
@@ -36036,7 +36036,7 @@
         <v>22</v>
       </c>
       <c r="C17" s="212" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="D17" s="109">
         <v>0.4</v>
@@ -36060,7 +36060,7 @@
     </row>
     <row r="18" spans="1:24">
       <c r="A18" s="16" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
       <c r="B18" s="57" t="s">
         <v>28</v>
@@ -36108,7 +36108,7 @@
         <v>8</v>
       </c>
       <c r="C19" s="147" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="D19" s="190">
         <v>-8</v>
@@ -36138,7 +36138,7 @@
         <v>8</v>
       </c>
       <c r="C20" s="212" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="D20" s="190">
         <v>-5</v>
@@ -36162,13 +36162,13 @@
     </row>
     <row r="21" spans="1:24" s="3" customFormat="1">
       <c r="A21" s="200" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="B21" s="81" t="s">
         <v>8</v>
       </c>
       <c r="C21" s="212" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="D21" s="223">
         <v>5.4</v>
@@ -36179,7 +36179,7 @@
       <c r="F21" s="195"/>
       <c r="G21" s="211"/>
       <c r="H21" s="70" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="I21" s="40"/>
       <c r="J21" s="101" t="s">
@@ -36192,13 +36192,13 @@
     </row>
     <row r="22" spans="1:24" s="3" customFormat="1">
       <c r="A22" s="200" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="B22" s="81" t="s">
         <v>8</v>
       </c>
       <c r="C22" s="212" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="D22" s="223">
         <v>0</v>
@@ -36362,7 +36362,7 @@
         <v>7</v>
       </c>
       <c r="C28" s="167" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="D28" s="71">
         <v>2</v>
@@ -36469,7 +36469,7 @@
         <v>168</v>
       </c>
       <c r="D31" s="166" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="E31" s="181" t="s">
         <v>242</v>
@@ -36577,8 +36577,8 @@
       <c r="X34" s="3"/>
     </row>
     <row r="35" spans="1:24" s="3" customFormat="1">
-      <c r="A35" s="200" t="s">
-        <v>1043</v>
+      <c r="A35" s="202" t="s">
+        <v>1062</v>
       </c>
       <c r="B35" s="166"/>
       <c r="C35" s="167" t="s">
@@ -36588,7 +36588,7 @@
         <v>0</v>
       </c>
       <c r="E35" s="181" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="F35" s="181"/>
       <c r="G35" s="181"/>
@@ -36672,7 +36672,7 @@
         <v>7</v>
       </c>
       <c r="C38" s="197" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="D38" s="6">
         <v>7</v>
@@ -36714,7 +36714,7 @@
         <v>363</v>
       </c>
       <c r="C39" s="197" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="D39" s="6">
         <v>0.08</v>
@@ -36758,7 +36758,7 @@
         <v>363</v>
       </c>
       <c r="C40" s="197" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="D40" s="6">
         <f>0.002*12</f>
@@ -36803,7 +36803,7 @@
         <v>364</v>
       </c>
       <c r="C41" s="197" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="D41" s="58">
         <v>3.3500000000000002E-2</v>
@@ -36857,7 +36857,7 @@
         <v>363</v>
       </c>
       <c r="C43" s="197" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="D43" s="6">
         <f>0.007*12</f>
@@ -36924,7 +36924,7 @@
         <v>8</v>
       </c>
       <c r="C45" s="147" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="D45" s="167">
         <v>-1</v>
@@ -36954,7 +36954,7 @@
         <v>8</v>
       </c>
       <c r="C46" s="147" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="D46" s="167">
         <v>1</v>
@@ -36984,7 +36984,7 @@
         <v>8</v>
       </c>
       <c r="C47" s="212" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="D47" s="167">
         <v>5.2</v>
@@ -37014,7 +37014,7 @@
         <v>8</v>
       </c>
       <c r="C48" s="212" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="D48" s="167">
         <v>7.2</v>
@@ -37044,7 +37044,7 @@
         <v>8</v>
       </c>
       <c r="C49" s="212" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="D49" s="190">
         <v>-8</v>
@@ -37076,7 +37076,7 @@
         <v>8</v>
       </c>
       <c r="C50" s="212" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="D50" s="190">
         <v>-5</v>
@@ -37102,13 +37102,13 @@
     </row>
     <row r="51" spans="1:24" s="189" customFormat="1">
       <c r="A51" s="200" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
       <c r="B51" s="81" t="s">
         <v>8</v>
       </c>
       <c r="C51" s="212" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="D51" s="223">
         <v>-5.4</v>
@@ -37119,7 +37119,7 @@
       <c r="F51" s="195"/>
       <c r="G51" s="211"/>
       <c r="H51" s="70" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="I51" s="40"/>
       <c r="J51" s="101" t="s">
@@ -37132,13 +37132,13 @@
     </row>
     <row r="52" spans="1:24" s="189" customFormat="1">
       <c r="A52" s="200" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
       <c r="B52" s="81" t="s">
         <v>8</v>
       </c>
       <c r="C52" s="212" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="D52" s="223">
         <v>0</v>
@@ -37166,7 +37166,7 @@
         <v>8</v>
       </c>
       <c r="C53" s="212" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="D53" s="6">
         <v>5</v>
@@ -37208,7 +37208,7 @@
         <v>8</v>
       </c>
       <c r="C54" s="212" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="D54" s="167">
         <v>7.5</v>
@@ -37238,7 +37238,7 @@
         <v>8</v>
       </c>
       <c r="C55" s="212" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="D55" s="167">
         <v>0</v>
@@ -37270,7 +37270,7 @@
         <v>8</v>
       </c>
       <c r="C56" s="212" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="D56" s="167">
         <v>0</v>
@@ -37302,7 +37302,7 @@
         <v>8</v>
       </c>
       <c r="C57" s="212" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="D57" s="167">
         <v>-1</v>
@@ -37332,7 +37332,7 @@
         <v>8</v>
       </c>
       <c r="C58" s="212" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="D58" s="167">
         <v>1</v>
@@ -37400,7 +37400,7 @@
         <v>8</v>
       </c>
       <c r="C60" s="212" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="D60" s="53" t="s">
         <v>416</v>
@@ -37434,7 +37434,7 @@
         <v>8</v>
       </c>
       <c r="C61" s="212" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="D61" s="53" t="s">
         <v>417</v>
@@ -37468,7 +37468,7 @@
         <v>5</v>
       </c>
       <c r="C62" s="212" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="D62" s="57" t="s">
         <v>250</v>
@@ -37500,7 +37500,7 @@
         <v>5</v>
       </c>
       <c r="C63" s="212" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="D63" s="110">
         <v>120</v>
@@ -37530,7 +37530,7 @@
         <v>5</v>
       </c>
       <c r="C64" s="212" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="D64" s="6" t="s">
         <v>255</v>
@@ -37560,7 +37560,7 @@
         <v>5</v>
       </c>
       <c r="C65" s="212" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="D65" s="57" t="s">
         <v>420</v>
@@ -37592,7 +37592,7 @@
         <v>8</v>
       </c>
       <c r="C66" s="212" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="D66" s="6">
         <v>1028.2</v>
@@ -37626,7 +37626,7 @@
         <v>8</v>
       </c>
       <c r="C67" s="212" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="D67" s="6">
         <v>1025.7</v>
@@ -37660,7 +37660,7 @@
         <v>8</v>
       </c>
       <c r="C68" s="212" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="D68" s="6">
         <v>1028.2</v>
@@ -37694,7 +37694,7 @@
         <v>8</v>
       </c>
       <c r="C69" s="212" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="D69" s="6">
         <v>1025.7</v>
@@ -37728,7 +37728,7 @@
         <v>364</v>
       </c>
       <c r="C70" s="6" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
       <c r="D70" s="111">
         <v>0.03</v>
@@ -37760,7 +37760,7 @@
         <v>364</v>
       </c>
       <c r="C71" s="6" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="D71" s="71">
         <v>3.6999999999999998E-2</v>
@@ -37792,7 +37792,7 @@
         <v>8</v>
       </c>
       <c r="C72" s="212" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="D72" s="57" t="s">
         <v>418</v>
@@ -37826,7 +37826,7 @@
         <v>8</v>
       </c>
       <c r="C73" s="212" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="D73" s="57" t="s">
         <v>419</v>
@@ -37860,7 +37860,7 @@
         <v>8</v>
       </c>
       <c r="C74" s="212" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="D74" s="78" t="s">
         <v>418</v>
@@ -37894,7 +37894,7 @@
         <v>8</v>
       </c>
       <c r="C75" s="212" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="D75" s="78" t="s">
         <v>419</v>
@@ -37928,7 +37928,7 @@
         <v>364</v>
       </c>
       <c r="C76" s="197" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
       <c r="D76" s="71">
         <v>1.2599999999999998E-2</v>
@@ -37960,7 +37960,7 @@
         <v>364</v>
       </c>
       <c r="C77" s="197" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="D77" s="71">
         <v>1.5800000000000002E-2</v>
@@ -37992,7 +37992,7 @@
         <v>8</v>
       </c>
       <c r="C78" s="212" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="D78" s="78" t="s">
         <v>418</v>
@@ -38024,7 +38024,7 @@
         <v>8</v>
       </c>
       <c r="C79" s="212" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="D79" s="78" t="s">
         <v>419</v>
@@ -38115,7 +38115,7 @@
         <v>364</v>
       </c>
       <c r="C82" s="197" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
       <c r="D82" s="71">
         <v>1.54E-2</v>
@@ -38147,7 +38147,7 @@
         <v>364</v>
       </c>
       <c r="C83" s="197" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="D83" s="71">
         <v>1.9300000000000001E-2</v>
@@ -38179,7 +38179,7 @@
         <v>8</v>
       </c>
       <c r="C84" s="212" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="D84" s="78" t="s">
         <v>418</v>
@@ -38211,7 +38211,7 @@
         <v>8</v>
       </c>
       <c r="C85" s="212" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="D85" s="78" t="s">
         <v>419</v>
@@ -38297,13 +38297,13 @@
     </row>
     <row r="88" spans="1:12" s="3" customFormat="1">
       <c r="A88" s="64" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
       <c r="B88" s="60" t="s">
         <v>364</v>
       </c>
       <c r="C88" s="197" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="D88" s="112">
         <v>8.9999999999999998E-4</v>
@@ -38329,7 +38329,7 @@
     </row>
     <row r="89" spans="1:12" s="3" customFormat="1">
       <c r="A89" s="64" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="B89" s="57" t="s">
         <v>5</v>
@@ -38361,7 +38361,7 @@
     </row>
     <row r="90" spans="1:12" s="3" customFormat="1">
       <c r="A90" s="64" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
       <c r="B90" s="57" t="s">
         <v>5</v>
@@ -38393,13 +38393,13 @@
     </row>
     <row r="91" spans="1:12" s="3" customFormat="1">
       <c r="A91" s="64" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="B91" s="60" t="s">
         <v>364</v>
       </c>
       <c r="C91" s="197" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="D91" s="5">
         <v>1.1000000000000001E-3</v>
@@ -38425,7 +38425,7 @@
     </row>
     <row r="92" spans="1:12" s="3" customFormat="1">
       <c r="A92" s="64" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="B92" s="57" t="s">
         <v>5</v>
@@ -38457,7 +38457,7 @@
     </row>
     <row r="93" spans="1:12" s="3" customFormat="1" ht="14.25" customHeight="1">
       <c r="A93" s="64" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
       <c r="B93" s="57" t="s">
         <v>5</v>
@@ -38533,7 +38533,7 @@
         <v>364</v>
       </c>
       <c r="C95" s="197" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="D95" s="75">
         <v>1.4999999999999999E-2</v>
@@ -38565,7 +38565,7 @@
         <v>7</v>
       </c>
       <c r="C96" s="197" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="D96" s="126">
         <v>0.06</v>
@@ -38657,7 +38657,7 @@
         <v>364</v>
       </c>
       <c r="C99" s="197" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="D99" s="126">
         <v>0.03</v>
@@ -38689,7 +38689,7 @@
         <v>364</v>
       </c>
       <c r="C100" s="197" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="D100" s="126">
         <v>0.05</v>
@@ -38721,7 +38721,7 @@
         <v>364</v>
       </c>
       <c r="C101" s="197" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="D101" s="13">
         <v>4.2999999999999997E-2</v>
@@ -38783,7 +38783,7 @@
         <v>22</v>
       </c>
       <c r="C103" s="80" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="D103" s="13">
         <v>0.44</v>
@@ -38815,7 +38815,7 @@
         <v>364</v>
       </c>
       <c r="C104" s="197" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="D104" s="75">
         <v>1.4999999999999999E-2</v>
@@ -38847,7 +38847,7 @@
         <v>364</v>
       </c>
       <c r="C105" s="197" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="D105" s="127">
         <v>0.06</v>
@@ -38879,7 +38879,7 @@
         <v>364</v>
       </c>
       <c r="C106" s="197" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="D106" s="75">
         <v>0.08</v>
@@ -38911,7 +38911,7 @@
         <v>364</v>
       </c>
       <c r="C107" s="197" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="D107" s="127">
         <v>0.06</v>

</xml_diff>

<commit_message>
Added negligible volume to the alveolar dead space to make sure it's included in compartment volume calculations.
</commit_message>
<xml_diff>
--- a/test/validation/SystemValidationData.xlsx
+++ b/test/validation/SystemValidationData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Source\engine\test\validation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Source\Pulse_Documentation\source\test\validation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAEB3C5F-1DB9-4466-8D76-BE940CA06CA6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17938C3E-B623-4B08-A45D-ABBAEFD3EECB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1830" yWindow="3450" windowWidth="27090" windowHeight="25230" tabRatio="724" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" tabRatio="724" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blood Chemistry" sheetId="4" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3895" uniqueCount="1063">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3896" uniqueCount="1064">
   <si>
     <t>Output</t>
   </si>
@@ -3349,6 +3349,9 @@
   </si>
   <si>
     <t>RespiratoryMuscleFatigue*</t>
+  </si>
+  <si>
+    <t>Negligible</t>
   </si>
 </sst>
 </file>
@@ -35543,10 +35546,10 @@
   <dimension ref="A1:X114"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B26" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A38" sqref="A38"/>
+      <selection pane="bottomRight" activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -35669,7 +35672,7 @@
         <v>168</v>
       </c>
       <c r="D3" s="187">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3" s="181" t="s">
         <v>242</v>
@@ -35677,7 +35680,9 @@
       <c r="F3" s="181" t="s">
         <v>1002</v>
       </c>
-      <c r="G3" s="181"/>
+      <c r="G3" s="181" t="s">
+        <v>1063</v>
+      </c>
       <c r="H3" s="70" t="s">
         <v>1003</v>
       </c>

</xml_diff>